<commit_message>
Aregar títulos en indicador de llamadas, actualizar archivo Scrum.xlsx
</commit_message>
<xml_diff>
--- a/Scrum.xlsx
+++ b/Scrum.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="13620"/>
   </bookViews>
   <sheets>
-    <sheet name="Actividades Febrero - Toño" sheetId="1" r:id="rId4"/>
-    <sheet name="Actividades Febrero - Mario" sheetId="2" r:id="rId5"/>
-    <sheet name="Actividades Febrero - Rosa" sheetId="3" r:id="rId6"/>
-    <sheet name="Nuevos módulos" sheetId="4" r:id="rId7"/>
-    <sheet name="Actividades Enero" sheetId="5" r:id="rId8"/>
-    <sheet name="Catálogo" sheetId="6" r:id="rId9"/>
-    <sheet name="Correo catálogos" sheetId="7" r:id="rId10"/>
+    <sheet name="Actividades Febrero - Toño" sheetId="1" r:id="rId1"/>
+    <sheet name="Actividades Febrero - Mario" sheetId="2" r:id="rId2"/>
+    <sheet name="Actividades Febrero - Rosa" sheetId="3" r:id="rId3"/>
+    <sheet name="Nuevos módulos" sheetId="4" r:id="rId4"/>
+    <sheet name="Actividades Enero" sheetId="5" r:id="rId5"/>
+    <sheet name="Catálogo" sheetId="6" r:id="rId6"/>
+    <sheet name="Correo catálogos" sheetId="7" r:id="rId7"/>
   </sheets>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="94">
   <si>
     <t>TOÑO</t>
   </si>
@@ -287,33 +290,32 @@
   </si>
   <si>
     <t>Para las direcciones: Ninguna tiene campos completos, ¿se agregarán así?</t>
+  </si>
+  <si>
+    <t>Indicadores - Agregar ganado/participado para cotizaciones y concursos</t>
+  </si>
+  <si>
+    <t>Todos - Actualizar de prospecto a actual</t>
+  </si>
+  <si>
+    <t>Indicadores - Modificar consulta con objetivo por ejecutivo</t>
+  </si>
+  <si>
+    <t>Indicadores - Módulo para asignar objetivos por ejecutivo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -668,291 +670,227 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="85">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="83">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="fffde9d9"/>
-      <rgbColor rgb="ff005392"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffdbe5f1"/>
-      <rgbColor rgb="fff2dbdb"/>
-      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFDE9D9"/>
+      <rgbColor rgb="FF005392"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFDBE5F1"/>
+      <rgbColor rgb="FFF2DBDB"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -1078,7 +1016,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1087,7 +1025,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1096,7 +1034,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1170,7 +1108,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1178,7 +1116,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1197,7 +1135,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1227,7 +1165,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1253,7 +1191,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1279,7 +1217,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1305,7 +1243,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1331,7 +1269,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1357,7 +1295,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1383,7 +1321,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1409,7 +1347,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1435,7 +1373,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1448,9 +1386,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1465,7 +1409,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="38000"/>
             </a:srgbClr>
@@ -1473,7 +1417,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1492,7 +1436,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1518,7 +1462,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1544,7 +1488,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1570,7 +1514,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1596,7 +1540,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1622,7 +1566,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1648,7 +1592,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1674,7 +1618,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1700,7 +1644,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1726,7 +1670,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1739,9 +1683,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1755,7 +1705,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1774,7 +1724,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1804,7 +1754,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1830,7 +1780,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1856,7 +1806,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1882,7 +1832,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1908,7 +1858,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1934,7 +1884,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1960,7 +1910,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1986,7 +1936,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2012,7 +1962,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2025,165 +1975,174 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:IV20"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="59.8516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6719" style="1" customWidth="1"/>
+    <col min="1" max="1" width="59.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" customWidth="1"/>
-    <col min="4" max="256" width="8.85156" style="1" customWidth="1"/>
+    <col min="4" max="256" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:3" ht="15" customHeight="1">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="4">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="7">
+    <row r="3" spans="1:3" ht="15" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <v>43071</v>
       </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="7">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <v>43071</v>
       </c>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="7">
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="6">
         <v>43071</v>
       </c>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="7">
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>43071</v>
       </c>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="13">
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1">
+      <c r="A8" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="15">
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1">
+      <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="7">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-    </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-    </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="22">
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1">
+      <c r="A12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-    </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" s="24"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-    </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="A14" s="25"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-    </row>
-    <row r="15" ht="15" customHeight="1" hidden="1">
-      <c r="A15" s="25"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-    </row>
-    <row r="16" ht="15" customHeight="1" hidden="1">
-      <c r="A16" s="25"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-    </row>
-    <row r="17" ht="15" customHeight="1" hidden="1">
-      <c r="A17" s="25"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-    </row>
-    <row r="18" ht="15" customHeight="1" hidden="1">
-      <c r="A18" s="25"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-    </row>
-    <row r="19" ht="15" customHeight="1">
-      <c r="A19" t="s" s="26">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1">
+      <c r="A13" s="20"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1">
+      <c r="A14" s="21"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="1:3" ht="15" hidden="1" customHeight="1">
+      <c r="A15" s="21"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+    </row>
+    <row r="16" spans="1:3" ht="15" hidden="1" customHeight="1">
+      <c r="A16" s="21"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" hidden="1" customHeight="1">
+      <c r="A17" s="21"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+    </row>
+    <row r="18" spans="1:3" ht="15" hidden="1" customHeight="1">
+      <c r="A18" s="21"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1">
+      <c r="A19" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-    </row>
-    <row r="20" ht="15" customHeight="1">
-      <c r="A20" t="s" s="27">
+      <c r="B19" s="79"/>
+      <c r="C19" s="80"/>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1">
+      <c r="A20" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="29"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2193,7 +2152,7 @@
     <mergeCell ref="A19:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2201,183 +2160,183 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:IV23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="75.5" style="30" customWidth="1"/>
-    <col min="2" max="2" width="12.6719" style="30" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="30" customWidth="1"/>
-    <col min="4" max="256" width="8.85156" style="30" customWidth="1"/>
+    <col min="1" max="1" width="75.42578125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="22" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="22" customWidth="1"/>
+    <col min="4" max="256" width="8.85546875" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:3" ht="15" customHeight="1">
+      <c r="A1" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="4">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="7">
+    <row r="3" spans="1:3" ht="15" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <v>43071</v>
       </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="7">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <v>43071</v>
       </c>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="7">
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1">
+      <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="6">
         <v>43071</v>
       </c>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="7">
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1">
+      <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>43071</v>
       </c>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="7">
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1">
+      <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>43071</v>
       </c>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="7">
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1">
+      <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="6">
         <v>43071</v>
       </c>
-      <c r="C8" s="9"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="13">
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1">
+      <c r="A10" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-    </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" t="s" s="15">
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1">
+      <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-    </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="7">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1">
+      <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-    </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" t="s" s="7">
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1">
+      <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-    </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="A14" s="10"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-    </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" t="s" s="22">
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1">
+      <c r="A14" s="8"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1">
+      <c r="A15" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-    </row>
-    <row r="16" ht="15" customHeight="1">
-      <c r="A16" t="s" s="15">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+    </row>
+    <row r="16" spans="1:3" ht="15" customHeight="1">
+      <c r="A16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-    </row>
-    <row r="17" ht="15" customHeight="1">
-      <c r="A17" t="s" s="7">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1">
+      <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-    </row>
-    <row r="18" ht="15" customHeight="1">
-      <c r="A18" s="25"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-    </row>
-    <row r="19" ht="15" customHeight="1">
-      <c r="A19" s="25"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-    </row>
-    <row r="20" ht="15" customHeight="1" hidden="1">
-      <c r="A20" s="25"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-    </row>
-    <row r="21" ht="15" customHeight="1" hidden="1">
-      <c r="A21" s="25"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
-    </row>
-    <row r="22" ht="15" customHeight="1">
-      <c r="A22" t="s" s="26">
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1">
+      <c r="A18" s="21"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1">
+      <c r="A19" s="21"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+    </row>
+    <row r="20" spans="1:3" ht="15" hidden="1" customHeight="1">
+      <c r="A20" s="21"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+    </row>
+    <row r="21" spans="1:3" ht="15" hidden="1" customHeight="1">
+      <c r="A21" s="21"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1">
+      <c r="A22" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
-    </row>
-    <row r="23" ht="15" customHeight="1">
-      <c r="A23" t="s" s="27">
+      <c r="B22" s="79"/>
+      <c r="C22" s="80"/>
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1">
+      <c r="A23" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2387,7 +2346,7 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2395,171 +2354,697 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:IV21"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="75.5" style="31" customWidth="1"/>
-    <col min="2" max="2" width="12.6719" style="31" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="31" customWidth="1"/>
-    <col min="4" max="256" width="8.85156" style="31" customWidth="1"/>
+    <col min="1" max="1" width="75.42578125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="23" customWidth="1"/>
+    <col min="4" max="256" width="8.85546875" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:256" ht="15" customHeight="1">
+      <c r="A1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="4">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+    </row>
+    <row r="2" spans="1:256" ht="15" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="7">
+    <row r="3" spans="1:256" ht="15" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <v>43071</v>
       </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="7">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:256" ht="15" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <v>43071</v>
       </c>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="7">
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:256" ht="15" customHeight="1">
+      <c r="A5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="6">
         <v>43071</v>
       </c>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="7">
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:256" ht="15" customHeight="1">
+      <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>43071</v>
       </c>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="7">
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:256" ht="15" customHeight="1">
+      <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>43071</v>
       </c>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="7">
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:256" ht="15" customHeight="1">
+      <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="6">
         <v>43071</v>
       </c>
-      <c r="C8" s="9"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="7">
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:256" ht="15" customHeight="1">
+      <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>43071</v>
       </c>
-      <c r="C9" s="9"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" t="s" s="13">
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:256" ht="15" customHeight="1">
+      <c r="A10" s="83" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="9">
+        <v>43071</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="66"/>
+      <c r="O10" s="66"/>
+      <c r="P10" s="66"/>
+      <c r="Q10" s="66"/>
+      <c r="R10" s="66"/>
+      <c r="S10" s="66"/>
+      <c r="T10" s="66"/>
+      <c r="U10" s="66"/>
+      <c r="V10" s="66"/>
+      <c r="W10" s="66"/>
+      <c r="X10" s="66"/>
+      <c r="Y10" s="66"/>
+      <c r="Z10" s="66"/>
+      <c r="AA10" s="66"/>
+      <c r="AB10" s="66"/>
+      <c r="AC10" s="66"/>
+      <c r="AD10" s="66"/>
+      <c r="AE10" s="66"/>
+      <c r="AF10" s="66"/>
+      <c r="AG10" s="66"/>
+      <c r="AH10" s="66"/>
+      <c r="AI10" s="66"/>
+      <c r="AJ10" s="66"/>
+      <c r="AK10" s="66"/>
+      <c r="AL10" s="66"/>
+      <c r="AM10" s="66"/>
+      <c r="AN10" s="66"/>
+      <c r="AO10" s="66"/>
+      <c r="AP10" s="66"/>
+      <c r="AQ10" s="66"/>
+      <c r="AR10" s="66"/>
+      <c r="AS10" s="66"/>
+      <c r="AT10" s="66"/>
+      <c r="AU10" s="66"/>
+      <c r="AV10" s="66"/>
+      <c r="AW10" s="66"/>
+      <c r="AX10" s="66"/>
+      <c r="AY10" s="66"/>
+      <c r="AZ10" s="66"/>
+      <c r="BA10" s="66"/>
+      <c r="BB10" s="66"/>
+      <c r="BC10" s="66"/>
+      <c r="BD10" s="66"/>
+      <c r="BE10" s="66"/>
+      <c r="BF10" s="66"/>
+      <c r="BG10" s="66"/>
+      <c r="BH10" s="66"/>
+      <c r="BI10" s="66"/>
+      <c r="BJ10" s="66"/>
+      <c r="BK10" s="66"/>
+      <c r="BL10" s="66"/>
+      <c r="BM10" s="66"/>
+      <c r="BN10" s="66"/>
+      <c r="BO10" s="66"/>
+      <c r="BP10" s="66"/>
+      <c r="BQ10" s="66"/>
+      <c r="BR10" s="66"/>
+      <c r="BS10" s="66"/>
+      <c r="BT10" s="66"/>
+      <c r="BU10" s="66"/>
+      <c r="BV10" s="66"/>
+      <c r="BW10" s="66"/>
+      <c r="BX10" s="66"/>
+      <c r="BY10" s="66"/>
+      <c r="BZ10" s="66"/>
+      <c r="CA10" s="66"/>
+      <c r="CB10" s="66"/>
+      <c r="CC10" s="66"/>
+      <c r="CD10" s="66"/>
+      <c r="CE10" s="66"/>
+      <c r="CF10" s="66"/>
+      <c r="CG10" s="66"/>
+      <c r="CH10" s="66"/>
+      <c r="CI10" s="66"/>
+      <c r="CJ10" s="66"/>
+      <c r="CK10" s="66"/>
+      <c r="CL10" s="66"/>
+      <c r="CM10" s="66"/>
+      <c r="CN10" s="66"/>
+      <c r="CO10" s="66"/>
+      <c r="CP10" s="66"/>
+      <c r="CQ10" s="66"/>
+      <c r="CR10" s="66"/>
+      <c r="CS10" s="66"/>
+      <c r="CT10" s="66"/>
+      <c r="CU10" s="66"/>
+      <c r="CV10" s="66"/>
+      <c r="CW10" s="66"/>
+      <c r="CX10" s="66"/>
+      <c r="CY10" s="66"/>
+      <c r="CZ10" s="66"/>
+      <c r="DA10" s="66"/>
+      <c r="DB10" s="66"/>
+      <c r="DC10" s="66"/>
+      <c r="DD10" s="66"/>
+      <c r="DE10" s="66"/>
+      <c r="DF10" s="66"/>
+      <c r="DG10" s="66"/>
+      <c r="DH10" s="66"/>
+      <c r="DI10" s="66"/>
+      <c r="DJ10" s="66"/>
+      <c r="DK10" s="66"/>
+      <c r="DL10" s="66"/>
+      <c r="DM10" s="66"/>
+      <c r="DN10" s="66"/>
+      <c r="DO10" s="66"/>
+      <c r="DP10" s="66"/>
+      <c r="DQ10" s="66"/>
+      <c r="DR10" s="66"/>
+      <c r="DS10" s="66"/>
+      <c r="DT10" s="66"/>
+      <c r="DU10" s="66"/>
+      <c r="DV10" s="66"/>
+      <c r="DW10" s="66"/>
+      <c r="DX10" s="66"/>
+      <c r="DY10" s="66"/>
+      <c r="DZ10" s="66"/>
+      <c r="EA10" s="66"/>
+      <c r="EB10" s="66"/>
+      <c r="EC10" s="66"/>
+      <c r="ED10" s="66"/>
+      <c r="EE10" s="66"/>
+      <c r="EF10" s="66"/>
+      <c r="EG10" s="66"/>
+      <c r="EH10" s="66"/>
+      <c r="EI10" s="66"/>
+      <c r="EJ10" s="66"/>
+      <c r="EK10" s="66"/>
+      <c r="EL10" s="66"/>
+      <c r="EM10" s="66"/>
+      <c r="EN10" s="66"/>
+      <c r="EO10" s="66"/>
+      <c r="EP10" s="66"/>
+      <c r="EQ10" s="66"/>
+      <c r="ER10" s="66"/>
+      <c r="ES10" s="66"/>
+      <c r="ET10" s="66"/>
+      <c r="EU10" s="66"/>
+      <c r="EV10" s="66"/>
+      <c r="EW10" s="66"/>
+      <c r="EX10" s="66"/>
+      <c r="EY10" s="66"/>
+      <c r="EZ10" s="66"/>
+      <c r="FA10" s="66"/>
+      <c r="FB10" s="66"/>
+      <c r="FC10" s="66"/>
+      <c r="FD10" s="66"/>
+      <c r="FE10" s="66"/>
+      <c r="FF10" s="66"/>
+      <c r="FG10" s="66"/>
+      <c r="FH10" s="66"/>
+      <c r="FI10" s="66"/>
+      <c r="FJ10" s="66"/>
+      <c r="FK10" s="66"/>
+      <c r="FL10" s="66"/>
+      <c r="FM10" s="66"/>
+      <c r="FN10" s="66"/>
+      <c r="FO10" s="66"/>
+      <c r="FP10" s="66"/>
+      <c r="FQ10" s="66"/>
+      <c r="FR10" s="66"/>
+      <c r="FS10" s="66"/>
+      <c r="FT10" s="66"/>
+      <c r="FU10" s="66"/>
+      <c r="FV10" s="66"/>
+      <c r="FW10" s="66"/>
+      <c r="FX10" s="66"/>
+      <c r="FY10" s="66"/>
+      <c r="FZ10" s="66"/>
+      <c r="GA10" s="66"/>
+      <c r="GB10" s="66"/>
+      <c r="GC10" s="66"/>
+      <c r="GD10" s="66"/>
+      <c r="GE10" s="66"/>
+      <c r="GF10" s="66"/>
+      <c r="GG10" s="66"/>
+      <c r="GH10" s="66"/>
+      <c r="GI10" s="66"/>
+      <c r="GJ10" s="66"/>
+      <c r="GK10" s="66"/>
+      <c r="GL10" s="66"/>
+      <c r="GM10" s="66"/>
+      <c r="GN10" s="66"/>
+      <c r="GO10" s="66"/>
+      <c r="GP10" s="66"/>
+      <c r="GQ10" s="66"/>
+      <c r="GR10" s="66"/>
+      <c r="GS10" s="66"/>
+      <c r="GT10" s="66"/>
+      <c r="GU10" s="66"/>
+      <c r="GV10" s="66"/>
+      <c r="GW10" s="66"/>
+      <c r="GX10" s="66"/>
+      <c r="GY10" s="66"/>
+      <c r="GZ10" s="66"/>
+      <c r="HA10" s="66"/>
+      <c r="HB10" s="66"/>
+      <c r="HC10" s="66"/>
+      <c r="HD10" s="66"/>
+      <c r="HE10" s="66"/>
+      <c r="HF10" s="66"/>
+      <c r="HG10" s="66"/>
+      <c r="HH10" s="66"/>
+      <c r="HI10" s="66"/>
+      <c r="HJ10" s="66"/>
+      <c r="HK10" s="66"/>
+      <c r="HL10" s="66"/>
+      <c r="HM10" s="66"/>
+      <c r="HN10" s="66"/>
+      <c r="HO10" s="66"/>
+      <c r="HP10" s="66"/>
+      <c r="HQ10" s="66"/>
+      <c r="HR10" s="66"/>
+      <c r="HS10" s="66"/>
+      <c r="HT10" s="66"/>
+      <c r="HU10" s="66"/>
+      <c r="HV10" s="66"/>
+      <c r="HW10" s="66"/>
+      <c r="HX10" s="66"/>
+      <c r="HY10" s="66"/>
+      <c r="HZ10" s="66"/>
+      <c r="IA10" s="66"/>
+      <c r="IB10" s="66"/>
+      <c r="IC10" s="66"/>
+      <c r="ID10" s="66"/>
+      <c r="IE10" s="66"/>
+      <c r="IF10" s="66"/>
+      <c r="IG10" s="66"/>
+      <c r="IH10" s="66"/>
+      <c r="II10" s="66"/>
+      <c r="IJ10" s="66"/>
+      <c r="IK10" s="66"/>
+      <c r="IL10" s="66"/>
+      <c r="IM10" s="66"/>
+      <c r="IN10" s="66"/>
+      <c r="IO10" s="66"/>
+      <c r="IP10" s="66"/>
+      <c r="IQ10" s="66"/>
+      <c r="IR10" s="66"/>
+      <c r="IS10" s="66"/>
+      <c r="IT10" s="66"/>
+      <c r="IU10" s="66"/>
+      <c r="IV10" s="66"/>
+    </row>
+    <row r="11" spans="1:256" ht="15" customHeight="1">
+      <c r="A11" s="83" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="9">
+        <v>43071</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="66"/>
+      <c r="R11" s="66"/>
+      <c r="S11" s="66"/>
+      <c r="T11" s="66"/>
+      <c r="U11" s="66"/>
+      <c r="V11" s="66"/>
+      <c r="W11" s="66"/>
+      <c r="X11" s="66"/>
+      <c r="Y11" s="66"/>
+      <c r="Z11" s="66"/>
+      <c r="AA11" s="66"/>
+      <c r="AB11" s="66"/>
+      <c r="AC11" s="66"/>
+      <c r="AD11" s="66"/>
+      <c r="AE11" s="66"/>
+      <c r="AF11" s="66"/>
+      <c r="AG11" s="66"/>
+      <c r="AH11" s="66"/>
+      <c r="AI11" s="66"/>
+      <c r="AJ11" s="66"/>
+      <c r="AK11" s="66"/>
+      <c r="AL11" s="66"/>
+      <c r="AM11" s="66"/>
+      <c r="AN11" s="66"/>
+      <c r="AO11" s="66"/>
+      <c r="AP11" s="66"/>
+      <c r="AQ11" s="66"/>
+      <c r="AR11" s="66"/>
+      <c r="AS11" s="66"/>
+      <c r="AT11" s="66"/>
+      <c r="AU11" s="66"/>
+      <c r="AV11" s="66"/>
+      <c r="AW11" s="66"/>
+      <c r="AX11" s="66"/>
+      <c r="AY11" s="66"/>
+      <c r="AZ11" s="66"/>
+      <c r="BA11" s="66"/>
+      <c r="BB11" s="66"/>
+      <c r="BC11" s="66"/>
+      <c r="BD11" s="66"/>
+      <c r="BE11" s="66"/>
+      <c r="BF11" s="66"/>
+      <c r="BG11" s="66"/>
+      <c r="BH11" s="66"/>
+      <c r="BI11" s="66"/>
+      <c r="BJ11" s="66"/>
+      <c r="BK11" s="66"/>
+      <c r="BL11" s="66"/>
+      <c r="BM11" s="66"/>
+      <c r="BN11" s="66"/>
+      <c r="BO11" s="66"/>
+      <c r="BP11" s="66"/>
+      <c r="BQ11" s="66"/>
+      <c r="BR11" s="66"/>
+      <c r="BS11" s="66"/>
+      <c r="BT11" s="66"/>
+      <c r="BU11" s="66"/>
+      <c r="BV11" s="66"/>
+      <c r="BW11" s="66"/>
+      <c r="BX11" s="66"/>
+      <c r="BY11" s="66"/>
+      <c r="BZ11" s="66"/>
+      <c r="CA11" s="66"/>
+      <c r="CB11" s="66"/>
+      <c r="CC11" s="66"/>
+      <c r="CD11" s="66"/>
+      <c r="CE11" s="66"/>
+      <c r="CF11" s="66"/>
+      <c r="CG11" s="66"/>
+      <c r="CH11" s="66"/>
+      <c r="CI11" s="66"/>
+      <c r="CJ11" s="66"/>
+      <c r="CK11" s="66"/>
+      <c r="CL11" s="66"/>
+      <c r="CM11" s="66"/>
+      <c r="CN11" s="66"/>
+      <c r="CO11" s="66"/>
+      <c r="CP11" s="66"/>
+      <c r="CQ11" s="66"/>
+      <c r="CR11" s="66"/>
+      <c r="CS11" s="66"/>
+      <c r="CT11" s="66"/>
+      <c r="CU11" s="66"/>
+      <c r="CV11" s="66"/>
+      <c r="CW11" s="66"/>
+      <c r="CX11" s="66"/>
+      <c r="CY11" s="66"/>
+      <c r="CZ11" s="66"/>
+      <c r="DA11" s="66"/>
+      <c r="DB11" s="66"/>
+      <c r="DC11" s="66"/>
+      <c r="DD11" s="66"/>
+      <c r="DE11" s="66"/>
+      <c r="DF11" s="66"/>
+      <c r="DG11" s="66"/>
+      <c r="DH11" s="66"/>
+      <c r="DI11" s="66"/>
+      <c r="DJ11" s="66"/>
+      <c r="DK11" s="66"/>
+      <c r="DL11" s="66"/>
+      <c r="DM11" s="66"/>
+      <c r="DN11" s="66"/>
+      <c r="DO11" s="66"/>
+      <c r="DP11" s="66"/>
+      <c r="DQ11" s="66"/>
+      <c r="DR11" s="66"/>
+      <c r="DS11" s="66"/>
+      <c r="DT11" s="66"/>
+      <c r="DU11" s="66"/>
+      <c r="DV11" s="66"/>
+      <c r="DW11" s="66"/>
+      <c r="DX11" s="66"/>
+      <c r="DY11" s="66"/>
+      <c r="DZ11" s="66"/>
+      <c r="EA11" s="66"/>
+      <c r="EB11" s="66"/>
+      <c r="EC11" s="66"/>
+      <c r="ED11" s="66"/>
+      <c r="EE11" s="66"/>
+      <c r="EF11" s="66"/>
+      <c r="EG11" s="66"/>
+      <c r="EH11" s="66"/>
+      <c r="EI11" s="66"/>
+      <c r="EJ11" s="66"/>
+      <c r="EK11" s="66"/>
+      <c r="EL11" s="66"/>
+      <c r="EM11" s="66"/>
+      <c r="EN11" s="66"/>
+      <c r="EO11" s="66"/>
+      <c r="EP11" s="66"/>
+      <c r="EQ11" s="66"/>
+      <c r="ER11" s="66"/>
+      <c r="ES11" s="66"/>
+      <c r="ET11" s="66"/>
+      <c r="EU11" s="66"/>
+      <c r="EV11" s="66"/>
+      <c r="EW11" s="66"/>
+      <c r="EX11" s="66"/>
+      <c r="EY11" s="66"/>
+      <c r="EZ11" s="66"/>
+      <c r="FA11" s="66"/>
+      <c r="FB11" s="66"/>
+      <c r="FC11" s="66"/>
+      <c r="FD11" s="66"/>
+      <c r="FE11" s="66"/>
+      <c r="FF11" s="66"/>
+      <c r="FG11" s="66"/>
+      <c r="FH11" s="66"/>
+      <c r="FI11" s="66"/>
+      <c r="FJ11" s="66"/>
+      <c r="FK11" s="66"/>
+      <c r="FL11" s="66"/>
+      <c r="FM11" s="66"/>
+      <c r="FN11" s="66"/>
+      <c r="FO11" s="66"/>
+      <c r="FP11" s="66"/>
+      <c r="FQ11" s="66"/>
+      <c r="FR11" s="66"/>
+      <c r="FS11" s="66"/>
+      <c r="FT11" s="66"/>
+      <c r="FU11" s="66"/>
+      <c r="FV11" s="66"/>
+      <c r="FW11" s="66"/>
+      <c r="FX11" s="66"/>
+      <c r="FY11" s="66"/>
+      <c r="FZ11" s="66"/>
+      <c r="GA11" s="66"/>
+      <c r="GB11" s="66"/>
+      <c r="GC11" s="66"/>
+      <c r="GD11" s="66"/>
+      <c r="GE11" s="66"/>
+      <c r="GF11" s="66"/>
+      <c r="GG11" s="66"/>
+      <c r="GH11" s="66"/>
+      <c r="GI11" s="66"/>
+      <c r="GJ11" s="66"/>
+      <c r="GK11" s="66"/>
+      <c r="GL11" s="66"/>
+      <c r="GM11" s="66"/>
+      <c r="GN11" s="66"/>
+      <c r="GO11" s="66"/>
+      <c r="GP11" s="66"/>
+      <c r="GQ11" s="66"/>
+      <c r="GR11" s="66"/>
+      <c r="GS11" s="66"/>
+      <c r="GT11" s="66"/>
+      <c r="GU11" s="66"/>
+      <c r="GV11" s="66"/>
+      <c r="GW11" s="66"/>
+      <c r="GX11" s="66"/>
+      <c r="GY11" s="66"/>
+      <c r="GZ11" s="66"/>
+      <c r="HA11" s="66"/>
+      <c r="HB11" s="66"/>
+      <c r="HC11" s="66"/>
+      <c r="HD11" s="66"/>
+      <c r="HE11" s="66"/>
+      <c r="HF11" s="66"/>
+      <c r="HG11" s="66"/>
+      <c r="HH11" s="66"/>
+      <c r="HI11" s="66"/>
+      <c r="HJ11" s="66"/>
+      <c r="HK11" s="66"/>
+      <c r="HL11" s="66"/>
+      <c r="HM11" s="66"/>
+      <c r="HN11" s="66"/>
+      <c r="HO11" s="66"/>
+      <c r="HP11" s="66"/>
+      <c r="HQ11" s="66"/>
+      <c r="HR11" s="66"/>
+      <c r="HS11" s="66"/>
+      <c r="HT11" s="66"/>
+      <c r="HU11" s="66"/>
+      <c r="HV11" s="66"/>
+      <c r="HW11" s="66"/>
+      <c r="HX11" s="66"/>
+      <c r="HY11" s="66"/>
+      <c r="HZ11" s="66"/>
+      <c r="IA11" s="66"/>
+      <c r="IB11" s="66"/>
+      <c r="IC11" s="66"/>
+      <c r="ID11" s="66"/>
+      <c r="IE11" s="66"/>
+      <c r="IF11" s="66"/>
+      <c r="IG11" s="66"/>
+      <c r="IH11" s="66"/>
+      <c r="II11" s="66"/>
+      <c r="IJ11" s="66"/>
+      <c r="IK11" s="66"/>
+      <c r="IL11" s="66"/>
+      <c r="IM11" s="66"/>
+      <c r="IN11" s="66"/>
+      <c r="IO11" s="66"/>
+      <c r="IP11" s="66"/>
+      <c r="IQ11" s="66"/>
+      <c r="IR11" s="66"/>
+      <c r="IS11" s="66"/>
+      <c r="IT11" s="66"/>
+      <c r="IU11" s="66"/>
+      <c r="IV11" s="66"/>
+    </row>
+    <row r="12" spans="1:256" ht="15" customHeight="1">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="1:256" ht="15" customHeight="1">
+      <c r="A13" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-    </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="15">
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
+    </row>
+    <row r="14" spans="1:256" ht="15" customHeight="1">
+      <c r="A14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-    </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" t="s" s="7">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+    </row>
+    <row r="15" spans="1:256" ht="15" customHeight="1">
+      <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-    </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="A14" s="10"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-    </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" t="s" s="22">
-        <v>11</v>
-      </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-    </row>
-    <row r="16" ht="15" customHeight="1">
-      <c r="A16" s="24"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+    </row>
+    <row r="16" spans="1:256" ht="15" customHeight="1">
+      <c r="A16" s="8"/>
       <c r="B16" s="16"/>
       <c r="C16" s="17"/>
     </row>
-    <row r="17" ht="15" customHeight="1">
-      <c r="A17" s="25"/>
-      <c r="B17" s="18"/>
+    <row r="17" spans="1:3" customFormat="1" ht="15" customHeight="1">
+      <c r="A17" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="19"/>
       <c r="C17" s="19"/>
     </row>
-    <row r="18" ht="15" customHeight="1">
-      <c r="A18" t="s" s="26">
+    <row r="18" spans="1:3" customFormat="1" ht="15" customHeight="1">
+      <c r="A18" s="20"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+    </row>
+    <row r="19" spans="1:3" customFormat="1" ht="15" customHeight="1">
+      <c r="A19" s="21"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+    </row>
+    <row r="20" spans="1:3" customFormat="1" ht="15" customHeight="1">
+      <c r="A20" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-    </row>
-    <row r="19" ht="15" customHeight="1">
-      <c r="A19" t="s" s="27">
+      <c r="B20" s="79"/>
+      <c r="C20" s="80"/>
+    </row>
+    <row r="21" spans="1:3" customFormat="1" ht="15" customHeight="1">
+      <c r="A21" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A20:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2567,93 +3052,361 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:IV9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="75.5" style="32" customWidth="1"/>
-    <col min="2" max="2" width="12.6719" style="32" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="32" customWidth="1"/>
-    <col min="4" max="256" width="8.85156" style="32" customWidth="1"/>
+    <col min="1" max="1" width="75.42578125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="24" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="24" customWidth="1"/>
+    <col min="4" max="256" width="8.85546875" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:256" ht="15" customHeight="1">
+      <c r="A1" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="4">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+    </row>
+    <row r="2" spans="1:256" ht="15" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="7">
+    <row r="3" spans="1:256" ht="15" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s" s="33">
+      <c r="B3" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="7">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:256" ht="15" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B4" t="s" s="33">
+      <c r="B4" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="7">
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:256" ht="15" customHeight="1">
+      <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" t="s" s="33">
+      <c r="B5" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="7">
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:256" ht="15" customHeight="1">
+      <c r="A6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B6" t="s" s="33">
+      <c r="B6" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="7">
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:256" ht="15" customHeight="1">
+      <c r="A7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B7" t="s" s="33">
+      <c r="B7" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="34"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="35"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:256" ht="15" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:256" ht="15" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="84" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="66"/>
+      <c r="S9" s="66"/>
+      <c r="T9" s="66"/>
+      <c r="U9" s="66"/>
+      <c r="V9" s="66"/>
+      <c r="W9" s="66"/>
+      <c r="X9" s="66"/>
+      <c r="Y9" s="66"/>
+      <c r="Z9" s="66"/>
+      <c r="AA9" s="66"/>
+      <c r="AB9" s="66"/>
+      <c r="AC9" s="66"/>
+      <c r="AD9" s="66"/>
+      <c r="AE9" s="66"/>
+      <c r="AF9" s="66"/>
+      <c r="AG9" s="66"/>
+      <c r="AH9" s="66"/>
+      <c r="AI9" s="66"/>
+      <c r="AJ9" s="66"/>
+      <c r="AK9" s="66"/>
+      <c r="AL9" s="66"/>
+      <c r="AM9" s="66"/>
+      <c r="AN9" s="66"/>
+      <c r="AO9" s="66"/>
+      <c r="AP9" s="66"/>
+      <c r="AQ9" s="66"/>
+      <c r="AR9" s="66"/>
+      <c r="AS9" s="66"/>
+      <c r="AT9" s="66"/>
+      <c r="AU9" s="66"/>
+      <c r="AV9" s="66"/>
+      <c r="AW9" s="66"/>
+      <c r="AX9" s="66"/>
+      <c r="AY9" s="66"/>
+      <c r="AZ9" s="66"/>
+      <c r="BA9" s="66"/>
+      <c r="BB9" s="66"/>
+      <c r="BC9" s="66"/>
+      <c r="BD9" s="66"/>
+      <c r="BE9" s="66"/>
+      <c r="BF9" s="66"/>
+      <c r="BG9" s="66"/>
+      <c r="BH9" s="66"/>
+      <c r="BI9" s="66"/>
+      <c r="BJ9" s="66"/>
+      <c r="BK9" s="66"/>
+      <c r="BL9" s="66"/>
+      <c r="BM9" s="66"/>
+      <c r="BN9" s="66"/>
+      <c r="BO9" s="66"/>
+      <c r="BP9" s="66"/>
+      <c r="BQ9" s="66"/>
+      <c r="BR9" s="66"/>
+      <c r="BS9" s="66"/>
+      <c r="BT9" s="66"/>
+      <c r="BU9" s="66"/>
+      <c r="BV9" s="66"/>
+      <c r="BW9" s="66"/>
+      <c r="BX9" s="66"/>
+      <c r="BY9" s="66"/>
+      <c r="BZ9" s="66"/>
+      <c r="CA9" s="66"/>
+      <c r="CB9" s="66"/>
+      <c r="CC9" s="66"/>
+      <c r="CD9" s="66"/>
+      <c r="CE9" s="66"/>
+      <c r="CF9" s="66"/>
+      <c r="CG9" s="66"/>
+      <c r="CH9" s="66"/>
+      <c r="CI9" s="66"/>
+      <c r="CJ9" s="66"/>
+      <c r="CK9" s="66"/>
+      <c r="CL9" s="66"/>
+      <c r="CM9" s="66"/>
+      <c r="CN9" s="66"/>
+      <c r="CO9" s="66"/>
+      <c r="CP9" s="66"/>
+      <c r="CQ9" s="66"/>
+      <c r="CR9" s="66"/>
+      <c r="CS9" s="66"/>
+      <c r="CT9" s="66"/>
+      <c r="CU9" s="66"/>
+      <c r="CV9" s="66"/>
+      <c r="CW9" s="66"/>
+      <c r="CX9" s="66"/>
+      <c r="CY9" s="66"/>
+      <c r="CZ9" s="66"/>
+      <c r="DA9" s="66"/>
+      <c r="DB9" s="66"/>
+      <c r="DC9" s="66"/>
+      <c r="DD9" s="66"/>
+      <c r="DE9" s="66"/>
+      <c r="DF9" s="66"/>
+      <c r="DG9" s="66"/>
+      <c r="DH9" s="66"/>
+      <c r="DI9" s="66"/>
+      <c r="DJ9" s="66"/>
+      <c r="DK9" s="66"/>
+      <c r="DL9" s="66"/>
+      <c r="DM9" s="66"/>
+      <c r="DN9" s="66"/>
+      <c r="DO9" s="66"/>
+      <c r="DP9" s="66"/>
+      <c r="DQ9" s="66"/>
+      <c r="DR9" s="66"/>
+      <c r="DS9" s="66"/>
+      <c r="DT9" s="66"/>
+      <c r="DU9" s="66"/>
+      <c r="DV9" s="66"/>
+      <c r="DW9" s="66"/>
+      <c r="DX9" s="66"/>
+      <c r="DY9" s="66"/>
+      <c r="DZ9" s="66"/>
+      <c r="EA9" s="66"/>
+      <c r="EB9" s="66"/>
+      <c r="EC9" s="66"/>
+      <c r="ED9" s="66"/>
+      <c r="EE9" s="66"/>
+      <c r="EF9" s="66"/>
+      <c r="EG9" s="66"/>
+      <c r="EH9" s="66"/>
+      <c r="EI9" s="66"/>
+      <c r="EJ9" s="66"/>
+      <c r="EK9" s="66"/>
+      <c r="EL9" s="66"/>
+      <c r="EM9" s="66"/>
+      <c r="EN9" s="66"/>
+      <c r="EO9" s="66"/>
+      <c r="EP9" s="66"/>
+      <c r="EQ9" s="66"/>
+      <c r="ER9" s="66"/>
+      <c r="ES9" s="66"/>
+      <c r="ET9" s="66"/>
+      <c r="EU9" s="66"/>
+      <c r="EV9" s="66"/>
+      <c r="EW9" s="66"/>
+      <c r="EX9" s="66"/>
+      <c r="EY9" s="66"/>
+      <c r="EZ9" s="66"/>
+      <c r="FA9" s="66"/>
+      <c r="FB9" s="66"/>
+      <c r="FC9" s="66"/>
+      <c r="FD9" s="66"/>
+      <c r="FE9" s="66"/>
+      <c r="FF9" s="66"/>
+      <c r="FG9" s="66"/>
+      <c r="FH9" s="66"/>
+      <c r="FI9" s="66"/>
+      <c r="FJ9" s="66"/>
+      <c r="FK9" s="66"/>
+      <c r="FL9" s="66"/>
+      <c r="FM9" s="66"/>
+      <c r="FN9" s="66"/>
+      <c r="FO9" s="66"/>
+      <c r="FP9" s="66"/>
+      <c r="FQ9" s="66"/>
+      <c r="FR9" s="66"/>
+      <c r="FS9" s="66"/>
+      <c r="FT9" s="66"/>
+      <c r="FU9" s="66"/>
+      <c r="FV9" s="66"/>
+      <c r="FW9" s="66"/>
+      <c r="FX9" s="66"/>
+      <c r="FY9" s="66"/>
+      <c r="FZ9" s="66"/>
+      <c r="GA9" s="66"/>
+      <c r="GB9" s="66"/>
+      <c r="GC9" s="66"/>
+      <c r="GD9" s="66"/>
+      <c r="GE9" s="66"/>
+      <c r="GF9" s="66"/>
+      <c r="GG9" s="66"/>
+      <c r="GH9" s="66"/>
+      <c r="GI9" s="66"/>
+      <c r="GJ9" s="66"/>
+      <c r="GK9" s="66"/>
+      <c r="GL9" s="66"/>
+      <c r="GM9" s="66"/>
+      <c r="GN9" s="66"/>
+      <c r="GO9" s="66"/>
+      <c r="GP9" s="66"/>
+      <c r="GQ9" s="66"/>
+      <c r="GR9" s="66"/>
+      <c r="GS9" s="66"/>
+      <c r="GT9" s="66"/>
+      <c r="GU9" s="66"/>
+      <c r="GV9" s="66"/>
+      <c r="GW9" s="66"/>
+      <c r="GX9" s="66"/>
+      <c r="GY9" s="66"/>
+      <c r="GZ9" s="66"/>
+      <c r="HA9" s="66"/>
+      <c r="HB9" s="66"/>
+      <c r="HC9" s="66"/>
+      <c r="HD9" s="66"/>
+      <c r="HE9" s="66"/>
+      <c r="HF9" s="66"/>
+      <c r="HG9" s="66"/>
+      <c r="HH9" s="66"/>
+      <c r="HI9" s="66"/>
+      <c r="HJ9" s="66"/>
+      <c r="HK9" s="66"/>
+      <c r="HL9" s="66"/>
+      <c r="HM9" s="66"/>
+      <c r="HN9" s="66"/>
+      <c r="HO9" s="66"/>
+      <c r="HP9" s="66"/>
+      <c r="HQ9" s="66"/>
+      <c r="HR9" s="66"/>
+      <c r="HS9" s="66"/>
+      <c r="HT9" s="66"/>
+      <c r="HU9" s="66"/>
+      <c r="HV9" s="66"/>
+      <c r="HW9" s="66"/>
+      <c r="HX9" s="66"/>
+      <c r="HY9" s="66"/>
+      <c r="HZ9" s="66"/>
+      <c r="IA9" s="66"/>
+      <c r="IB9" s="66"/>
+      <c r="IC9" s="66"/>
+      <c r="ID9" s="66"/>
+      <c r="IE9" s="66"/>
+      <c r="IF9" s="66"/>
+      <c r="IG9" s="66"/>
+      <c r="IH9" s="66"/>
+      <c r="II9" s="66"/>
+      <c r="IJ9" s="66"/>
+      <c r="IK9" s="66"/>
+      <c r="IL9" s="66"/>
+      <c r="IM9" s="66"/>
+      <c r="IN9" s="66"/>
+      <c r="IO9" s="66"/>
+      <c r="IP9" s="66"/>
+      <c r="IQ9" s="66"/>
+      <c r="IR9" s="66"/>
+      <c r="IS9" s="66"/>
+      <c r="IT9" s="66"/>
+      <c r="IU9" s="66"/>
+      <c r="IV9" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2661,302 +3414,302 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:IV18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="37.6719" style="36" customWidth="1"/>
-    <col min="2" max="2" width="10.6719" style="36" customWidth="1"/>
-    <col min="3" max="3" width="4.67188" style="36" customWidth="1"/>
-    <col min="4" max="4" width="63.6719" style="36" customWidth="1"/>
-    <col min="5" max="5" width="10.6719" style="36" customWidth="1"/>
-    <col min="6" max="6" width="4.67188" style="36" customWidth="1"/>
-    <col min="7" max="7" width="34" style="36" customWidth="1"/>
-    <col min="8" max="8" width="10.6719" style="36" customWidth="1"/>
-    <col min="9" max="256" width="8.85156" style="36" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" style="26" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="26" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="26" customWidth="1"/>
+    <col min="4" max="4" width="63.7109375" style="26" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="26" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" style="26" customWidth="1"/>
+    <col min="7" max="7" width="34" style="26" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="26" customWidth="1"/>
+    <col min="9" max="256" width="8.85546875" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="37">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="39"/>
-      <c r="D1" t="s" s="40">
+      <c r="B1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39"/>
-      <c r="G1" t="s" s="40">
+      <c r="E1" s="28"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="41"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="42">
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1">
+      <c r="A2" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="43">
+      <c r="B2" s="33">
         <v>42715</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" t="s" s="45">
+      <c r="C2" s="34"/>
+      <c r="D2" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="46">
+      <c r="E2" s="36">
         <v>42714</v>
       </c>
-      <c r="F2" s="47"/>
-      <c r="G2" t="s" s="45">
+      <c r="F2" s="37"/>
+      <c r="G2" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="48">
+      <c r="H2" s="38">
         <v>42714</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="49">
+    <row r="3" spans="1:8" ht="15" customHeight="1">
+      <c r="A3" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>42715</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" t="s" s="42">
+      <c r="C3" s="14"/>
+      <c r="D3" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="33">
         <v>42349</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" t="s" s="50">
+      <c r="F3" s="14"/>
+      <c r="G3" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="51">
+      <c r="H3" s="41">
         <v>42715</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="52">
+    <row r="4" spans="1:8" ht="15" customHeight="1">
+      <c r="A4" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="36">
         <v>42714</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" t="s" s="33">
+      <c r="C4" s="43"/>
+      <c r="D4" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>42349</v>
       </c>
-      <c r="F4" s="44"/>
-      <c r="G4" t="s" s="45">
+      <c r="F4" s="34"/>
+      <c r="G4" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="48">
+      <c r="H4" s="38">
         <v>42714</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="42">
+    <row r="5" spans="1:8" ht="15" customHeight="1">
+      <c r="A5" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="43">
+      <c r="B5" s="33">
         <v>42715</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="44"/>
-      <c r="G5" t="s" s="45">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="48">
+      <c r="H5" s="38">
         <v>42714</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="49">
+    <row r="6" spans="1:8" ht="15" customHeight="1">
+      <c r="A6" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <v>42715</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="51"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="55">
+      <c r="C6" s="14"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="41"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1">
+      <c r="A7" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="47"/>
-      <c r="D7" t="s" s="57">
+      <c r="B7" s="46"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="47"/>
-      <c r="G7" t="s" s="57">
+      <c r="E7" s="46"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="H7" s="58"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="42">
+      <c r="H7" s="48"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1">
+      <c r="A8" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="18"/>
-      <c r="D8" t="s" s="42">
+      <c r="B8" s="12"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="18"/>
-      <c r="G8" t="s" s="42">
+      <c r="E8" s="12"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="43">
+      <c r="H8" s="33">
         <v>42715</v>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="33">
+    <row r="9" spans="1:8" ht="15" customHeight="1">
+      <c r="A9" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" t="s" s="33">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" t="s" s="33">
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="18"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-    </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" t="s" s="59">
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1">
+      <c r="A11" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="47"/>
-      <c r="D11" t="s" s="60">
+      <c r="B11" s="19"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="47"/>
-      <c r="G11" t="s" s="60">
+      <c r="E11" s="19"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="61"/>
-    </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="42">
+      <c r="H11" s="51"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1">
+      <c r="A12" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="18"/>
-      <c r="D12" t="s" s="42">
+      <c r="B12" s="12"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="62"/>
-      <c r="F12" s="18"/>
-      <c r="G12" t="s" s="42">
+      <c r="E12" s="52"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="62"/>
-    </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" t="s" s="33">
+      <c r="H12" s="52"/>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="63"/>
-      <c r="F13" s="18"/>
-      <c r="G13" t="s" s="33">
+      <c r="E13" s="53"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-    </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" ht="15" customHeight="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-    </row>
-    <row r="17" ht="15" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-    </row>
-    <row r="18" ht="15" customHeight="1">
-      <c r="A18" t="s" s="64">
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" customHeight="1">
+      <c r="A18" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="66"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="82"/>
+      <c r="G18" s="82"/>
+      <c r="H18" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A18:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2964,151 +3717,150 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:IV13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="37" style="67" customWidth="1"/>
-    <col min="2" max="2" width="15.1719" style="67" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="67" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="67" customWidth="1"/>
-    <col min="5" max="5" width="54.8516" style="67" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="67" customWidth="1"/>
+    <col min="1" max="1" width="37" style="55" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="55" customWidth="1"/>
+    <col min="3" max="4" width="8.85546875" style="55" customWidth="1"/>
+    <col min="5" max="5" width="54.85546875" style="55" customWidth="1"/>
+    <col min="6" max="256" width="8.85546875" style="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="68">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="68">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1">
+      <c r="A2" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="68">
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="B3" t="s" s="68">
+      <c r="B3" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="68">
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="B4" t="s" s="68">
+      <c r="B4" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="69"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="69"/>
-      <c r="B6" t="s" s="68">
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1">
+      <c r="A5" s="57"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1">
+      <c r="A6" s="57"/>
+      <c r="B6" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="C6" t="s" s="68">
+      <c r="C6" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="68">
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1">
+      <c r="A7" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" t="s" s="68">
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="56" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="68">
+    <row r="8" spans="1:5" ht="15" customHeight="1">
+      <c r="A8" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="70">
+      <c r="B8" s="58">
         <v>3</v>
       </c>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="71">
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1">
+      <c r="A9" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="72">
+      <c r="B9" s="60">
         <v>10</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="60">
         <v>12</v>
       </c>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="73"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="69"/>
-    </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" s="73"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="69"/>
-    </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="75">
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1">
+      <c r="A10" s="61"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="57"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1">
+      <c r="A11" s="61"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="57"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1">
+      <c r="A12" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="B12" t="s" s="76">
+      <c r="B12" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="77"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-    </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" t="s" s="68">
+      <c r="C12" s="65"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1">
+      <c r="A13" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3116,131 +3868,128 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:IV13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="119.852" style="78" customWidth="1"/>
-    <col min="2" max="2" width="5.35156" style="78" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="78" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="78" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="78" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="78" customWidth="1"/>
+    <col min="1" max="1" width="119.85546875" style="66" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="66" customWidth="1"/>
+    <col min="3" max="256" width="8.85546875" style="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="68">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="68">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="79">
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="80">
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1">
+      <c r="A5" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-    </row>
-    <row r="6" ht="45" customHeight="1">
-      <c r="A6" t="s" s="81">
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+    </row>
+    <row r="6" spans="1:5" ht="45" customHeight="1">
+      <c r="A6" s="69" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="69"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="79">
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1">
+      <c r="A7" s="57"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1">
+      <c r="A8" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-    </row>
-    <row r="9" ht="30" customHeight="1">
-      <c r="A9" t="s" s="80">
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" customHeight="1">
+      <c r="A9" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="81">
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1">
+      <c r="A10" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-    </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" s="69"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-    </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" s="69"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-    </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" s="82"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1">
+      <c r="A11" s="57"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1">
+      <c r="A12" s="57"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1">
+      <c r="A13" s="70"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Cambiar Producto -> SKU / No. Parte, Modificar consulta con objetivo por ejecutivo incluyendo script para modificar la base de datos
</commit_message>
<xml_diff>
--- a/Scrum.xlsx
+++ b/Scrum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="13620"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="7980" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Actividades Febrero - Toño" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="95">
   <si>
     <t>TOÑO</t>
   </si>
@@ -302,13 +302,16 @@
   </si>
   <si>
     <t>Indicadores - Módulo para asignar objetivos por ejecutivo</t>
+  </si>
+  <si>
+    <t>BUG - Cotización, no se ve la descripción en la previsualización</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -319,6 +322,19 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -672,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -758,6 +774,8 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -782,8 +800,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1996,7 +2018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -2009,11 +2031,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -2068,11 +2090,11 @@
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1">
       <c r="A9" s="11" t="s">
@@ -2131,18 +2153,18 @@
       <c r="C18" s="15"/>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="79"/>
-      <c r="C19" s="80"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="82"/>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1">
-      <c r="A20" s="71" t="s">
+      <c r="A20" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="72"/>
-      <c r="C20" s="73"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2174,11 +2196,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -2251,11 +2273,11 @@
       <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1">
-      <c r="A10" s="74" t="s">
+      <c r="A10" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="77"/>
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1">
       <c r="A11" s="11" t="s">
@@ -2325,18 +2347,18 @@
       <c r="C21" s="15"/>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1">
-      <c r="A22" s="78" t="s">
+      <c r="A22" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="79"/>
-      <c r="C22" s="80"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="82"/>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="73"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2355,26 +2377,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV21"/>
+  <dimension ref="A1:IV22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="75.42578125" style="23" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="23" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="256" width="8.85546875" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:256" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -2397,13 +2419,15 @@
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:256" ht="15" customHeight="1">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="90">
         <v>43071</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="87">
+        <v>43041</v>
+      </c>
     </row>
     <row r="5" spans="1:256" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
@@ -2451,13 +2475,15 @@
       <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:256" ht="15" customHeight="1">
-      <c r="A10" s="83" t="s">
+      <c r="A10" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="86">
         <v>43071</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="87">
+        <v>43041</v>
+      </c>
       <c r="D10" s="66"/>
       <c r="E10" s="66"/>
       <c r="F10" s="66"/>
@@ -2713,7 +2739,7 @@
       <c r="IV10" s="66"/>
     </row>
     <row r="11" spans="1:256" ht="15" customHeight="1">
-      <c r="A11" s="83" t="s">
+      <c r="A11" s="71" t="s">
         <v>91</v>
       </c>
       <c r="B11" s="9">
@@ -2980,11 +3006,11 @@
       <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:256" ht="15" customHeight="1">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="77"/>
     </row>
     <row r="14" spans="1:256" ht="15" customHeight="1">
       <c r="A14" s="11" t="s">
@@ -3001,50 +3027,1575 @@
       <c r="C15" s="15"/>
     </row>
     <row r="16" spans="1:256" ht="15" customHeight="1">
-      <c r="A16" s="8"/>
+      <c r="A16" s="88" t="s">
+        <v>94</v>
+      </c>
       <c r="B16" s="16"/>
       <c r="C16" s="17"/>
-    </row>
-    <row r="17" spans="1:3" customFormat="1" ht="15" customHeight="1">
-      <c r="A17" s="18" t="s">
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="66"/>
+      <c r="N16" s="66"/>
+      <c r="O16" s="66"/>
+      <c r="P16" s="66"/>
+      <c r="Q16" s="66"/>
+      <c r="R16" s="66"/>
+      <c r="S16" s="66"/>
+      <c r="T16" s="66"/>
+      <c r="U16" s="66"/>
+      <c r="V16" s="66"/>
+      <c r="W16" s="66"/>
+      <c r="X16" s="66"/>
+      <c r="Y16" s="66"/>
+      <c r="Z16" s="66"/>
+      <c r="AA16" s="66"/>
+      <c r="AB16" s="66"/>
+      <c r="AC16" s="66"/>
+      <c r="AD16" s="66"/>
+      <c r="AE16" s="66"/>
+      <c r="AF16" s="66"/>
+      <c r="AG16" s="66"/>
+      <c r="AH16" s="66"/>
+      <c r="AI16" s="66"/>
+      <c r="AJ16" s="66"/>
+      <c r="AK16" s="66"/>
+      <c r="AL16" s="66"/>
+      <c r="AM16" s="66"/>
+      <c r="AN16" s="66"/>
+      <c r="AO16" s="66"/>
+      <c r="AP16" s="66"/>
+      <c r="AQ16" s="66"/>
+      <c r="AR16" s="66"/>
+      <c r="AS16" s="66"/>
+      <c r="AT16" s="66"/>
+      <c r="AU16" s="66"/>
+      <c r="AV16" s="66"/>
+      <c r="AW16" s="66"/>
+      <c r="AX16" s="66"/>
+      <c r="AY16" s="66"/>
+      <c r="AZ16" s="66"/>
+      <c r="BA16" s="66"/>
+      <c r="BB16" s="66"/>
+      <c r="BC16" s="66"/>
+      <c r="BD16" s="66"/>
+      <c r="BE16" s="66"/>
+      <c r="BF16" s="66"/>
+      <c r="BG16" s="66"/>
+      <c r="BH16" s="66"/>
+      <c r="BI16" s="66"/>
+      <c r="BJ16" s="66"/>
+      <c r="BK16" s="66"/>
+      <c r="BL16" s="66"/>
+      <c r="BM16" s="66"/>
+      <c r="BN16" s="66"/>
+      <c r="BO16" s="66"/>
+      <c r="BP16" s="66"/>
+      <c r="BQ16" s="66"/>
+      <c r="BR16" s="66"/>
+      <c r="BS16" s="66"/>
+      <c r="BT16" s="66"/>
+      <c r="BU16" s="66"/>
+      <c r="BV16" s="66"/>
+      <c r="BW16" s="66"/>
+      <c r="BX16" s="66"/>
+      <c r="BY16" s="66"/>
+      <c r="BZ16" s="66"/>
+      <c r="CA16" s="66"/>
+      <c r="CB16" s="66"/>
+      <c r="CC16" s="66"/>
+      <c r="CD16" s="66"/>
+      <c r="CE16" s="66"/>
+      <c r="CF16" s="66"/>
+      <c r="CG16" s="66"/>
+      <c r="CH16" s="66"/>
+      <c r="CI16" s="66"/>
+      <c r="CJ16" s="66"/>
+      <c r="CK16" s="66"/>
+      <c r="CL16" s="66"/>
+      <c r="CM16" s="66"/>
+      <c r="CN16" s="66"/>
+      <c r="CO16" s="66"/>
+      <c r="CP16" s="66"/>
+      <c r="CQ16" s="66"/>
+      <c r="CR16" s="66"/>
+      <c r="CS16" s="66"/>
+      <c r="CT16" s="66"/>
+      <c r="CU16" s="66"/>
+      <c r="CV16" s="66"/>
+      <c r="CW16" s="66"/>
+      <c r="CX16" s="66"/>
+      <c r="CY16" s="66"/>
+      <c r="CZ16" s="66"/>
+      <c r="DA16" s="66"/>
+      <c r="DB16" s="66"/>
+      <c r="DC16" s="66"/>
+      <c r="DD16" s="66"/>
+      <c r="DE16" s="66"/>
+      <c r="DF16" s="66"/>
+      <c r="DG16" s="66"/>
+      <c r="DH16" s="66"/>
+      <c r="DI16" s="66"/>
+      <c r="DJ16" s="66"/>
+      <c r="DK16" s="66"/>
+      <c r="DL16" s="66"/>
+      <c r="DM16" s="66"/>
+      <c r="DN16" s="66"/>
+      <c r="DO16" s="66"/>
+      <c r="DP16" s="66"/>
+      <c r="DQ16" s="66"/>
+      <c r="DR16" s="66"/>
+      <c r="DS16" s="66"/>
+      <c r="DT16" s="66"/>
+      <c r="DU16" s="66"/>
+      <c r="DV16" s="66"/>
+      <c r="DW16" s="66"/>
+      <c r="DX16" s="66"/>
+      <c r="DY16" s="66"/>
+      <c r="DZ16" s="66"/>
+      <c r="EA16" s="66"/>
+      <c r="EB16" s="66"/>
+      <c r="EC16" s="66"/>
+      <c r="ED16" s="66"/>
+      <c r="EE16" s="66"/>
+      <c r="EF16" s="66"/>
+      <c r="EG16" s="66"/>
+      <c r="EH16" s="66"/>
+      <c r="EI16" s="66"/>
+      <c r="EJ16" s="66"/>
+      <c r="EK16" s="66"/>
+      <c r="EL16" s="66"/>
+      <c r="EM16" s="66"/>
+      <c r="EN16" s="66"/>
+      <c r="EO16" s="66"/>
+      <c r="EP16" s="66"/>
+      <c r="EQ16" s="66"/>
+      <c r="ER16" s="66"/>
+      <c r="ES16" s="66"/>
+      <c r="ET16" s="66"/>
+      <c r="EU16" s="66"/>
+      <c r="EV16" s="66"/>
+      <c r="EW16" s="66"/>
+      <c r="EX16" s="66"/>
+      <c r="EY16" s="66"/>
+      <c r="EZ16" s="66"/>
+      <c r="FA16" s="66"/>
+      <c r="FB16" s="66"/>
+      <c r="FC16" s="66"/>
+      <c r="FD16" s="66"/>
+      <c r="FE16" s="66"/>
+      <c r="FF16" s="66"/>
+      <c r="FG16" s="66"/>
+      <c r="FH16" s="66"/>
+      <c r="FI16" s="66"/>
+      <c r="FJ16" s="66"/>
+      <c r="FK16" s="66"/>
+      <c r="FL16" s="66"/>
+      <c r="FM16" s="66"/>
+      <c r="FN16" s="66"/>
+      <c r="FO16" s="66"/>
+      <c r="FP16" s="66"/>
+      <c r="FQ16" s="66"/>
+      <c r="FR16" s="66"/>
+      <c r="FS16" s="66"/>
+      <c r="FT16" s="66"/>
+      <c r="FU16" s="66"/>
+      <c r="FV16" s="66"/>
+      <c r="FW16" s="66"/>
+      <c r="FX16" s="66"/>
+      <c r="FY16" s="66"/>
+      <c r="FZ16" s="66"/>
+      <c r="GA16" s="66"/>
+      <c r="GB16" s="66"/>
+      <c r="GC16" s="66"/>
+      <c r="GD16" s="66"/>
+      <c r="GE16" s="66"/>
+      <c r="GF16" s="66"/>
+      <c r="GG16" s="66"/>
+      <c r="GH16" s="66"/>
+      <c r="GI16" s="66"/>
+      <c r="GJ16" s="66"/>
+      <c r="GK16" s="66"/>
+      <c r="GL16" s="66"/>
+      <c r="GM16" s="66"/>
+      <c r="GN16" s="66"/>
+      <c r="GO16" s="66"/>
+      <c r="GP16" s="66"/>
+      <c r="GQ16" s="66"/>
+      <c r="GR16" s="66"/>
+      <c r="GS16" s="66"/>
+      <c r="GT16" s="66"/>
+      <c r="GU16" s="66"/>
+      <c r="GV16" s="66"/>
+      <c r="GW16" s="66"/>
+      <c r="GX16" s="66"/>
+      <c r="GY16" s="66"/>
+      <c r="GZ16" s="66"/>
+      <c r="HA16" s="66"/>
+      <c r="HB16" s="66"/>
+      <c r="HC16" s="66"/>
+      <c r="HD16" s="66"/>
+      <c r="HE16" s="66"/>
+      <c r="HF16" s="66"/>
+      <c r="HG16" s="66"/>
+      <c r="HH16" s="66"/>
+      <c r="HI16" s="66"/>
+      <c r="HJ16" s="66"/>
+      <c r="HK16" s="66"/>
+      <c r="HL16" s="66"/>
+      <c r="HM16" s="66"/>
+      <c r="HN16" s="66"/>
+      <c r="HO16" s="66"/>
+      <c r="HP16" s="66"/>
+      <c r="HQ16" s="66"/>
+      <c r="HR16" s="66"/>
+      <c r="HS16" s="66"/>
+      <c r="HT16" s="66"/>
+      <c r="HU16" s="66"/>
+      <c r="HV16" s="66"/>
+      <c r="HW16" s="66"/>
+      <c r="HX16" s="66"/>
+      <c r="HY16" s="66"/>
+      <c r="HZ16" s="66"/>
+      <c r="IA16" s="66"/>
+      <c r="IB16" s="66"/>
+      <c r="IC16" s="66"/>
+      <c r="ID16" s="66"/>
+      <c r="IE16" s="66"/>
+      <c r="IF16" s="66"/>
+      <c r="IG16" s="66"/>
+      <c r="IH16" s="66"/>
+      <c r="II16" s="66"/>
+      <c r="IJ16" s="66"/>
+      <c r="IK16" s="66"/>
+      <c r="IL16" s="66"/>
+      <c r="IM16" s="66"/>
+      <c r="IN16" s="66"/>
+      <c r="IO16" s="66"/>
+      <c r="IP16" s="66"/>
+      <c r="IQ16" s="66"/>
+      <c r="IR16" s="66"/>
+      <c r="IS16" s="66"/>
+      <c r="IT16" s="66"/>
+      <c r="IU16" s="66"/>
+      <c r="IV16" s="66"/>
+    </row>
+    <row r="17" spans="1:256" ht="15" customHeight="1">
+      <c r="A17" s="8"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+    </row>
+    <row r="18" spans="1:256" ht="15" customHeight="1">
+      <c r="A18" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-    </row>
-    <row r="18" spans="1:3" customFormat="1" ht="15" customHeight="1">
-      <c r="A18" s="20"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-    </row>
-    <row r="19" spans="1:3" customFormat="1" ht="15" customHeight="1">
-      <c r="A19" s="21"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-    </row>
-    <row r="20" spans="1:3" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="78" t="s">
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+      <c r="AA18"/>
+      <c r="AB18"/>
+      <c r="AC18"/>
+      <c r="AD18"/>
+      <c r="AE18"/>
+      <c r="AF18"/>
+      <c r="AG18"/>
+      <c r="AH18"/>
+      <c r="AI18"/>
+      <c r="AJ18"/>
+      <c r="AK18"/>
+      <c r="AL18"/>
+      <c r="AM18"/>
+      <c r="AN18"/>
+      <c r="AO18"/>
+      <c r="AP18"/>
+      <c r="AQ18"/>
+      <c r="AR18"/>
+      <c r="AS18"/>
+      <c r="AT18"/>
+      <c r="AU18"/>
+      <c r="AV18"/>
+      <c r="AW18"/>
+      <c r="AX18"/>
+      <c r="AY18"/>
+      <c r="AZ18"/>
+      <c r="BA18"/>
+      <c r="BB18"/>
+      <c r="BC18"/>
+      <c r="BD18"/>
+      <c r="BE18"/>
+      <c r="BF18"/>
+      <c r="BG18"/>
+      <c r="BH18"/>
+      <c r="BI18"/>
+      <c r="BJ18"/>
+      <c r="BK18"/>
+      <c r="BL18"/>
+      <c r="BM18"/>
+      <c r="BN18"/>
+      <c r="BO18"/>
+      <c r="BP18"/>
+      <c r="BQ18"/>
+      <c r="BR18"/>
+      <c r="BS18"/>
+      <c r="BT18"/>
+      <c r="BU18"/>
+      <c r="BV18"/>
+      <c r="BW18"/>
+      <c r="BX18"/>
+      <c r="BY18"/>
+      <c r="BZ18"/>
+      <c r="CA18"/>
+      <c r="CB18"/>
+      <c r="CC18"/>
+      <c r="CD18"/>
+      <c r="CE18"/>
+      <c r="CF18"/>
+      <c r="CG18"/>
+      <c r="CH18"/>
+      <c r="CI18"/>
+      <c r="CJ18"/>
+      <c r="CK18"/>
+      <c r="CL18"/>
+      <c r="CM18"/>
+      <c r="CN18"/>
+      <c r="CO18"/>
+      <c r="CP18"/>
+      <c r="CQ18"/>
+      <c r="CR18"/>
+      <c r="CS18"/>
+      <c r="CT18"/>
+      <c r="CU18"/>
+      <c r="CV18"/>
+      <c r="CW18"/>
+      <c r="CX18"/>
+      <c r="CY18"/>
+      <c r="CZ18"/>
+      <c r="DA18"/>
+      <c r="DB18"/>
+      <c r="DC18"/>
+      <c r="DD18"/>
+      <c r="DE18"/>
+      <c r="DF18"/>
+      <c r="DG18"/>
+      <c r="DH18"/>
+      <c r="DI18"/>
+      <c r="DJ18"/>
+      <c r="DK18"/>
+      <c r="DL18"/>
+      <c r="DM18"/>
+      <c r="DN18"/>
+      <c r="DO18"/>
+      <c r="DP18"/>
+      <c r="DQ18"/>
+      <c r="DR18"/>
+      <c r="DS18"/>
+      <c r="DT18"/>
+      <c r="DU18"/>
+      <c r="DV18"/>
+      <c r="DW18"/>
+      <c r="DX18"/>
+      <c r="DY18"/>
+      <c r="DZ18"/>
+      <c r="EA18"/>
+      <c r="EB18"/>
+      <c r="EC18"/>
+      <c r="ED18"/>
+      <c r="EE18"/>
+      <c r="EF18"/>
+      <c r="EG18"/>
+      <c r="EH18"/>
+      <c r="EI18"/>
+      <c r="EJ18"/>
+      <c r="EK18"/>
+      <c r="EL18"/>
+      <c r="EM18"/>
+      <c r="EN18"/>
+      <c r="EO18"/>
+      <c r="EP18"/>
+      <c r="EQ18"/>
+      <c r="ER18"/>
+      <c r="ES18"/>
+      <c r="ET18"/>
+      <c r="EU18"/>
+      <c r="EV18"/>
+      <c r="EW18"/>
+      <c r="EX18"/>
+      <c r="EY18"/>
+      <c r="EZ18"/>
+      <c r="FA18"/>
+      <c r="FB18"/>
+      <c r="FC18"/>
+      <c r="FD18"/>
+      <c r="FE18"/>
+      <c r="FF18"/>
+      <c r="FG18"/>
+      <c r="FH18"/>
+      <c r="FI18"/>
+      <c r="FJ18"/>
+      <c r="FK18"/>
+      <c r="FL18"/>
+      <c r="FM18"/>
+      <c r="FN18"/>
+      <c r="FO18"/>
+      <c r="FP18"/>
+      <c r="FQ18"/>
+      <c r="FR18"/>
+      <c r="FS18"/>
+      <c r="FT18"/>
+      <c r="FU18"/>
+      <c r="FV18"/>
+      <c r="FW18"/>
+      <c r="FX18"/>
+      <c r="FY18"/>
+      <c r="FZ18"/>
+      <c r="GA18"/>
+      <c r="GB18"/>
+      <c r="GC18"/>
+      <c r="GD18"/>
+      <c r="GE18"/>
+      <c r="GF18"/>
+      <c r="GG18"/>
+      <c r="GH18"/>
+      <c r="GI18"/>
+      <c r="GJ18"/>
+      <c r="GK18"/>
+      <c r="GL18"/>
+      <c r="GM18"/>
+      <c r="GN18"/>
+      <c r="GO18"/>
+      <c r="GP18"/>
+      <c r="GQ18"/>
+      <c r="GR18"/>
+      <c r="GS18"/>
+      <c r="GT18"/>
+      <c r="GU18"/>
+      <c r="GV18"/>
+      <c r="GW18"/>
+      <c r="GX18"/>
+      <c r="GY18"/>
+      <c r="GZ18"/>
+      <c r="HA18"/>
+      <c r="HB18"/>
+      <c r="HC18"/>
+      <c r="HD18"/>
+      <c r="HE18"/>
+      <c r="HF18"/>
+      <c r="HG18"/>
+      <c r="HH18"/>
+      <c r="HI18"/>
+      <c r="HJ18"/>
+      <c r="HK18"/>
+      <c r="HL18"/>
+      <c r="HM18"/>
+      <c r="HN18"/>
+      <c r="HO18"/>
+      <c r="HP18"/>
+      <c r="HQ18"/>
+      <c r="HR18"/>
+      <c r="HS18"/>
+      <c r="HT18"/>
+      <c r="HU18"/>
+      <c r="HV18"/>
+      <c r="HW18"/>
+      <c r="HX18"/>
+      <c r="HY18"/>
+      <c r="HZ18"/>
+      <c r="IA18"/>
+      <c r="IB18"/>
+      <c r="IC18"/>
+      <c r="ID18"/>
+      <c r="IE18"/>
+      <c r="IF18"/>
+      <c r="IG18"/>
+      <c r="IH18"/>
+      <c r="II18"/>
+      <c r="IJ18"/>
+      <c r="IK18"/>
+      <c r="IL18"/>
+      <c r="IM18"/>
+      <c r="IN18"/>
+      <c r="IO18"/>
+      <c r="IP18"/>
+      <c r="IQ18"/>
+      <c r="IR18"/>
+      <c r="IS18"/>
+      <c r="IT18"/>
+      <c r="IU18"/>
+      <c r="IV18"/>
+    </row>
+    <row r="19" spans="1:256" ht="15" customHeight="1">
+      <c r="A19" s="20"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+      <c r="AB19"/>
+      <c r="AC19"/>
+      <c r="AD19"/>
+      <c r="AE19"/>
+      <c r="AF19"/>
+      <c r="AG19"/>
+      <c r="AH19"/>
+      <c r="AI19"/>
+      <c r="AJ19"/>
+      <c r="AK19"/>
+      <c r="AL19"/>
+      <c r="AM19"/>
+      <c r="AN19"/>
+      <c r="AO19"/>
+      <c r="AP19"/>
+      <c r="AQ19"/>
+      <c r="AR19"/>
+      <c r="AS19"/>
+      <c r="AT19"/>
+      <c r="AU19"/>
+      <c r="AV19"/>
+      <c r="AW19"/>
+      <c r="AX19"/>
+      <c r="AY19"/>
+      <c r="AZ19"/>
+      <c r="BA19"/>
+      <c r="BB19"/>
+      <c r="BC19"/>
+      <c r="BD19"/>
+      <c r="BE19"/>
+      <c r="BF19"/>
+      <c r="BG19"/>
+      <c r="BH19"/>
+      <c r="BI19"/>
+      <c r="BJ19"/>
+      <c r="BK19"/>
+      <c r="BL19"/>
+      <c r="BM19"/>
+      <c r="BN19"/>
+      <c r="BO19"/>
+      <c r="BP19"/>
+      <c r="BQ19"/>
+      <c r="BR19"/>
+      <c r="BS19"/>
+      <c r="BT19"/>
+      <c r="BU19"/>
+      <c r="BV19"/>
+      <c r="BW19"/>
+      <c r="BX19"/>
+      <c r="BY19"/>
+      <c r="BZ19"/>
+      <c r="CA19"/>
+      <c r="CB19"/>
+      <c r="CC19"/>
+      <c r="CD19"/>
+      <c r="CE19"/>
+      <c r="CF19"/>
+      <c r="CG19"/>
+      <c r="CH19"/>
+      <c r="CI19"/>
+      <c r="CJ19"/>
+      <c r="CK19"/>
+      <c r="CL19"/>
+      <c r="CM19"/>
+      <c r="CN19"/>
+      <c r="CO19"/>
+      <c r="CP19"/>
+      <c r="CQ19"/>
+      <c r="CR19"/>
+      <c r="CS19"/>
+      <c r="CT19"/>
+      <c r="CU19"/>
+      <c r="CV19"/>
+      <c r="CW19"/>
+      <c r="CX19"/>
+      <c r="CY19"/>
+      <c r="CZ19"/>
+      <c r="DA19"/>
+      <c r="DB19"/>
+      <c r="DC19"/>
+      <c r="DD19"/>
+      <c r="DE19"/>
+      <c r="DF19"/>
+      <c r="DG19"/>
+      <c r="DH19"/>
+      <c r="DI19"/>
+      <c r="DJ19"/>
+      <c r="DK19"/>
+      <c r="DL19"/>
+      <c r="DM19"/>
+      <c r="DN19"/>
+      <c r="DO19"/>
+      <c r="DP19"/>
+      <c r="DQ19"/>
+      <c r="DR19"/>
+      <c r="DS19"/>
+      <c r="DT19"/>
+      <c r="DU19"/>
+      <c r="DV19"/>
+      <c r="DW19"/>
+      <c r="DX19"/>
+      <c r="DY19"/>
+      <c r="DZ19"/>
+      <c r="EA19"/>
+      <c r="EB19"/>
+      <c r="EC19"/>
+      <c r="ED19"/>
+      <c r="EE19"/>
+      <c r="EF19"/>
+      <c r="EG19"/>
+      <c r="EH19"/>
+      <c r="EI19"/>
+      <c r="EJ19"/>
+      <c r="EK19"/>
+      <c r="EL19"/>
+      <c r="EM19"/>
+      <c r="EN19"/>
+      <c r="EO19"/>
+      <c r="EP19"/>
+      <c r="EQ19"/>
+      <c r="ER19"/>
+      <c r="ES19"/>
+      <c r="ET19"/>
+      <c r="EU19"/>
+      <c r="EV19"/>
+      <c r="EW19"/>
+      <c r="EX19"/>
+      <c r="EY19"/>
+      <c r="EZ19"/>
+      <c r="FA19"/>
+      <c r="FB19"/>
+      <c r="FC19"/>
+      <c r="FD19"/>
+      <c r="FE19"/>
+      <c r="FF19"/>
+      <c r="FG19"/>
+      <c r="FH19"/>
+      <c r="FI19"/>
+      <c r="FJ19"/>
+      <c r="FK19"/>
+      <c r="FL19"/>
+      <c r="FM19"/>
+      <c r="FN19"/>
+      <c r="FO19"/>
+      <c r="FP19"/>
+      <c r="FQ19"/>
+      <c r="FR19"/>
+      <c r="FS19"/>
+      <c r="FT19"/>
+      <c r="FU19"/>
+      <c r="FV19"/>
+      <c r="FW19"/>
+      <c r="FX19"/>
+      <c r="FY19"/>
+      <c r="FZ19"/>
+      <c r="GA19"/>
+      <c r="GB19"/>
+      <c r="GC19"/>
+      <c r="GD19"/>
+      <c r="GE19"/>
+      <c r="GF19"/>
+      <c r="GG19"/>
+      <c r="GH19"/>
+      <c r="GI19"/>
+      <c r="GJ19"/>
+      <c r="GK19"/>
+      <c r="GL19"/>
+      <c r="GM19"/>
+      <c r="GN19"/>
+      <c r="GO19"/>
+      <c r="GP19"/>
+      <c r="GQ19"/>
+      <c r="GR19"/>
+      <c r="GS19"/>
+      <c r="GT19"/>
+      <c r="GU19"/>
+      <c r="GV19"/>
+      <c r="GW19"/>
+      <c r="GX19"/>
+      <c r="GY19"/>
+      <c r="GZ19"/>
+      <c r="HA19"/>
+      <c r="HB19"/>
+      <c r="HC19"/>
+      <c r="HD19"/>
+      <c r="HE19"/>
+      <c r="HF19"/>
+      <c r="HG19"/>
+      <c r="HH19"/>
+      <c r="HI19"/>
+      <c r="HJ19"/>
+      <c r="HK19"/>
+      <c r="HL19"/>
+      <c r="HM19"/>
+      <c r="HN19"/>
+      <c r="HO19"/>
+      <c r="HP19"/>
+      <c r="HQ19"/>
+      <c r="HR19"/>
+      <c r="HS19"/>
+      <c r="HT19"/>
+      <c r="HU19"/>
+      <c r="HV19"/>
+      <c r="HW19"/>
+      <c r="HX19"/>
+      <c r="HY19"/>
+      <c r="HZ19"/>
+      <c r="IA19"/>
+      <c r="IB19"/>
+      <c r="IC19"/>
+      <c r="ID19"/>
+      <c r="IE19"/>
+      <c r="IF19"/>
+      <c r="IG19"/>
+      <c r="IH19"/>
+      <c r="II19"/>
+      <c r="IJ19"/>
+      <c r="IK19"/>
+      <c r="IL19"/>
+      <c r="IM19"/>
+      <c r="IN19"/>
+      <c r="IO19"/>
+      <c r="IP19"/>
+      <c r="IQ19"/>
+      <c r="IR19"/>
+      <c r="IS19"/>
+      <c r="IT19"/>
+      <c r="IU19"/>
+      <c r="IV19"/>
+    </row>
+    <row r="20" spans="1:256" ht="15" customHeight="1">
+      <c r="A20" s="21"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+      <c r="AB20"/>
+      <c r="AC20"/>
+      <c r="AD20"/>
+      <c r="AE20"/>
+      <c r="AF20"/>
+      <c r="AG20"/>
+      <c r="AH20"/>
+      <c r="AI20"/>
+      <c r="AJ20"/>
+      <c r="AK20"/>
+      <c r="AL20"/>
+      <c r="AM20"/>
+      <c r="AN20"/>
+      <c r="AO20"/>
+      <c r="AP20"/>
+      <c r="AQ20"/>
+      <c r="AR20"/>
+      <c r="AS20"/>
+      <c r="AT20"/>
+      <c r="AU20"/>
+      <c r="AV20"/>
+      <c r="AW20"/>
+      <c r="AX20"/>
+      <c r="AY20"/>
+      <c r="AZ20"/>
+      <c r="BA20"/>
+      <c r="BB20"/>
+      <c r="BC20"/>
+      <c r="BD20"/>
+      <c r="BE20"/>
+      <c r="BF20"/>
+      <c r="BG20"/>
+      <c r="BH20"/>
+      <c r="BI20"/>
+      <c r="BJ20"/>
+      <c r="BK20"/>
+      <c r="BL20"/>
+      <c r="BM20"/>
+      <c r="BN20"/>
+      <c r="BO20"/>
+      <c r="BP20"/>
+      <c r="BQ20"/>
+      <c r="BR20"/>
+      <c r="BS20"/>
+      <c r="BT20"/>
+      <c r="BU20"/>
+      <c r="BV20"/>
+      <c r="BW20"/>
+      <c r="BX20"/>
+      <c r="BY20"/>
+      <c r="BZ20"/>
+      <c r="CA20"/>
+      <c r="CB20"/>
+      <c r="CC20"/>
+      <c r="CD20"/>
+      <c r="CE20"/>
+      <c r="CF20"/>
+      <c r="CG20"/>
+      <c r="CH20"/>
+      <c r="CI20"/>
+      <c r="CJ20"/>
+      <c r="CK20"/>
+      <c r="CL20"/>
+      <c r="CM20"/>
+      <c r="CN20"/>
+      <c r="CO20"/>
+      <c r="CP20"/>
+      <c r="CQ20"/>
+      <c r="CR20"/>
+      <c r="CS20"/>
+      <c r="CT20"/>
+      <c r="CU20"/>
+      <c r="CV20"/>
+      <c r="CW20"/>
+      <c r="CX20"/>
+      <c r="CY20"/>
+      <c r="CZ20"/>
+      <c r="DA20"/>
+      <c r="DB20"/>
+      <c r="DC20"/>
+      <c r="DD20"/>
+      <c r="DE20"/>
+      <c r="DF20"/>
+      <c r="DG20"/>
+      <c r="DH20"/>
+      <c r="DI20"/>
+      <c r="DJ20"/>
+      <c r="DK20"/>
+      <c r="DL20"/>
+      <c r="DM20"/>
+      <c r="DN20"/>
+      <c r="DO20"/>
+      <c r="DP20"/>
+      <c r="DQ20"/>
+      <c r="DR20"/>
+      <c r="DS20"/>
+      <c r="DT20"/>
+      <c r="DU20"/>
+      <c r="DV20"/>
+      <c r="DW20"/>
+      <c r="DX20"/>
+      <c r="DY20"/>
+      <c r="DZ20"/>
+      <c r="EA20"/>
+      <c r="EB20"/>
+      <c r="EC20"/>
+      <c r="ED20"/>
+      <c r="EE20"/>
+      <c r="EF20"/>
+      <c r="EG20"/>
+      <c r="EH20"/>
+      <c r="EI20"/>
+      <c r="EJ20"/>
+      <c r="EK20"/>
+      <c r="EL20"/>
+      <c r="EM20"/>
+      <c r="EN20"/>
+      <c r="EO20"/>
+      <c r="EP20"/>
+      <c r="EQ20"/>
+      <c r="ER20"/>
+      <c r="ES20"/>
+      <c r="ET20"/>
+      <c r="EU20"/>
+      <c r="EV20"/>
+      <c r="EW20"/>
+      <c r="EX20"/>
+      <c r="EY20"/>
+      <c r="EZ20"/>
+      <c r="FA20"/>
+      <c r="FB20"/>
+      <c r="FC20"/>
+      <c r="FD20"/>
+      <c r="FE20"/>
+      <c r="FF20"/>
+      <c r="FG20"/>
+      <c r="FH20"/>
+      <c r="FI20"/>
+      <c r="FJ20"/>
+      <c r="FK20"/>
+      <c r="FL20"/>
+      <c r="FM20"/>
+      <c r="FN20"/>
+      <c r="FO20"/>
+      <c r="FP20"/>
+      <c r="FQ20"/>
+      <c r="FR20"/>
+      <c r="FS20"/>
+      <c r="FT20"/>
+      <c r="FU20"/>
+      <c r="FV20"/>
+      <c r="FW20"/>
+      <c r="FX20"/>
+      <c r="FY20"/>
+      <c r="FZ20"/>
+      <c r="GA20"/>
+      <c r="GB20"/>
+      <c r="GC20"/>
+      <c r="GD20"/>
+      <c r="GE20"/>
+      <c r="GF20"/>
+      <c r="GG20"/>
+      <c r="GH20"/>
+      <c r="GI20"/>
+      <c r="GJ20"/>
+      <c r="GK20"/>
+      <c r="GL20"/>
+      <c r="GM20"/>
+      <c r="GN20"/>
+      <c r="GO20"/>
+      <c r="GP20"/>
+      <c r="GQ20"/>
+      <c r="GR20"/>
+      <c r="GS20"/>
+      <c r="GT20"/>
+      <c r="GU20"/>
+      <c r="GV20"/>
+      <c r="GW20"/>
+      <c r="GX20"/>
+      <c r="GY20"/>
+      <c r="GZ20"/>
+      <c r="HA20"/>
+      <c r="HB20"/>
+      <c r="HC20"/>
+      <c r="HD20"/>
+      <c r="HE20"/>
+      <c r="HF20"/>
+      <c r="HG20"/>
+      <c r="HH20"/>
+      <c r="HI20"/>
+      <c r="HJ20"/>
+      <c r="HK20"/>
+      <c r="HL20"/>
+      <c r="HM20"/>
+      <c r="HN20"/>
+      <c r="HO20"/>
+      <c r="HP20"/>
+      <c r="HQ20"/>
+      <c r="HR20"/>
+      <c r="HS20"/>
+      <c r="HT20"/>
+      <c r="HU20"/>
+      <c r="HV20"/>
+      <c r="HW20"/>
+      <c r="HX20"/>
+      <c r="HY20"/>
+      <c r="HZ20"/>
+      <c r="IA20"/>
+      <c r="IB20"/>
+      <c r="IC20"/>
+      <c r="ID20"/>
+      <c r="IE20"/>
+      <c r="IF20"/>
+      <c r="IG20"/>
+      <c r="IH20"/>
+      <c r="II20"/>
+      <c r="IJ20"/>
+      <c r="IK20"/>
+      <c r="IL20"/>
+      <c r="IM20"/>
+      <c r="IN20"/>
+      <c r="IO20"/>
+      <c r="IP20"/>
+      <c r="IQ20"/>
+      <c r="IR20"/>
+      <c r="IS20"/>
+      <c r="IT20"/>
+      <c r="IU20"/>
+      <c r="IV20"/>
+    </row>
+    <row r="21" spans="1:256" ht="15" customHeight="1">
+      <c r="A21" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="79"/>
-      <c r="C20" s="80"/>
-    </row>
-    <row r="21" spans="1:3" customFormat="1" ht="15" customHeight="1">
-      <c r="A21" s="71" t="s">
+      <c r="B21" s="81"/>
+      <c r="C21" s="82"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21"/>
+      <c r="AB21"/>
+      <c r="AC21"/>
+      <c r="AD21"/>
+      <c r="AE21"/>
+      <c r="AF21"/>
+      <c r="AG21"/>
+      <c r="AH21"/>
+      <c r="AI21"/>
+      <c r="AJ21"/>
+      <c r="AK21"/>
+      <c r="AL21"/>
+      <c r="AM21"/>
+      <c r="AN21"/>
+      <c r="AO21"/>
+      <c r="AP21"/>
+      <c r="AQ21"/>
+      <c r="AR21"/>
+      <c r="AS21"/>
+      <c r="AT21"/>
+      <c r="AU21"/>
+      <c r="AV21"/>
+      <c r="AW21"/>
+      <c r="AX21"/>
+      <c r="AY21"/>
+      <c r="AZ21"/>
+      <c r="BA21"/>
+      <c r="BB21"/>
+      <c r="BC21"/>
+      <c r="BD21"/>
+      <c r="BE21"/>
+      <c r="BF21"/>
+      <c r="BG21"/>
+      <c r="BH21"/>
+      <c r="BI21"/>
+      <c r="BJ21"/>
+      <c r="BK21"/>
+      <c r="BL21"/>
+      <c r="BM21"/>
+      <c r="BN21"/>
+      <c r="BO21"/>
+      <c r="BP21"/>
+      <c r="BQ21"/>
+      <c r="BR21"/>
+      <c r="BS21"/>
+      <c r="BT21"/>
+      <c r="BU21"/>
+      <c r="BV21"/>
+      <c r="BW21"/>
+      <c r="BX21"/>
+      <c r="BY21"/>
+      <c r="BZ21"/>
+      <c r="CA21"/>
+      <c r="CB21"/>
+      <c r="CC21"/>
+      <c r="CD21"/>
+      <c r="CE21"/>
+      <c r="CF21"/>
+      <c r="CG21"/>
+      <c r="CH21"/>
+      <c r="CI21"/>
+      <c r="CJ21"/>
+      <c r="CK21"/>
+      <c r="CL21"/>
+      <c r="CM21"/>
+      <c r="CN21"/>
+      <c r="CO21"/>
+      <c r="CP21"/>
+      <c r="CQ21"/>
+      <c r="CR21"/>
+      <c r="CS21"/>
+      <c r="CT21"/>
+      <c r="CU21"/>
+      <c r="CV21"/>
+      <c r="CW21"/>
+      <c r="CX21"/>
+      <c r="CY21"/>
+      <c r="CZ21"/>
+      <c r="DA21"/>
+      <c r="DB21"/>
+      <c r="DC21"/>
+      <c r="DD21"/>
+      <c r="DE21"/>
+      <c r="DF21"/>
+      <c r="DG21"/>
+      <c r="DH21"/>
+      <c r="DI21"/>
+      <c r="DJ21"/>
+      <c r="DK21"/>
+      <c r="DL21"/>
+      <c r="DM21"/>
+      <c r="DN21"/>
+      <c r="DO21"/>
+      <c r="DP21"/>
+      <c r="DQ21"/>
+      <c r="DR21"/>
+      <c r="DS21"/>
+      <c r="DT21"/>
+      <c r="DU21"/>
+      <c r="DV21"/>
+      <c r="DW21"/>
+      <c r="DX21"/>
+      <c r="DY21"/>
+      <c r="DZ21"/>
+      <c r="EA21"/>
+      <c r="EB21"/>
+      <c r="EC21"/>
+      <c r="ED21"/>
+      <c r="EE21"/>
+      <c r="EF21"/>
+      <c r="EG21"/>
+      <c r="EH21"/>
+      <c r="EI21"/>
+      <c r="EJ21"/>
+      <c r="EK21"/>
+      <c r="EL21"/>
+      <c r="EM21"/>
+      <c r="EN21"/>
+      <c r="EO21"/>
+      <c r="EP21"/>
+      <c r="EQ21"/>
+      <c r="ER21"/>
+      <c r="ES21"/>
+      <c r="ET21"/>
+      <c r="EU21"/>
+      <c r="EV21"/>
+      <c r="EW21"/>
+      <c r="EX21"/>
+      <c r="EY21"/>
+      <c r="EZ21"/>
+      <c r="FA21"/>
+      <c r="FB21"/>
+      <c r="FC21"/>
+      <c r="FD21"/>
+      <c r="FE21"/>
+      <c r="FF21"/>
+      <c r="FG21"/>
+      <c r="FH21"/>
+      <c r="FI21"/>
+      <c r="FJ21"/>
+      <c r="FK21"/>
+      <c r="FL21"/>
+      <c r="FM21"/>
+      <c r="FN21"/>
+      <c r="FO21"/>
+      <c r="FP21"/>
+      <c r="FQ21"/>
+      <c r="FR21"/>
+      <c r="FS21"/>
+      <c r="FT21"/>
+      <c r="FU21"/>
+      <c r="FV21"/>
+      <c r="FW21"/>
+      <c r="FX21"/>
+      <c r="FY21"/>
+      <c r="FZ21"/>
+      <c r="GA21"/>
+      <c r="GB21"/>
+      <c r="GC21"/>
+      <c r="GD21"/>
+      <c r="GE21"/>
+      <c r="GF21"/>
+      <c r="GG21"/>
+      <c r="GH21"/>
+      <c r="GI21"/>
+      <c r="GJ21"/>
+      <c r="GK21"/>
+      <c r="GL21"/>
+      <c r="GM21"/>
+      <c r="GN21"/>
+      <c r="GO21"/>
+      <c r="GP21"/>
+      <c r="GQ21"/>
+      <c r="GR21"/>
+      <c r="GS21"/>
+      <c r="GT21"/>
+      <c r="GU21"/>
+      <c r="GV21"/>
+      <c r="GW21"/>
+      <c r="GX21"/>
+      <c r="GY21"/>
+      <c r="GZ21"/>
+      <c r="HA21"/>
+      <c r="HB21"/>
+      <c r="HC21"/>
+      <c r="HD21"/>
+      <c r="HE21"/>
+      <c r="HF21"/>
+      <c r="HG21"/>
+      <c r="HH21"/>
+      <c r="HI21"/>
+      <c r="HJ21"/>
+      <c r="HK21"/>
+      <c r="HL21"/>
+      <c r="HM21"/>
+      <c r="HN21"/>
+      <c r="HO21"/>
+      <c r="HP21"/>
+      <c r="HQ21"/>
+      <c r="HR21"/>
+      <c r="HS21"/>
+      <c r="HT21"/>
+      <c r="HU21"/>
+      <c r="HV21"/>
+      <c r="HW21"/>
+      <c r="HX21"/>
+      <c r="HY21"/>
+      <c r="HZ21"/>
+      <c r="IA21"/>
+      <c r="IB21"/>
+      <c r="IC21"/>
+      <c r="ID21"/>
+      <c r="IE21"/>
+      <c r="IF21"/>
+      <c r="IG21"/>
+      <c r="IH21"/>
+      <c r="II21"/>
+      <c r="IJ21"/>
+      <c r="IK21"/>
+      <c r="IL21"/>
+      <c r="IM21"/>
+      <c r="IN21"/>
+      <c r="IO21"/>
+      <c r="IP21"/>
+      <c r="IQ21"/>
+      <c r="IR21"/>
+      <c r="IS21"/>
+      <c r="IT21"/>
+      <c r="IU21"/>
+      <c r="IV21"/>
+    </row>
+    <row r="22" spans="1:256" ht="15" customHeight="1">
+      <c r="A22" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="73"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="75"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="Y22"/>
+      <c r="Z22"/>
+      <c r="AA22"/>
+      <c r="AB22"/>
+      <c r="AC22"/>
+      <c r="AD22"/>
+      <c r="AE22"/>
+      <c r="AF22"/>
+      <c r="AG22"/>
+      <c r="AH22"/>
+      <c r="AI22"/>
+      <c r="AJ22"/>
+      <c r="AK22"/>
+      <c r="AL22"/>
+      <c r="AM22"/>
+      <c r="AN22"/>
+      <c r="AO22"/>
+      <c r="AP22"/>
+      <c r="AQ22"/>
+      <c r="AR22"/>
+      <c r="AS22"/>
+      <c r="AT22"/>
+      <c r="AU22"/>
+      <c r="AV22"/>
+      <c r="AW22"/>
+      <c r="AX22"/>
+      <c r="AY22"/>
+      <c r="AZ22"/>
+      <c r="BA22"/>
+      <c r="BB22"/>
+      <c r="BC22"/>
+      <c r="BD22"/>
+      <c r="BE22"/>
+      <c r="BF22"/>
+      <c r="BG22"/>
+      <c r="BH22"/>
+      <c r="BI22"/>
+      <c r="BJ22"/>
+      <c r="BK22"/>
+      <c r="BL22"/>
+      <c r="BM22"/>
+      <c r="BN22"/>
+      <c r="BO22"/>
+      <c r="BP22"/>
+      <c r="BQ22"/>
+      <c r="BR22"/>
+      <c r="BS22"/>
+      <c r="BT22"/>
+      <c r="BU22"/>
+      <c r="BV22"/>
+      <c r="BW22"/>
+      <c r="BX22"/>
+      <c r="BY22"/>
+      <c r="BZ22"/>
+      <c r="CA22"/>
+      <c r="CB22"/>
+      <c r="CC22"/>
+      <c r="CD22"/>
+      <c r="CE22"/>
+      <c r="CF22"/>
+      <c r="CG22"/>
+      <c r="CH22"/>
+      <c r="CI22"/>
+      <c r="CJ22"/>
+      <c r="CK22"/>
+      <c r="CL22"/>
+      <c r="CM22"/>
+      <c r="CN22"/>
+      <c r="CO22"/>
+      <c r="CP22"/>
+      <c r="CQ22"/>
+      <c r="CR22"/>
+      <c r="CS22"/>
+      <c r="CT22"/>
+      <c r="CU22"/>
+      <c r="CV22"/>
+      <c r="CW22"/>
+      <c r="CX22"/>
+      <c r="CY22"/>
+      <c r="CZ22"/>
+      <c r="DA22"/>
+      <c r="DB22"/>
+      <c r="DC22"/>
+      <c r="DD22"/>
+      <c r="DE22"/>
+      <c r="DF22"/>
+      <c r="DG22"/>
+      <c r="DH22"/>
+      <c r="DI22"/>
+      <c r="DJ22"/>
+      <c r="DK22"/>
+      <c r="DL22"/>
+      <c r="DM22"/>
+      <c r="DN22"/>
+      <c r="DO22"/>
+      <c r="DP22"/>
+      <c r="DQ22"/>
+      <c r="DR22"/>
+      <c r="DS22"/>
+      <c r="DT22"/>
+      <c r="DU22"/>
+      <c r="DV22"/>
+      <c r="DW22"/>
+      <c r="DX22"/>
+      <c r="DY22"/>
+      <c r="DZ22"/>
+      <c r="EA22"/>
+      <c r="EB22"/>
+      <c r="EC22"/>
+      <c r="ED22"/>
+      <c r="EE22"/>
+      <c r="EF22"/>
+      <c r="EG22"/>
+      <c r="EH22"/>
+      <c r="EI22"/>
+      <c r="EJ22"/>
+      <c r="EK22"/>
+      <c r="EL22"/>
+      <c r="EM22"/>
+      <c r="EN22"/>
+      <c r="EO22"/>
+      <c r="EP22"/>
+      <c r="EQ22"/>
+      <c r="ER22"/>
+      <c r="ES22"/>
+      <c r="ET22"/>
+      <c r="EU22"/>
+      <c r="EV22"/>
+      <c r="EW22"/>
+      <c r="EX22"/>
+      <c r="EY22"/>
+      <c r="EZ22"/>
+      <c r="FA22"/>
+      <c r="FB22"/>
+      <c r="FC22"/>
+      <c r="FD22"/>
+      <c r="FE22"/>
+      <c r="FF22"/>
+      <c r="FG22"/>
+      <c r="FH22"/>
+      <c r="FI22"/>
+      <c r="FJ22"/>
+      <c r="FK22"/>
+      <c r="FL22"/>
+      <c r="FM22"/>
+      <c r="FN22"/>
+      <c r="FO22"/>
+      <c r="FP22"/>
+      <c r="FQ22"/>
+      <c r="FR22"/>
+      <c r="FS22"/>
+      <c r="FT22"/>
+      <c r="FU22"/>
+      <c r="FV22"/>
+      <c r="FW22"/>
+      <c r="FX22"/>
+      <c r="FY22"/>
+      <c r="FZ22"/>
+      <c r="GA22"/>
+      <c r="GB22"/>
+      <c r="GC22"/>
+      <c r="GD22"/>
+      <c r="GE22"/>
+      <c r="GF22"/>
+      <c r="GG22"/>
+      <c r="GH22"/>
+      <c r="GI22"/>
+      <c r="GJ22"/>
+      <c r="GK22"/>
+      <c r="GL22"/>
+      <c r="GM22"/>
+      <c r="GN22"/>
+      <c r="GO22"/>
+      <c r="GP22"/>
+      <c r="GQ22"/>
+      <c r="GR22"/>
+      <c r="GS22"/>
+      <c r="GT22"/>
+      <c r="GU22"/>
+      <c r="GV22"/>
+      <c r="GW22"/>
+      <c r="GX22"/>
+      <c r="GY22"/>
+      <c r="GZ22"/>
+      <c r="HA22"/>
+      <c r="HB22"/>
+      <c r="HC22"/>
+      <c r="HD22"/>
+      <c r="HE22"/>
+      <c r="HF22"/>
+      <c r="HG22"/>
+      <c r="HH22"/>
+      <c r="HI22"/>
+      <c r="HJ22"/>
+      <c r="HK22"/>
+      <c r="HL22"/>
+      <c r="HM22"/>
+      <c r="HN22"/>
+      <c r="HO22"/>
+      <c r="HP22"/>
+      <c r="HQ22"/>
+      <c r="HR22"/>
+      <c r="HS22"/>
+      <c r="HT22"/>
+      <c r="HU22"/>
+      <c r="HV22"/>
+      <c r="HW22"/>
+      <c r="HX22"/>
+      <c r="HY22"/>
+      <c r="HZ22"/>
+      <c r="IA22"/>
+      <c r="IB22"/>
+      <c r="IC22"/>
+      <c r="ID22"/>
+      <c r="IE22"/>
+      <c r="IF22"/>
+      <c r="IG22"/>
+      <c r="IH22"/>
+      <c r="II22"/>
+      <c r="IJ22"/>
+      <c r="IK22"/>
+      <c r="IL22"/>
+      <c r="IM22"/>
+      <c r="IN22"/>
+      <c r="IO22"/>
+      <c r="IP22"/>
+      <c r="IQ22"/>
+      <c r="IR22"/>
+      <c r="IS22"/>
+      <c r="IT22"/>
+      <c r="IU22"/>
+      <c r="IV22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3068,11 +4619,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:256" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -3143,7 +4694,7 @@
       <c r="A9" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="72" t="s">
         <v>40</v>
       </c>
       <c r="C9" s="7"/>
@@ -3693,15 +5244,15 @@
       <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="81" t="s">
+      <c r="A18" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="82"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="82"/>
+      <c r="B18" s="84"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="84"/>
+      <c r="G18" s="84"/>
       <c r="H18" s="54"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregar CC para correos y enviar cotizaciones con copia al correo del ejecutivo
</commit_message>
<xml_diff>
--- a/Scrum.xlsx
+++ b/Scrum.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="96">
   <si>
     <t>TOÑO</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>BUG - Cotización, no se ve la descripción en la previsualización</t>
+  </si>
+  <si>
+    <t>BUG - Cotización, revisar cuando se agrega un nuevo producto</t>
   </si>
 </sst>
 </file>
@@ -776,6 +779,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,12 +809,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2031,11 +2034,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -2090,11 +2093,11 @@
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1">
       <c r="A9" s="11" t="s">
@@ -2153,18 +2156,18 @@
       <c r="C18" s="15"/>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="81"/>
-      <c r="C19" s="82"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="88"/>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1">
-      <c r="A20" s="73" t="s">
+      <c r="A20" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="74"/>
-      <c r="C20" s="75"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2196,11 +2199,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -2273,11 +2276,11 @@
       <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1">
-      <c r="A10" s="76" t="s">
+      <c r="A10" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="83"/>
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1">
       <c r="A11" s="11" t="s">
@@ -2347,18 +2350,18 @@
       <c r="C21" s="15"/>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1">
-      <c r="A22" s="80" t="s">
+      <c r="A22" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="81"/>
-      <c r="C22" s="82"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="88"/>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="75"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2377,10 +2380,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV22"/>
+  <dimension ref="A1:IV23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2392,11 +2395,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
     </row>
     <row r="2" spans="1:256" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -2410,22 +2413,24 @@
       </c>
     </row>
     <row r="3" spans="1:256" ht="15" customHeight="1">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="78">
         <v>43071</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="75">
+        <v>43041</v>
+      </c>
     </row>
     <row r="4" spans="1:256" ht="15" customHeight="1">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="90">
+      <c r="B4" s="78">
         <v>43071</v>
       </c>
-      <c r="C4" s="87">
+      <c r="C4" s="75">
         <v>43041</v>
       </c>
     </row>
@@ -2475,13 +2480,13 @@
       <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:256" ht="15" customHeight="1">
-      <c r="A10" s="85" t="s">
+      <c r="A10" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="86">
+      <c r="B10" s="74">
         <v>43071</v>
       </c>
-      <c r="C10" s="87">
+      <c r="C10" s="75">
         <v>43041</v>
       </c>
       <c r="D10" s="66"/>
@@ -3006,11 +3011,11 @@
       <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:256" ht="15" customHeight="1">
-      <c r="A13" s="76" t="s">
+      <c r="A13" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="83"/>
     </row>
     <row r="14" spans="1:256" ht="15" customHeight="1">
       <c r="A14" s="11" t="s">
@@ -3027,7 +3032,7 @@
       <c r="C15" s="15"/>
     </row>
     <row r="16" spans="1:256" ht="15" customHeight="1">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="76" t="s">
         <v>94</v>
       </c>
       <c r="B16" s="16"/>
@@ -3287,274 +3292,276 @@
       <c r="IV16" s="66"/>
     </row>
     <row r="17" spans="1:256" ht="15" customHeight="1">
-      <c r="A17" s="8"/>
+      <c r="A17" s="76" t="s">
+        <v>95</v>
+      </c>
       <c r="B17" s="16"/>
       <c r="C17" s="17"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="66"/>
+      <c r="O17" s="66"/>
+      <c r="P17" s="66"/>
+      <c r="Q17" s="66"/>
+      <c r="R17" s="66"/>
+      <c r="S17" s="66"/>
+      <c r="T17" s="66"/>
+      <c r="U17" s="66"/>
+      <c r="V17" s="66"/>
+      <c r="W17" s="66"/>
+      <c r="X17" s="66"/>
+      <c r="Y17" s="66"/>
+      <c r="Z17" s="66"/>
+      <c r="AA17" s="66"/>
+      <c r="AB17" s="66"/>
+      <c r="AC17" s="66"/>
+      <c r="AD17" s="66"/>
+      <c r="AE17" s="66"/>
+      <c r="AF17" s="66"/>
+      <c r="AG17" s="66"/>
+      <c r="AH17" s="66"/>
+      <c r="AI17" s="66"/>
+      <c r="AJ17" s="66"/>
+      <c r="AK17" s="66"/>
+      <c r="AL17" s="66"/>
+      <c r="AM17" s="66"/>
+      <c r="AN17" s="66"/>
+      <c r="AO17" s="66"/>
+      <c r="AP17" s="66"/>
+      <c r="AQ17" s="66"/>
+      <c r="AR17" s="66"/>
+      <c r="AS17" s="66"/>
+      <c r="AT17" s="66"/>
+      <c r="AU17" s="66"/>
+      <c r="AV17" s="66"/>
+      <c r="AW17" s="66"/>
+      <c r="AX17" s="66"/>
+      <c r="AY17" s="66"/>
+      <c r="AZ17" s="66"/>
+      <c r="BA17" s="66"/>
+      <c r="BB17" s="66"/>
+      <c r="BC17" s="66"/>
+      <c r="BD17" s="66"/>
+      <c r="BE17" s="66"/>
+      <c r="BF17" s="66"/>
+      <c r="BG17" s="66"/>
+      <c r="BH17" s="66"/>
+      <c r="BI17" s="66"/>
+      <c r="BJ17" s="66"/>
+      <c r="BK17" s="66"/>
+      <c r="BL17" s="66"/>
+      <c r="BM17" s="66"/>
+      <c r="BN17" s="66"/>
+      <c r="BO17" s="66"/>
+      <c r="BP17" s="66"/>
+      <c r="BQ17" s="66"/>
+      <c r="BR17" s="66"/>
+      <c r="BS17" s="66"/>
+      <c r="BT17" s="66"/>
+      <c r="BU17" s="66"/>
+      <c r="BV17" s="66"/>
+      <c r="BW17" s="66"/>
+      <c r="BX17" s="66"/>
+      <c r="BY17" s="66"/>
+      <c r="BZ17" s="66"/>
+      <c r="CA17" s="66"/>
+      <c r="CB17" s="66"/>
+      <c r="CC17" s="66"/>
+      <c r="CD17" s="66"/>
+      <c r="CE17" s="66"/>
+      <c r="CF17" s="66"/>
+      <c r="CG17" s="66"/>
+      <c r="CH17" s="66"/>
+      <c r="CI17" s="66"/>
+      <c r="CJ17" s="66"/>
+      <c r="CK17" s="66"/>
+      <c r="CL17" s="66"/>
+      <c r="CM17" s="66"/>
+      <c r="CN17" s="66"/>
+      <c r="CO17" s="66"/>
+      <c r="CP17" s="66"/>
+      <c r="CQ17" s="66"/>
+      <c r="CR17" s="66"/>
+      <c r="CS17" s="66"/>
+      <c r="CT17" s="66"/>
+      <c r="CU17" s="66"/>
+      <c r="CV17" s="66"/>
+      <c r="CW17" s="66"/>
+      <c r="CX17" s="66"/>
+      <c r="CY17" s="66"/>
+      <c r="CZ17" s="66"/>
+      <c r="DA17" s="66"/>
+      <c r="DB17" s="66"/>
+      <c r="DC17" s="66"/>
+      <c r="DD17" s="66"/>
+      <c r="DE17" s="66"/>
+      <c r="DF17" s="66"/>
+      <c r="DG17" s="66"/>
+      <c r="DH17" s="66"/>
+      <c r="DI17" s="66"/>
+      <c r="DJ17" s="66"/>
+      <c r="DK17" s="66"/>
+      <c r="DL17" s="66"/>
+      <c r="DM17" s="66"/>
+      <c r="DN17" s="66"/>
+      <c r="DO17" s="66"/>
+      <c r="DP17" s="66"/>
+      <c r="DQ17" s="66"/>
+      <c r="DR17" s="66"/>
+      <c r="DS17" s="66"/>
+      <c r="DT17" s="66"/>
+      <c r="DU17" s="66"/>
+      <c r="DV17" s="66"/>
+      <c r="DW17" s="66"/>
+      <c r="DX17" s="66"/>
+      <c r="DY17" s="66"/>
+      <c r="DZ17" s="66"/>
+      <c r="EA17" s="66"/>
+      <c r="EB17" s="66"/>
+      <c r="EC17" s="66"/>
+      <c r="ED17" s="66"/>
+      <c r="EE17" s="66"/>
+      <c r="EF17" s="66"/>
+      <c r="EG17" s="66"/>
+      <c r="EH17" s="66"/>
+      <c r="EI17" s="66"/>
+      <c r="EJ17" s="66"/>
+      <c r="EK17" s="66"/>
+      <c r="EL17" s="66"/>
+      <c r="EM17" s="66"/>
+      <c r="EN17" s="66"/>
+      <c r="EO17" s="66"/>
+      <c r="EP17" s="66"/>
+      <c r="EQ17" s="66"/>
+      <c r="ER17" s="66"/>
+      <c r="ES17" s="66"/>
+      <c r="ET17" s="66"/>
+      <c r="EU17" s="66"/>
+      <c r="EV17" s="66"/>
+      <c r="EW17" s="66"/>
+      <c r="EX17" s="66"/>
+      <c r="EY17" s="66"/>
+      <c r="EZ17" s="66"/>
+      <c r="FA17" s="66"/>
+      <c r="FB17" s="66"/>
+      <c r="FC17" s="66"/>
+      <c r="FD17" s="66"/>
+      <c r="FE17" s="66"/>
+      <c r="FF17" s="66"/>
+      <c r="FG17" s="66"/>
+      <c r="FH17" s="66"/>
+      <c r="FI17" s="66"/>
+      <c r="FJ17" s="66"/>
+      <c r="FK17" s="66"/>
+      <c r="FL17" s="66"/>
+      <c r="FM17" s="66"/>
+      <c r="FN17" s="66"/>
+      <c r="FO17" s="66"/>
+      <c r="FP17" s="66"/>
+      <c r="FQ17" s="66"/>
+      <c r="FR17" s="66"/>
+      <c r="FS17" s="66"/>
+      <c r="FT17" s="66"/>
+      <c r="FU17" s="66"/>
+      <c r="FV17" s="66"/>
+      <c r="FW17" s="66"/>
+      <c r="FX17" s="66"/>
+      <c r="FY17" s="66"/>
+      <c r="FZ17" s="66"/>
+      <c r="GA17" s="66"/>
+      <c r="GB17" s="66"/>
+      <c r="GC17" s="66"/>
+      <c r="GD17" s="66"/>
+      <c r="GE17" s="66"/>
+      <c r="GF17" s="66"/>
+      <c r="GG17" s="66"/>
+      <c r="GH17" s="66"/>
+      <c r="GI17" s="66"/>
+      <c r="GJ17" s="66"/>
+      <c r="GK17" s="66"/>
+      <c r="GL17" s="66"/>
+      <c r="GM17" s="66"/>
+      <c r="GN17" s="66"/>
+      <c r="GO17" s="66"/>
+      <c r="GP17" s="66"/>
+      <c r="GQ17" s="66"/>
+      <c r="GR17" s="66"/>
+      <c r="GS17" s="66"/>
+      <c r="GT17" s="66"/>
+      <c r="GU17" s="66"/>
+      <c r="GV17" s="66"/>
+      <c r="GW17" s="66"/>
+      <c r="GX17" s="66"/>
+      <c r="GY17" s="66"/>
+      <c r="GZ17" s="66"/>
+      <c r="HA17" s="66"/>
+      <c r="HB17" s="66"/>
+      <c r="HC17" s="66"/>
+      <c r="HD17" s="66"/>
+      <c r="HE17" s="66"/>
+      <c r="HF17" s="66"/>
+      <c r="HG17" s="66"/>
+      <c r="HH17" s="66"/>
+      <c r="HI17" s="66"/>
+      <c r="HJ17" s="66"/>
+      <c r="HK17" s="66"/>
+      <c r="HL17" s="66"/>
+      <c r="HM17" s="66"/>
+      <c r="HN17" s="66"/>
+      <c r="HO17" s="66"/>
+      <c r="HP17" s="66"/>
+      <c r="HQ17" s="66"/>
+      <c r="HR17" s="66"/>
+      <c r="HS17" s="66"/>
+      <c r="HT17" s="66"/>
+      <c r="HU17" s="66"/>
+      <c r="HV17" s="66"/>
+      <c r="HW17" s="66"/>
+      <c r="HX17" s="66"/>
+      <c r="HY17" s="66"/>
+      <c r="HZ17" s="66"/>
+      <c r="IA17" s="66"/>
+      <c r="IB17" s="66"/>
+      <c r="IC17" s="66"/>
+      <c r="ID17" s="66"/>
+      <c r="IE17" s="66"/>
+      <c r="IF17" s="66"/>
+      <c r="IG17" s="66"/>
+      <c r="IH17" s="66"/>
+      <c r="II17" s="66"/>
+      <c r="IJ17" s="66"/>
+      <c r="IK17" s="66"/>
+      <c r="IL17" s="66"/>
+      <c r="IM17" s="66"/>
+      <c r="IN17" s="66"/>
+      <c r="IO17" s="66"/>
+      <c r="IP17" s="66"/>
+      <c r="IQ17" s="66"/>
+      <c r="IR17" s="66"/>
+      <c r="IS17" s="66"/>
+      <c r="IT17" s="66"/>
+      <c r="IU17" s="66"/>
+      <c r="IV17" s="66"/>
     </row>
     <row r="18" spans="1:256" ht="15" customHeight="1">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="8"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+    </row>
+    <row r="19" spans="1:256" ht="15" customHeight="1">
+      <c r="A19" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18"/>
-      <c r="N18"/>
-      <c r="O18"/>
-      <c r="P18"/>
-      <c r="Q18"/>
-      <c r="R18"/>
-      <c r="S18"/>
-      <c r="T18"/>
-      <c r="U18"/>
-      <c r="V18"/>
-      <c r="W18"/>
-      <c r="X18"/>
-      <c r="Y18"/>
-      <c r="Z18"/>
-      <c r="AA18"/>
-      <c r="AB18"/>
-      <c r="AC18"/>
-      <c r="AD18"/>
-      <c r="AE18"/>
-      <c r="AF18"/>
-      <c r="AG18"/>
-      <c r="AH18"/>
-      <c r="AI18"/>
-      <c r="AJ18"/>
-      <c r="AK18"/>
-      <c r="AL18"/>
-      <c r="AM18"/>
-      <c r="AN18"/>
-      <c r="AO18"/>
-      <c r="AP18"/>
-      <c r="AQ18"/>
-      <c r="AR18"/>
-      <c r="AS18"/>
-      <c r="AT18"/>
-      <c r="AU18"/>
-      <c r="AV18"/>
-      <c r="AW18"/>
-      <c r="AX18"/>
-      <c r="AY18"/>
-      <c r="AZ18"/>
-      <c r="BA18"/>
-      <c r="BB18"/>
-      <c r="BC18"/>
-      <c r="BD18"/>
-      <c r="BE18"/>
-      <c r="BF18"/>
-      <c r="BG18"/>
-      <c r="BH18"/>
-      <c r="BI18"/>
-      <c r="BJ18"/>
-      <c r="BK18"/>
-      <c r="BL18"/>
-      <c r="BM18"/>
-      <c r="BN18"/>
-      <c r="BO18"/>
-      <c r="BP18"/>
-      <c r="BQ18"/>
-      <c r="BR18"/>
-      <c r="BS18"/>
-      <c r="BT18"/>
-      <c r="BU18"/>
-      <c r="BV18"/>
-      <c r="BW18"/>
-      <c r="BX18"/>
-      <c r="BY18"/>
-      <c r="BZ18"/>
-      <c r="CA18"/>
-      <c r="CB18"/>
-      <c r="CC18"/>
-      <c r="CD18"/>
-      <c r="CE18"/>
-      <c r="CF18"/>
-      <c r="CG18"/>
-      <c r="CH18"/>
-      <c r="CI18"/>
-      <c r="CJ18"/>
-      <c r="CK18"/>
-      <c r="CL18"/>
-      <c r="CM18"/>
-      <c r="CN18"/>
-      <c r="CO18"/>
-      <c r="CP18"/>
-      <c r="CQ18"/>
-      <c r="CR18"/>
-      <c r="CS18"/>
-      <c r="CT18"/>
-      <c r="CU18"/>
-      <c r="CV18"/>
-      <c r="CW18"/>
-      <c r="CX18"/>
-      <c r="CY18"/>
-      <c r="CZ18"/>
-      <c r="DA18"/>
-      <c r="DB18"/>
-      <c r="DC18"/>
-      <c r="DD18"/>
-      <c r="DE18"/>
-      <c r="DF18"/>
-      <c r="DG18"/>
-      <c r="DH18"/>
-      <c r="DI18"/>
-      <c r="DJ18"/>
-      <c r="DK18"/>
-      <c r="DL18"/>
-      <c r="DM18"/>
-      <c r="DN18"/>
-      <c r="DO18"/>
-      <c r="DP18"/>
-      <c r="DQ18"/>
-      <c r="DR18"/>
-      <c r="DS18"/>
-      <c r="DT18"/>
-      <c r="DU18"/>
-      <c r="DV18"/>
-      <c r="DW18"/>
-      <c r="DX18"/>
-      <c r="DY18"/>
-      <c r="DZ18"/>
-      <c r="EA18"/>
-      <c r="EB18"/>
-      <c r="EC18"/>
-      <c r="ED18"/>
-      <c r="EE18"/>
-      <c r="EF18"/>
-      <c r="EG18"/>
-      <c r="EH18"/>
-      <c r="EI18"/>
-      <c r="EJ18"/>
-      <c r="EK18"/>
-      <c r="EL18"/>
-      <c r="EM18"/>
-      <c r="EN18"/>
-      <c r="EO18"/>
-      <c r="EP18"/>
-      <c r="EQ18"/>
-      <c r="ER18"/>
-      <c r="ES18"/>
-      <c r="ET18"/>
-      <c r="EU18"/>
-      <c r="EV18"/>
-      <c r="EW18"/>
-      <c r="EX18"/>
-      <c r="EY18"/>
-      <c r="EZ18"/>
-      <c r="FA18"/>
-      <c r="FB18"/>
-      <c r="FC18"/>
-      <c r="FD18"/>
-      <c r="FE18"/>
-      <c r="FF18"/>
-      <c r="FG18"/>
-      <c r="FH18"/>
-      <c r="FI18"/>
-      <c r="FJ18"/>
-      <c r="FK18"/>
-      <c r="FL18"/>
-      <c r="FM18"/>
-      <c r="FN18"/>
-      <c r="FO18"/>
-      <c r="FP18"/>
-      <c r="FQ18"/>
-      <c r="FR18"/>
-      <c r="FS18"/>
-      <c r="FT18"/>
-      <c r="FU18"/>
-      <c r="FV18"/>
-      <c r="FW18"/>
-      <c r="FX18"/>
-      <c r="FY18"/>
-      <c r="FZ18"/>
-      <c r="GA18"/>
-      <c r="GB18"/>
-      <c r="GC18"/>
-      <c r="GD18"/>
-      <c r="GE18"/>
-      <c r="GF18"/>
-      <c r="GG18"/>
-      <c r="GH18"/>
-      <c r="GI18"/>
-      <c r="GJ18"/>
-      <c r="GK18"/>
-      <c r="GL18"/>
-      <c r="GM18"/>
-      <c r="GN18"/>
-      <c r="GO18"/>
-      <c r="GP18"/>
-      <c r="GQ18"/>
-      <c r="GR18"/>
-      <c r="GS18"/>
-      <c r="GT18"/>
-      <c r="GU18"/>
-      <c r="GV18"/>
-      <c r="GW18"/>
-      <c r="GX18"/>
-      <c r="GY18"/>
-      <c r="GZ18"/>
-      <c r="HA18"/>
-      <c r="HB18"/>
-      <c r="HC18"/>
-      <c r="HD18"/>
-      <c r="HE18"/>
-      <c r="HF18"/>
-      <c r="HG18"/>
-      <c r="HH18"/>
-      <c r="HI18"/>
-      <c r="HJ18"/>
-      <c r="HK18"/>
-      <c r="HL18"/>
-      <c r="HM18"/>
-      <c r="HN18"/>
-      <c r="HO18"/>
-      <c r="HP18"/>
-      <c r="HQ18"/>
-      <c r="HR18"/>
-      <c r="HS18"/>
-      <c r="HT18"/>
-      <c r="HU18"/>
-      <c r="HV18"/>
-      <c r="HW18"/>
-      <c r="HX18"/>
-      <c r="HY18"/>
-      <c r="HZ18"/>
-      <c r="IA18"/>
-      <c r="IB18"/>
-      <c r="IC18"/>
-      <c r="ID18"/>
-      <c r="IE18"/>
-      <c r="IF18"/>
-      <c r="IG18"/>
-      <c r="IH18"/>
-      <c r="II18"/>
-      <c r="IJ18"/>
-      <c r="IK18"/>
-      <c r="IL18"/>
-      <c r="IM18"/>
-      <c r="IN18"/>
-      <c r="IO18"/>
-      <c r="IP18"/>
-      <c r="IQ18"/>
-      <c r="IR18"/>
-      <c r="IS18"/>
-      <c r="IT18"/>
-      <c r="IU18"/>
-      <c r="IV18"/>
-    </row>
-    <row r="19" spans="1:256" ht="15" customHeight="1">
-      <c r="A19" s="20"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
@@ -3810,9 +3817,9 @@
       <c r="IV19"/>
     </row>
     <row r="20" spans="1:256" ht="15" customHeight="1">
-      <c r="A20" s="21"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
@@ -4068,11 +4075,9 @@
       <c r="IV20"/>
     </row>
     <row r="21" spans="1:256" ht="15" customHeight="1">
-      <c r="A21" s="80" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="82"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
@@ -4328,11 +4333,11 @@
       <c r="IV21"/>
     </row>
     <row r="22" spans="1:256" ht="15" customHeight="1">
-      <c r="A22" s="73" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="74"/>
-      <c r="C22" s="75"/>
+      <c r="A22" s="86" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="87"/>
+      <c r="C22" s="88"/>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22"/>
@@ -4587,12 +4592,272 @@
       <c r="IU22"/>
       <c r="IV22"/>
     </row>
+    <row r="23" spans="1:256" ht="15" customHeight="1">
+      <c r="A23" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="80"/>
+      <c r="C23" s="81"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+      <c r="U23"/>
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="Y23"/>
+      <c r="Z23"/>
+      <c r="AA23"/>
+      <c r="AB23"/>
+      <c r="AC23"/>
+      <c r="AD23"/>
+      <c r="AE23"/>
+      <c r="AF23"/>
+      <c r="AG23"/>
+      <c r="AH23"/>
+      <c r="AI23"/>
+      <c r="AJ23"/>
+      <c r="AK23"/>
+      <c r="AL23"/>
+      <c r="AM23"/>
+      <c r="AN23"/>
+      <c r="AO23"/>
+      <c r="AP23"/>
+      <c r="AQ23"/>
+      <c r="AR23"/>
+      <c r="AS23"/>
+      <c r="AT23"/>
+      <c r="AU23"/>
+      <c r="AV23"/>
+      <c r="AW23"/>
+      <c r="AX23"/>
+      <c r="AY23"/>
+      <c r="AZ23"/>
+      <c r="BA23"/>
+      <c r="BB23"/>
+      <c r="BC23"/>
+      <c r="BD23"/>
+      <c r="BE23"/>
+      <c r="BF23"/>
+      <c r="BG23"/>
+      <c r="BH23"/>
+      <c r="BI23"/>
+      <c r="BJ23"/>
+      <c r="BK23"/>
+      <c r="BL23"/>
+      <c r="BM23"/>
+      <c r="BN23"/>
+      <c r="BO23"/>
+      <c r="BP23"/>
+      <c r="BQ23"/>
+      <c r="BR23"/>
+      <c r="BS23"/>
+      <c r="BT23"/>
+      <c r="BU23"/>
+      <c r="BV23"/>
+      <c r="BW23"/>
+      <c r="BX23"/>
+      <c r="BY23"/>
+      <c r="BZ23"/>
+      <c r="CA23"/>
+      <c r="CB23"/>
+      <c r="CC23"/>
+      <c r="CD23"/>
+      <c r="CE23"/>
+      <c r="CF23"/>
+      <c r="CG23"/>
+      <c r="CH23"/>
+      <c r="CI23"/>
+      <c r="CJ23"/>
+      <c r="CK23"/>
+      <c r="CL23"/>
+      <c r="CM23"/>
+      <c r="CN23"/>
+      <c r="CO23"/>
+      <c r="CP23"/>
+      <c r="CQ23"/>
+      <c r="CR23"/>
+      <c r="CS23"/>
+      <c r="CT23"/>
+      <c r="CU23"/>
+      <c r="CV23"/>
+      <c r="CW23"/>
+      <c r="CX23"/>
+      <c r="CY23"/>
+      <c r="CZ23"/>
+      <c r="DA23"/>
+      <c r="DB23"/>
+      <c r="DC23"/>
+      <c r="DD23"/>
+      <c r="DE23"/>
+      <c r="DF23"/>
+      <c r="DG23"/>
+      <c r="DH23"/>
+      <c r="DI23"/>
+      <c r="DJ23"/>
+      <c r="DK23"/>
+      <c r="DL23"/>
+      <c r="DM23"/>
+      <c r="DN23"/>
+      <c r="DO23"/>
+      <c r="DP23"/>
+      <c r="DQ23"/>
+      <c r="DR23"/>
+      <c r="DS23"/>
+      <c r="DT23"/>
+      <c r="DU23"/>
+      <c r="DV23"/>
+      <c r="DW23"/>
+      <c r="DX23"/>
+      <c r="DY23"/>
+      <c r="DZ23"/>
+      <c r="EA23"/>
+      <c r="EB23"/>
+      <c r="EC23"/>
+      <c r="ED23"/>
+      <c r="EE23"/>
+      <c r="EF23"/>
+      <c r="EG23"/>
+      <c r="EH23"/>
+      <c r="EI23"/>
+      <c r="EJ23"/>
+      <c r="EK23"/>
+      <c r="EL23"/>
+      <c r="EM23"/>
+      <c r="EN23"/>
+      <c r="EO23"/>
+      <c r="EP23"/>
+      <c r="EQ23"/>
+      <c r="ER23"/>
+      <c r="ES23"/>
+      <c r="ET23"/>
+      <c r="EU23"/>
+      <c r="EV23"/>
+      <c r="EW23"/>
+      <c r="EX23"/>
+      <c r="EY23"/>
+      <c r="EZ23"/>
+      <c r="FA23"/>
+      <c r="FB23"/>
+      <c r="FC23"/>
+      <c r="FD23"/>
+      <c r="FE23"/>
+      <c r="FF23"/>
+      <c r="FG23"/>
+      <c r="FH23"/>
+      <c r="FI23"/>
+      <c r="FJ23"/>
+      <c r="FK23"/>
+      <c r="FL23"/>
+      <c r="FM23"/>
+      <c r="FN23"/>
+      <c r="FO23"/>
+      <c r="FP23"/>
+      <c r="FQ23"/>
+      <c r="FR23"/>
+      <c r="FS23"/>
+      <c r="FT23"/>
+      <c r="FU23"/>
+      <c r="FV23"/>
+      <c r="FW23"/>
+      <c r="FX23"/>
+      <c r="FY23"/>
+      <c r="FZ23"/>
+      <c r="GA23"/>
+      <c r="GB23"/>
+      <c r="GC23"/>
+      <c r="GD23"/>
+      <c r="GE23"/>
+      <c r="GF23"/>
+      <c r="GG23"/>
+      <c r="GH23"/>
+      <c r="GI23"/>
+      <c r="GJ23"/>
+      <c r="GK23"/>
+      <c r="GL23"/>
+      <c r="GM23"/>
+      <c r="GN23"/>
+      <c r="GO23"/>
+      <c r="GP23"/>
+      <c r="GQ23"/>
+      <c r="GR23"/>
+      <c r="GS23"/>
+      <c r="GT23"/>
+      <c r="GU23"/>
+      <c r="GV23"/>
+      <c r="GW23"/>
+      <c r="GX23"/>
+      <c r="GY23"/>
+      <c r="GZ23"/>
+      <c r="HA23"/>
+      <c r="HB23"/>
+      <c r="HC23"/>
+      <c r="HD23"/>
+      <c r="HE23"/>
+      <c r="HF23"/>
+      <c r="HG23"/>
+      <c r="HH23"/>
+      <c r="HI23"/>
+      <c r="HJ23"/>
+      <c r="HK23"/>
+      <c r="HL23"/>
+      <c r="HM23"/>
+      <c r="HN23"/>
+      <c r="HO23"/>
+      <c r="HP23"/>
+      <c r="HQ23"/>
+      <c r="HR23"/>
+      <c r="HS23"/>
+      <c r="HT23"/>
+      <c r="HU23"/>
+      <c r="HV23"/>
+      <c r="HW23"/>
+      <c r="HX23"/>
+      <c r="HY23"/>
+      <c r="HZ23"/>
+      <c r="IA23"/>
+      <c r="IB23"/>
+      <c r="IC23"/>
+      <c r="ID23"/>
+      <c r="IE23"/>
+      <c r="IF23"/>
+      <c r="IG23"/>
+      <c r="IH23"/>
+      <c r="II23"/>
+      <c r="IJ23"/>
+      <c r="IK23"/>
+      <c r="IL23"/>
+      <c r="IM23"/>
+      <c r="IN23"/>
+      <c r="IO23"/>
+      <c r="IP23"/>
+      <c r="IQ23"/>
+      <c r="IR23"/>
+      <c r="IS23"/>
+      <c r="IT23"/>
+      <c r="IU23"/>
+      <c r="IV23"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4619,11 +4884,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
     </row>
     <row r="2" spans="1:256" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -5244,15 +5509,15 @@
       <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="83" t="s">
+      <c r="A18" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="84"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84"/>
+      <c r="B18" s="90"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
       <c r="H18" s="54"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregar condiciones de compra, nueva dirección y conmutador al final de la cotización
</commit_message>
<xml_diff>
--- a/Scrum.xlsx
+++ b/Scrum.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="98">
   <si>
     <t>TOÑO</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Cotizaciones - Cambiar Producto -&gt; SKU / No. Parte</t>
   </si>
   <si>
-    <t>Cotizaciones - Mostrar dirección fiscal</t>
-  </si>
-  <si>
     <t>Cotizaciones - Capturables: vigencia y tiempos de entrega</t>
   </si>
   <si>
@@ -308,6 +305,15 @@
   </si>
   <si>
     <t>BUG - Cotización, revisar cuando se agrega un nuevo producto</t>
+  </si>
+  <si>
+    <t>Cotización - Enviar como PDF y Excel</t>
+  </si>
+  <si>
+    <t>Cotización - Agregar CP de cliente?</t>
+  </si>
+  <si>
+    <t>Cotizaciones - Mostrar dirección fiscal ??</t>
   </si>
 </sst>
 </file>
@@ -691,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -809,6 +815,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2380,7 +2388,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV23"/>
+  <dimension ref="A1:IV25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -2435,17 +2443,272 @@
       </c>
     </row>
     <row r="5" spans="1:256" ht="15" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="A5" s="77" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="78">
         <v>43071</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="92">
+        <v>43041</v>
+      </c>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="66"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="66"/>
+      <c r="U5" s="66"/>
+      <c r="V5" s="66"/>
+      <c r="W5" s="66"/>
+      <c r="X5" s="66"/>
+      <c r="Y5" s="66"/>
+      <c r="Z5" s="66"/>
+      <c r="AA5" s="66"/>
+      <c r="AB5" s="66"/>
+      <c r="AC5" s="66"/>
+      <c r="AD5" s="66"/>
+      <c r="AE5" s="66"/>
+      <c r="AF5" s="66"/>
+      <c r="AG5" s="66"/>
+      <c r="AH5" s="66"/>
+      <c r="AI5" s="66"/>
+      <c r="AJ5" s="66"/>
+      <c r="AK5" s="66"/>
+      <c r="AL5" s="66"/>
+      <c r="AM5" s="66"/>
+      <c r="AN5" s="66"/>
+      <c r="AO5" s="66"/>
+      <c r="AP5" s="66"/>
+      <c r="AQ5" s="66"/>
+      <c r="AR5" s="66"/>
+      <c r="AS5" s="66"/>
+      <c r="AT5" s="66"/>
+      <c r="AU5" s="66"/>
+      <c r="AV5" s="66"/>
+      <c r="AW5" s="66"/>
+      <c r="AX5" s="66"/>
+      <c r="AY5" s="66"/>
+      <c r="AZ5" s="66"/>
+      <c r="BA5" s="66"/>
+      <c r="BB5" s="66"/>
+      <c r="BC5" s="66"/>
+      <c r="BD5" s="66"/>
+      <c r="BE5" s="66"/>
+      <c r="BF5" s="66"/>
+      <c r="BG5" s="66"/>
+      <c r="BH5" s="66"/>
+      <c r="BI5" s="66"/>
+      <c r="BJ5" s="66"/>
+      <c r="BK5" s="66"/>
+      <c r="BL5" s="66"/>
+      <c r="BM5" s="66"/>
+      <c r="BN5" s="66"/>
+      <c r="BO5" s="66"/>
+      <c r="BP5" s="66"/>
+      <c r="BQ5" s="66"/>
+      <c r="BR5" s="66"/>
+      <c r="BS5" s="66"/>
+      <c r="BT5" s="66"/>
+      <c r="BU5" s="66"/>
+      <c r="BV5" s="66"/>
+      <c r="BW5" s="66"/>
+      <c r="BX5" s="66"/>
+      <c r="BY5" s="66"/>
+      <c r="BZ5" s="66"/>
+      <c r="CA5" s="66"/>
+      <c r="CB5" s="66"/>
+      <c r="CC5" s="66"/>
+      <c r="CD5" s="66"/>
+      <c r="CE5" s="66"/>
+      <c r="CF5" s="66"/>
+      <c r="CG5" s="66"/>
+      <c r="CH5" s="66"/>
+      <c r="CI5" s="66"/>
+      <c r="CJ5" s="66"/>
+      <c r="CK5" s="66"/>
+      <c r="CL5" s="66"/>
+      <c r="CM5" s="66"/>
+      <c r="CN5" s="66"/>
+      <c r="CO5" s="66"/>
+      <c r="CP5" s="66"/>
+      <c r="CQ5" s="66"/>
+      <c r="CR5" s="66"/>
+      <c r="CS5" s="66"/>
+      <c r="CT5" s="66"/>
+      <c r="CU5" s="66"/>
+      <c r="CV5" s="66"/>
+      <c r="CW5" s="66"/>
+      <c r="CX5" s="66"/>
+      <c r="CY5" s="66"/>
+      <c r="CZ5" s="66"/>
+      <c r="DA5" s="66"/>
+      <c r="DB5" s="66"/>
+      <c r="DC5" s="66"/>
+      <c r="DD5" s="66"/>
+      <c r="DE5" s="66"/>
+      <c r="DF5" s="66"/>
+      <c r="DG5" s="66"/>
+      <c r="DH5" s="66"/>
+      <c r="DI5" s="66"/>
+      <c r="DJ5" s="66"/>
+      <c r="DK5" s="66"/>
+      <c r="DL5" s="66"/>
+      <c r="DM5" s="66"/>
+      <c r="DN5" s="66"/>
+      <c r="DO5" s="66"/>
+      <c r="DP5" s="66"/>
+      <c r="DQ5" s="66"/>
+      <c r="DR5" s="66"/>
+      <c r="DS5" s="66"/>
+      <c r="DT5" s="66"/>
+      <c r="DU5" s="66"/>
+      <c r="DV5" s="66"/>
+      <c r="DW5" s="66"/>
+      <c r="DX5" s="66"/>
+      <c r="DY5" s="66"/>
+      <c r="DZ5" s="66"/>
+      <c r="EA5" s="66"/>
+      <c r="EB5" s="66"/>
+      <c r="EC5" s="66"/>
+      <c r="ED5" s="66"/>
+      <c r="EE5" s="66"/>
+      <c r="EF5" s="66"/>
+      <c r="EG5" s="66"/>
+      <c r="EH5" s="66"/>
+      <c r="EI5" s="66"/>
+      <c r="EJ5" s="66"/>
+      <c r="EK5" s="66"/>
+      <c r="EL5" s="66"/>
+      <c r="EM5" s="66"/>
+      <c r="EN5" s="66"/>
+      <c r="EO5" s="66"/>
+      <c r="EP5" s="66"/>
+      <c r="EQ5" s="66"/>
+      <c r="ER5" s="66"/>
+      <c r="ES5" s="66"/>
+      <c r="ET5" s="66"/>
+      <c r="EU5" s="66"/>
+      <c r="EV5" s="66"/>
+      <c r="EW5" s="66"/>
+      <c r="EX5" s="66"/>
+      <c r="EY5" s="66"/>
+      <c r="EZ5" s="66"/>
+      <c r="FA5" s="66"/>
+      <c r="FB5" s="66"/>
+      <c r="FC5" s="66"/>
+      <c r="FD5" s="66"/>
+      <c r="FE5" s="66"/>
+      <c r="FF5" s="66"/>
+      <c r="FG5" s="66"/>
+      <c r="FH5" s="66"/>
+      <c r="FI5" s="66"/>
+      <c r="FJ5" s="66"/>
+      <c r="FK5" s="66"/>
+      <c r="FL5" s="66"/>
+      <c r="FM5" s="66"/>
+      <c r="FN5" s="66"/>
+      <c r="FO5" s="66"/>
+      <c r="FP5" s="66"/>
+      <c r="FQ5" s="66"/>
+      <c r="FR5" s="66"/>
+      <c r="FS5" s="66"/>
+      <c r="FT5" s="66"/>
+      <c r="FU5" s="66"/>
+      <c r="FV5" s="66"/>
+      <c r="FW5" s="66"/>
+      <c r="FX5" s="66"/>
+      <c r="FY5" s="66"/>
+      <c r="FZ5" s="66"/>
+      <c r="GA5" s="66"/>
+      <c r="GB5" s="66"/>
+      <c r="GC5" s="66"/>
+      <c r="GD5" s="66"/>
+      <c r="GE5" s="66"/>
+      <c r="GF5" s="66"/>
+      <c r="GG5" s="66"/>
+      <c r="GH5" s="66"/>
+      <c r="GI5" s="66"/>
+      <c r="GJ5" s="66"/>
+      <c r="GK5" s="66"/>
+      <c r="GL5" s="66"/>
+      <c r="GM5" s="66"/>
+      <c r="GN5" s="66"/>
+      <c r="GO5" s="66"/>
+      <c r="GP5" s="66"/>
+      <c r="GQ5" s="66"/>
+      <c r="GR5" s="66"/>
+      <c r="GS5" s="66"/>
+      <c r="GT5" s="66"/>
+      <c r="GU5" s="66"/>
+      <c r="GV5" s="66"/>
+      <c r="GW5" s="66"/>
+      <c r="GX5" s="66"/>
+      <c r="GY5" s="66"/>
+      <c r="GZ5" s="66"/>
+      <c r="HA5" s="66"/>
+      <c r="HB5" s="66"/>
+      <c r="HC5" s="66"/>
+      <c r="HD5" s="66"/>
+      <c r="HE5" s="66"/>
+      <c r="HF5" s="66"/>
+      <c r="HG5" s="66"/>
+      <c r="HH5" s="66"/>
+      <c r="HI5" s="66"/>
+      <c r="HJ5" s="66"/>
+      <c r="HK5" s="66"/>
+      <c r="HL5" s="66"/>
+      <c r="HM5" s="66"/>
+      <c r="HN5" s="66"/>
+      <c r="HO5" s="66"/>
+      <c r="HP5" s="66"/>
+      <c r="HQ5" s="66"/>
+      <c r="HR5" s="66"/>
+      <c r="HS5" s="66"/>
+      <c r="HT5" s="66"/>
+      <c r="HU5" s="66"/>
+      <c r="HV5" s="66"/>
+      <c r="HW5" s="66"/>
+      <c r="HX5" s="66"/>
+      <c r="HY5" s="66"/>
+      <c r="HZ5" s="66"/>
+      <c r="IA5" s="66"/>
+      <c r="IB5" s="66"/>
+      <c r="IC5" s="66"/>
+      <c r="ID5" s="66"/>
+      <c r="IE5" s="66"/>
+      <c r="IF5" s="66"/>
+      <c r="IG5" s="66"/>
+      <c r="IH5" s="66"/>
+      <c r="II5" s="66"/>
+      <c r="IJ5" s="66"/>
+      <c r="IK5" s="66"/>
+      <c r="IL5" s="66"/>
+      <c r="IM5" s="66"/>
+      <c r="IN5" s="66"/>
+      <c r="IO5" s="66"/>
+      <c r="IP5" s="66"/>
+      <c r="IQ5" s="66"/>
+      <c r="IR5" s="66"/>
+      <c r="IS5" s="66"/>
+      <c r="IT5" s="66"/>
+      <c r="IU5" s="66"/>
+      <c r="IV5" s="66"/>
     </row>
     <row r="6" spans="1:256" ht="15" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="6">
         <v>43071</v>
@@ -2453,13 +2716,15 @@
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:256" ht="15" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="6">
+      <c r="A7" s="77" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="78">
         <v>43071</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="75">
+        <v>43041</v>
+      </c>
     </row>
     <row r="8" spans="1:256" ht="15" customHeight="1">
       <c r="A8" s="5" t="s">
@@ -2471,24 +2736,277 @@
       <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:256" ht="15" customHeight="1">
-      <c r="A9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="6">
+      <c r="A9" s="73" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="74">
         <v>43071</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="75">
+        <v>43041</v>
+      </c>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="66"/>
+      <c r="S9" s="66"/>
+      <c r="T9" s="66"/>
+      <c r="U9" s="66"/>
+      <c r="V9" s="66"/>
+      <c r="W9" s="66"/>
+      <c r="X9" s="66"/>
+      <c r="Y9" s="66"/>
+      <c r="Z9" s="66"/>
+      <c r="AA9" s="66"/>
+      <c r="AB9" s="66"/>
+      <c r="AC9" s="66"/>
+      <c r="AD9" s="66"/>
+      <c r="AE9" s="66"/>
+      <c r="AF9" s="66"/>
+      <c r="AG9" s="66"/>
+      <c r="AH9" s="66"/>
+      <c r="AI9" s="66"/>
+      <c r="AJ9" s="66"/>
+      <c r="AK9" s="66"/>
+      <c r="AL9" s="66"/>
+      <c r="AM9" s="66"/>
+      <c r="AN9" s="66"/>
+      <c r="AO9" s="66"/>
+      <c r="AP9" s="66"/>
+      <c r="AQ9" s="66"/>
+      <c r="AR9" s="66"/>
+      <c r="AS9" s="66"/>
+      <c r="AT9" s="66"/>
+      <c r="AU9" s="66"/>
+      <c r="AV9" s="66"/>
+      <c r="AW9" s="66"/>
+      <c r="AX9" s="66"/>
+      <c r="AY9" s="66"/>
+      <c r="AZ9" s="66"/>
+      <c r="BA9" s="66"/>
+      <c r="BB9" s="66"/>
+      <c r="BC9" s="66"/>
+      <c r="BD9" s="66"/>
+      <c r="BE9" s="66"/>
+      <c r="BF9" s="66"/>
+      <c r="BG9" s="66"/>
+      <c r="BH9" s="66"/>
+      <c r="BI9" s="66"/>
+      <c r="BJ9" s="66"/>
+      <c r="BK9" s="66"/>
+      <c r="BL9" s="66"/>
+      <c r="BM9" s="66"/>
+      <c r="BN9" s="66"/>
+      <c r="BO9" s="66"/>
+      <c r="BP9" s="66"/>
+      <c r="BQ9" s="66"/>
+      <c r="BR9" s="66"/>
+      <c r="BS9" s="66"/>
+      <c r="BT9" s="66"/>
+      <c r="BU9" s="66"/>
+      <c r="BV9" s="66"/>
+      <c r="BW9" s="66"/>
+      <c r="BX9" s="66"/>
+      <c r="BY9" s="66"/>
+      <c r="BZ9" s="66"/>
+      <c r="CA9" s="66"/>
+      <c r="CB9" s="66"/>
+      <c r="CC9" s="66"/>
+      <c r="CD9" s="66"/>
+      <c r="CE9" s="66"/>
+      <c r="CF9" s="66"/>
+      <c r="CG9" s="66"/>
+      <c r="CH9" s="66"/>
+      <c r="CI9" s="66"/>
+      <c r="CJ9" s="66"/>
+      <c r="CK9" s="66"/>
+      <c r="CL9" s="66"/>
+      <c r="CM9" s="66"/>
+      <c r="CN9" s="66"/>
+      <c r="CO9" s="66"/>
+      <c r="CP9" s="66"/>
+      <c r="CQ9" s="66"/>
+      <c r="CR9" s="66"/>
+      <c r="CS9" s="66"/>
+      <c r="CT9" s="66"/>
+      <c r="CU9" s="66"/>
+      <c r="CV9" s="66"/>
+      <c r="CW9" s="66"/>
+      <c r="CX9" s="66"/>
+      <c r="CY9" s="66"/>
+      <c r="CZ9" s="66"/>
+      <c r="DA9" s="66"/>
+      <c r="DB9" s="66"/>
+      <c r="DC9" s="66"/>
+      <c r="DD9" s="66"/>
+      <c r="DE9" s="66"/>
+      <c r="DF9" s="66"/>
+      <c r="DG9" s="66"/>
+      <c r="DH9" s="66"/>
+      <c r="DI9" s="66"/>
+      <c r="DJ9" s="66"/>
+      <c r="DK9" s="66"/>
+      <c r="DL9" s="66"/>
+      <c r="DM9" s="66"/>
+      <c r="DN9" s="66"/>
+      <c r="DO9" s="66"/>
+      <c r="DP9" s="66"/>
+      <c r="DQ9" s="66"/>
+      <c r="DR9" s="66"/>
+      <c r="DS9" s="66"/>
+      <c r="DT9" s="66"/>
+      <c r="DU9" s="66"/>
+      <c r="DV9" s="66"/>
+      <c r="DW9" s="66"/>
+      <c r="DX9" s="66"/>
+      <c r="DY9" s="66"/>
+      <c r="DZ9" s="66"/>
+      <c r="EA9" s="66"/>
+      <c r="EB9" s="66"/>
+      <c r="EC9" s="66"/>
+      <c r="ED9" s="66"/>
+      <c r="EE9" s="66"/>
+      <c r="EF9" s="66"/>
+      <c r="EG9" s="66"/>
+      <c r="EH9" s="66"/>
+      <c r="EI9" s="66"/>
+      <c r="EJ9" s="66"/>
+      <c r="EK9" s="66"/>
+      <c r="EL9" s="66"/>
+      <c r="EM9" s="66"/>
+      <c r="EN9" s="66"/>
+      <c r="EO9" s="66"/>
+      <c r="EP9" s="66"/>
+      <c r="EQ9" s="66"/>
+      <c r="ER9" s="66"/>
+      <c r="ES9" s="66"/>
+      <c r="ET9" s="66"/>
+      <c r="EU9" s="66"/>
+      <c r="EV9" s="66"/>
+      <c r="EW9" s="66"/>
+      <c r="EX9" s="66"/>
+      <c r="EY9" s="66"/>
+      <c r="EZ9" s="66"/>
+      <c r="FA9" s="66"/>
+      <c r="FB9" s="66"/>
+      <c r="FC9" s="66"/>
+      <c r="FD9" s="66"/>
+      <c r="FE9" s="66"/>
+      <c r="FF9" s="66"/>
+      <c r="FG9" s="66"/>
+      <c r="FH9" s="66"/>
+      <c r="FI9" s="66"/>
+      <c r="FJ9" s="66"/>
+      <c r="FK9" s="66"/>
+      <c r="FL9" s="66"/>
+      <c r="FM9" s="66"/>
+      <c r="FN9" s="66"/>
+      <c r="FO9" s="66"/>
+      <c r="FP9" s="66"/>
+      <c r="FQ9" s="66"/>
+      <c r="FR9" s="66"/>
+      <c r="FS9" s="66"/>
+      <c r="FT9" s="66"/>
+      <c r="FU9" s="66"/>
+      <c r="FV9" s="66"/>
+      <c r="FW9" s="66"/>
+      <c r="FX9" s="66"/>
+      <c r="FY9" s="66"/>
+      <c r="FZ9" s="66"/>
+      <c r="GA9" s="66"/>
+      <c r="GB9" s="66"/>
+      <c r="GC9" s="66"/>
+      <c r="GD9" s="66"/>
+      <c r="GE9" s="66"/>
+      <c r="GF9" s="66"/>
+      <c r="GG9" s="66"/>
+      <c r="GH9" s="66"/>
+      <c r="GI9" s="66"/>
+      <c r="GJ9" s="66"/>
+      <c r="GK9" s="66"/>
+      <c r="GL9" s="66"/>
+      <c r="GM9" s="66"/>
+      <c r="GN9" s="66"/>
+      <c r="GO9" s="66"/>
+      <c r="GP9" s="66"/>
+      <c r="GQ9" s="66"/>
+      <c r="GR9" s="66"/>
+      <c r="GS9" s="66"/>
+      <c r="GT9" s="66"/>
+      <c r="GU9" s="66"/>
+      <c r="GV9" s="66"/>
+      <c r="GW9" s="66"/>
+      <c r="GX9" s="66"/>
+      <c r="GY9" s="66"/>
+      <c r="GZ9" s="66"/>
+      <c r="HA9" s="66"/>
+      <c r="HB9" s="66"/>
+      <c r="HC9" s="66"/>
+      <c r="HD9" s="66"/>
+      <c r="HE9" s="66"/>
+      <c r="HF9" s="66"/>
+      <c r="HG9" s="66"/>
+      <c r="HH9" s="66"/>
+      <c r="HI9" s="66"/>
+      <c r="HJ9" s="66"/>
+      <c r="HK9" s="66"/>
+      <c r="HL9" s="66"/>
+      <c r="HM9" s="66"/>
+      <c r="HN9" s="66"/>
+      <c r="HO9" s="66"/>
+      <c r="HP9" s="66"/>
+      <c r="HQ9" s="66"/>
+      <c r="HR9" s="66"/>
+      <c r="HS9" s="66"/>
+      <c r="HT9" s="66"/>
+      <c r="HU9" s="66"/>
+      <c r="HV9" s="66"/>
+      <c r="HW9" s="66"/>
+      <c r="HX9" s="66"/>
+      <c r="HY9" s="66"/>
+      <c r="HZ9" s="66"/>
+      <c r="IA9" s="66"/>
+      <c r="IB9" s="66"/>
+      <c r="IC9" s="66"/>
+      <c r="ID9" s="66"/>
+      <c r="IE9" s="66"/>
+      <c r="IF9" s="66"/>
+      <c r="IG9" s="66"/>
+      <c r="IH9" s="66"/>
+      <c r="II9" s="66"/>
+      <c r="IJ9" s="66"/>
+      <c r="IK9" s="66"/>
+      <c r="IL9" s="66"/>
+      <c r="IM9" s="66"/>
+      <c r="IN9" s="66"/>
+      <c r="IO9" s="66"/>
+      <c r="IP9" s="66"/>
+      <c r="IQ9" s="66"/>
+      <c r="IR9" s="66"/>
+      <c r="IS9" s="66"/>
+      <c r="IT9" s="66"/>
+      <c r="IU9" s="66"/>
+      <c r="IV9" s="66"/>
     </row>
     <row r="10" spans="1:256" ht="15" customHeight="1">
-      <c r="A10" s="73" t="s">
-        <v>92</v>
-      </c>
-      <c r="B10" s="74">
+      <c r="A10" s="71" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="9">
         <v>43071</v>
       </c>
-      <c r="C10" s="75">
-        <v>43041</v>
-      </c>
+      <c r="C10" s="10"/>
       <c r="D10" s="66"/>
       <c r="E10" s="66"/>
       <c r="F10" s="66"/>
@@ -2744,292 +3262,543 @@
       <c r="IV10" s="66"/>
     </row>
     <row r="11" spans="1:256" ht="15" customHeight="1">
-      <c r="A11" s="71" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="9">
-        <v>43071</v>
-      </c>
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="10"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
-      <c r="O11" s="66"/>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="66"/>
-      <c r="R11" s="66"/>
-      <c r="S11" s="66"/>
-      <c r="T11" s="66"/>
-      <c r="U11" s="66"/>
-      <c r="V11" s="66"/>
-      <c r="W11" s="66"/>
-      <c r="X11" s="66"/>
-      <c r="Y11" s="66"/>
-      <c r="Z11" s="66"/>
-      <c r="AA11" s="66"/>
-      <c r="AB11" s="66"/>
-      <c r="AC11" s="66"/>
-      <c r="AD11" s="66"/>
-      <c r="AE11" s="66"/>
-      <c r="AF11" s="66"/>
-      <c r="AG11" s="66"/>
-      <c r="AH11" s="66"/>
-      <c r="AI11" s="66"/>
-      <c r="AJ11" s="66"/>
-      <c r="AK11" s="66"/>
-      <c r="AL11" s="66"/>
-      <c r="AM11" s="66"/>
-      <c r="AN11" s="66"/>
-      <c r="AO11" s="66"/>
-      <c r="AP11" s="66"/>
-      <c r="AQ11" s="66"/>
-      <c r="AR11" s="66"/>
-      <c r="AS11" s="66"/>
-      <c r="AT11" s="66"/>
-      <c r="AU11" s="66"/>
-      <c r="AV11" s="66"/>
-      <c r="AW11" s="66"/>
-      <c r="AX11" s="66"/>
-      <c r="AY11" s="66"/>
-      <c r="AZ11" s="66"/>
-      <c r="BA11" s="66"/>
-      <c r="BB11" s="66"/>
-      <c r="BC11" s="66"/>
-      <c r="BD11" s="66"/>
-      <c r="BE11" s="66"/>
-      <c r="BF11" s="66"/>
-      <c r="BG11" s="66"/>
-      <c r="BH11" s="66"/>
-      <c r="BI11" s="66"/>
-      <c r="BJ11" s="66"/>
-      <c r="BK11" s="66"/>
-      <c r="BL11" s="66"/>
-      <c r="BM11" s="66"/>
-      <c r="BN11" s="66"/>
-      <c r="BO11" s="66"/>
-      <c r="BP11" s="66"/>
-      <c r="BQ11" s="66"/>
-      <c r="BR11" s="66"/>
-      <c r="BS11" s="66"/>
-      <c r="BT11" s="66"/>
-      <c r="BU11" s="66"/>
-      <c r="BV11" s="66"/>
-      <c r="BW11" s="66"/>
-      <c r="BX11" s="66"/>
-      <c r="BY11" s="66"/>
-      <c r="BZ11" s="66"/>
-      <c r="CA11" s="66"/>
-      <c r="CB11" s="66"/>
-      <c r="CC11" s="66"/>
-      <c r="CD11" s="66"/>
-      <c r="CE11" s="66"/>
-      <c r="CF11" s="66"/>
-      <c r="CG11" s="66"/>
-      <c r="CH11" s="66"/>
-      <c r="CI11" s="66"/>
-      <c r="CJ11" s="66"/>
-      <c r="CK11" s="66"/>
-      <c r="CL11" s="66"/>
-      <c r="CM11" s="66"/>
-      <c r="CN11" s="66"/>
-      <c r="CO11" s="66"/>
-      <c r="CP11" s="66"/>
-      <c r="CQ11" s="66"/>
-      <c r="CR11" s="66"/>
-      <c r="CS11" s="66"/>
-      <c r="CT11" s="66"/>
-      <c r="CU11" s="66"/>
-      <c r="CV11" s="66"/>
-      <c r="CW11" s="66"/>
-      <c r="CX11" s="66"/>
-      <c r="CY11" s="66"/>
-      <c r="CZ11" s="66"/>
-      <c r="DA11" s="66"/>
-      <c r="DB11" s="66"/>
-      <c r="DC11" s="66"/>
-      <c r="DD11" s="66"/>
-      <c r="DE11" s="66"/>
-      <c r="DF11" s="66"/>
-      <c r="DG11" s="66"/>
-      <c r="DH11" s="66"/>
-      <c r="DI11" s="66"/>
-      <c r="DJ11" s="66"/>
-      <c r="DK11" s="66"/>
-      <c r="DL11" s="66"/>
-      <c r="DM11" s="66"/>
-      <c r="DN11" s="66"/>
-      <c r="DO11" s="66"/>
-      <c r="DP11" s="66"/>
-      <c r="DQ11" s="66"/>
-      <c r="DR11" s="66"/>
-      <c r="DS11" s="66"/>
-      <c r="DT11" s="66"/>
-      <c r="DU11" s="66"/>
-      <c r="DV11" s="66"/>
-      <c r="DW11" s="66"/>
-      <c r="DX11" s="66"/>
-      <c r="DY11" s="66"/>
-      <c r="DZ11" s="66"/>
-      <c r="EA11" s="66"/>
-      <c r="EB11" s="66"/>
-      <c r="EC11" s="66"/>
-      <c r="ED11" s="66"/>
-      <c r="EE11" s="66"/>
-      <c r="EF11" s="66"/>
-      <c r="EG11" s="66"/>
-      <c r="EH11" s="66"/>
-      <c r="EI11" s="66"/>
-      <c r="EJ11" s="66"/>
-      <c r="EK11" s="66"/>
-      <c r="EL11" s="66"/>
-      <c r="EM11" s="66"/>
-      <c r="EN11" s="66"/>
-      <c r="EO11" s="66"/>
-      <c r="EP11" s="66"/>
-      <c r="EQ11" s="66"/>
-      <c r="ER11" s="66"/>
-      <c r="ES11" s="66"/>
-      <c r="ET11" s="66"/>
-      <c r="EU11" s="66"/>
-      <c r="EV11" s="66"/>
-      <c r="EW11" s="66"/>
-      <c r="EX11" s="66"/>
-      <c r="EY11" s="66"/>
-      <c r="EZ11" s="66"/>
-      <c r="FA11" s="66"/>
-      <c r="FB11" s="66"/>
-      <c r="FC11" s="66"/>
-      <c r="FD11" s="66"/>
-      <c r="FE11" s="66"/>
-      <c r="FF11" s="66"/>
-      <c r="FG11" s="66"/>
-      <c r="FH11" s="66"/>
-      <c r="FI11" s="66"/>
-      <c r="FJ11" s="66"/>
-      <c r="FK11" s="66"/>
-      <c r="FL11" s="66"/>
-      <c r="FM11" s="66"/>
-      <c r="FN11" s="66"/>
-      <c r="FO11" s="66"/>
-      <c r="FP11" s="66"/>
-      <c r="FQ11" s="66"/>
-      <c r="FR11" s="66"/>
-      <c r="FS11" s="66"/>
-      <c r="FT11" s="66"/>
-      <c r="FU11" s="66"/>
-      <c r="FV11" s="66"/>
-      <c r="FW11" s="66"/>
-      <c r="FX11" s="66"/>
-      <c r="FY11" s="66"/>
-      <c r="FZ11" s="66"/>
-      <c r="GA11" s="66"/>
-      <c r="GB11" s="66"/>
-      <c r="GC11" s="66"/>
-      <c r="GD11" s="66"/>
-      <c r="GE11" s="66"/>
-      <c r="GF11" s="66"/>
-      <c r="GG11" s="66"/>
-      <c r="GH11" s="66"/>
-      <c r="GI11" s="66"/>
-      <c r="GJ11" s="66"/>
-      <c r="GK11" s="66"/>
-      <c r="GL11" s="66"/>
-      <c r="GM11" s="66"/>
-      <c r="GN11" s="66"/>
-      <c r="GO11" s="66"/>
-      <c r="GP11" s="66"/>
-      <c r="GQ11" s="66"/>
-      <c r="GR11" s="66"/>
-      <c r="GS11" s="66"/>
-      <c r="GT11" s="66"/>
-      <c r="GU11" s="66"/>
-      <c r="GV11" s="66"/>
-      <c r="GW11" s="66"/>
-      <c r="GX11" s="66"/>
-      <c r="GY11" s="66"/>
-      <c r="GZ11" s="66"/>
-      <c r="HA11" s="66"/>
-      <c r="HB11" s="66"/>
-      <c r="HC11" s="66"/>
-      <c r="HD11" s="66"/>
-      <c r="HE11" s="66"/>
-      <c r="HF11" s="66"/>
-      <c r="HG11" s="66"/>
-      <c r="HH11" s="66"/>
-      <c r="HI11" s="66"/>
-      <c r="HJ11" s="66"/>
-      <c r="HK11" s="66"/>
-      <c r="HL11" s="66"/>
-      <c r="HM11" s="66"/>
-      <c r="HN11" s="66"/>
-      <c r="HO11" s="66"/>
-      <c r="HP11" s="66"/>
-      <c r="HQ11" s="66"/>
-      <c r="HR11" s="66"/>
-      <c r="HS11" s="66"/>
-      <c r="HT11" s="66"/>
-      <c r="HU11" s="66"/>
-      <c r="HV11" s="66"/>
-      <c r="HW11" s="66"/>
-      <c r="HX11" s="66"/>
-      <c r="HY11" s="66"/>
-      <c r="HZ11" s="66"/>
-      <c r="IA11" s="66"/>
-      <c r="IB11" s="66"/>
-      <c r="IC11" s="66"/>
-      <c r="ID11" s="66"/>
-      <c r="IE11" s="66"/>
-      <c r="IF11" s="66"/>
-      <c r="IG11" s="66"/>
-      <c r="IH11" s="66"/>
-      <c r="II11" s="66"/>
-      <c r="IJ11" s="66"/>
-      <c r="IK11" s="66"/>
-      <c r="IL11" s="66"/>
-      <c r="IM11" s="66"/>
-      <c r="IN11" s="66"/>
-      <c r="IO11" s="66"/>
-      <c r="IP11" s="66"/>
-      <c r="IQ11" s="66"/>
-      <c r="IR11" s="66"/>
-      <c r="IS11" s="66"/>
-      <c r="IT11" s="66"/>
-      <c r="IU11" s="66"/>
-      <c r="IV11" s="66"/>
     </row>
     <row r="12" spans="1:256" ht="15" customHeight="1">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
+      <c r="A12" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
     </row>
     <row r="13" spans="1:256" ht="15" customHeight="1">
-      <c r="A13" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="83"/>
-      <c r="C13" s="83"/>
+      <c r="A13" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
     </row>
     <row r="14" spans="1:256" ht="15" customHeight="1">
-      <c r="A14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
+      <c r="A14" s="91" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="66"/>
+      <c r="L14" s="66"/>
+      <c r="M14" s="66"/>
+      <c r="N14" s="66"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="66"/>
+      <c r="Q14" s="66"/>
+      <c r="R14" s="66"/>
+      <c r="S14" s="66"/>
+      <c r="T14" s="66"/>
+      <c r="U14" s="66"/>
+      <c r="V14" s="66"/>
+      <c r="W14" s="66"/>
+      <c r="X14" s="66"/>
+      <c r="Y14" s="66"/>
+      <c r="Z14" s="66"/>
+      <c r="AA14" s="66"/>
+      <c r="AB14" s="66"/>
+      <c r="AC14" s="66"/>
+      <c r="AD14" s="66"/>
+      <c r="AE14" s="66"/>
+      <c r="AF14" s="66"/>
+      <c r="AG14" s="66"/>
+      <c r="AH14" s="66"/>
+      <c r="AI14" s="66"/>
+      <c r="AJ14" s="66"/>
+      <c r="AK14" s="66"/>
+      <c r="AL14" s="66"/>
+      <c r="AM14" s="66"/>
+      <c r="AN14" s="66"/>
+      <c r="AO14" s="66"/>
+      <c r="AP14" s="66"/>
+      <c r="AQ14" s="66"/>
+      <c r="AR14" s="66"/>
+      <c r="AS14" s="66"/>
+      <c r="AT14" s="66"/>
+      <c r="AU14" s="66"/>
+      <c r="AV14" s="66"/>
+      <c r="AW14" s="66"/>
+      <c r="AX14" s="66"/>
+      <c r="AY14" s="66"/>
+      <c r="AZ14" s="66"/>
+      <c r="BA14" s="66"/>
+      <c r="BB14" s="66"/>
+      <c r="BC14" s="66"/>
+      <c r="BD14" s="66"/>
+      <c r="BE14" s="66"/>
+      <c r="BF14" s="66"/>
+      <c r="BG14" s="66"/>
+      <c r="BH14" s="66"/>
+      <c r="BI14" s="66"/>
+      <c r="BJ14" s="66"/>
+      <c r="BK14" s="66"/>
+      <c r="BL14" s="66"/>
+      <c r="BM14" s="66"/>
+      <c r="BN14" s="66"/>
+      <c r="BO14" s="66"/>
+      <c r="BP14" s="66"/>
+      <c r="BQ14" s="66"/>
+      <c r="BR14" s="66"/>
+      <c r="BS14" s="66"/>
+      <c r="BT14" s="66"/>
+      <c r="BU14" s="66"/>
+      <c r="BV14" s="66"/>
+      <c r="BW14" s="66"/>
+      <c r="BX14" s="66"/>
+      <c r="BY14" s="66"/>
+      <c r="BZ14" s="66"/>
+      <c r="CA14" s="66"/>
+      <c r="CB14" s="66"/>
+      <c r="CC14" s="66"/>
+      <c r="CD14" s="66"/>
+      <c r="CE14" s="66"/>
+      <c r="CF14" s="66"/>
+      <c r="CG14" s="66"/>
+      <c r="CH14" s="66"/>
+      <c r="CI14" s="66"/>
+      <c r="CJ14" s="66"/>
+      <c r="CK14" s="66"/>
+      <c r="CL14" s="66"/>
+      <c r="CM14" s="66"/>
+      <c r="CN14" s="66"/>
+      <c r="CO14" s="66"/>
+      <c r="CP14" s="66"/>
+      <c r="CQ14" s="66"/>
+      <c r="CR14" s="66"/>
+      <c r="CS14" s="66"/>
+      <c r="CT14" s="66"/>
+      <c r="CU14" s="66"/>
+      <c r="CV14" s="66"/>
+      <c r="CW14" s="66"/>
+      <c r="CX14" s="66"/>
+      <c r="CY14" s="66"/>
+      <c r="CZ14" s="66"/>
+      <c r="DA14" s="66"/>
+      <c r="DB14" s="66"/>
+      <c r="DC14" s="66"/>
+      <c r="DD14" s="66"/>
+      <c r="DE14" s="66"/>
+      <c r="DF14" s="66"/>
+      <c r="DG14" s="66"/>
+      <c r="DH14" s="66"/>
+      <c r="DI14" s="66"/>
+      <c r="DJ14" s="66"/>
+      <c r="DK14" s="66"/>
+      <c r="DL14" s="66"/>
+      <c r="DM14" s="66"/>
+      <c r="DN14" s="66"/>
+      <c r="DO14" s="66"/>
+      <c r="DP14" s="66"/>
+      <c r="DQ14" s="66"/>
+      <c r="DR14" s="66"/>
+      <c r="DS14" s="66"/>
+      <c r="DT14" s="66"/>
+      <c r="DU14" s="66"/>
+      <c r="DV14" s="66"/>
+      <c r="DW14" s="66"/>
+      <c r="DX14" s="66"/>
+      <c r="DY14" s="66"/>
+      <c r="DZ14" s="66"/>
+      <c r="EA14" s="66"/>
+      <c r="EB14" s="66"/>
+      <c r="EC14" s="66"/>
+      <c r="ED14" s="66"/>
+      <c r="EE14" s="66"/>
+      <c r="EF14" s="66"/>
+      <c r="EG14" s="66"/>
+      <c r="EH14" s="66"/>
+      <c r="EI14" s="66"/>
+      <c r="EJ14" s="66"/>
+      <c r="EK14" s="66"/>
+      <c r="EL14" s="66"/>
+      <c r="EM14" s="66"/>
+      <c r="EN14" s="66"/>
+      <c r="EO14" s="66"/>
+      <c r="EP14" s="66"/>
+      <c r="EQ14" s="66"/>
+      <c r="ER14" s="66"/>
+      <c r="ES14" s="66"/>
+      <c r="ET14" s="66"/>
+      <c r="EU14" s="66"/>
+      <c r="EV14" s="66"/>
+      <c r="EW14" s="66"/>
+      <c r="EX14" s="66"/>
+      <c r="EY14" s="66"/>
+      <c r="EZ14" s="66"/>
+      <c r="FA14" s="66"/>
+      <c r="FB14" s="66"/>
+      <c r="FC14" s="66"/>
+      <c r="FD14" s="66"/>
+      <c r="FE14" s="66"/>
+      <c r="FF14" s="66"/>
+      <c r="FG14" s="66"/>
+      <c r="FH14" s="66"/>
+      <c r="FI14" s="66"/>
+      <c r="FJ14" s="66"/>
+      <c r="FK14" s="66"/>
+      <c r="FL14" s="66"/>
+      <c r="FM14" s="66"/>
+      <c r="FN14" s="66"/>
+      <c r="FO14" s="66"/>
+      <c r="FP14" s="66"/>
+      <c r="FQ14" s="66"/>
+      <c r="FR14" s="66"/>
+      <c r="FS14" s="66"/>
+      <c r="FT14" s="66"/>
+      <c r="FU14" s="66"/>
+      <c r="FV14" s="66"/>
+      <c r="FW14" s="66"/>
+      <c r="FX14" s="66"/>
+      <c r="FY14" s="66"/>
+      <c r="FZ14" s="66"/>
+      <c r="GA14" s="66"/>
+      <c r="GB14" s="66"/>
+      <c r="GC14" s="66"/>
+      <c r="GD14" s="66"/>
+      <c r="GE14" s="66"/>
+      <c r="GF14" s="66"/>
+      <c r="GG14" s="66"/>
+      <c r="GH14" s="66"/>
+      <c r="GI14" s="66"/>
+      <c r="GJ14" s="66"/>
+      <c r="GK14" s="66"/>
+      <c r="GL14" s="66"/>
+      <c r="GM14" s="66"/>
+      <c r="GN14" s="66"/>
+      <c r="GO14" s="66"/>
+      <c r="GP14" s="66"/>
+      <c r="GQ14" s="66"/>
+      <c r="GR14" s="66"/>
+      <c r="GS14" s="66"/>
+      <c r="GT14" s="66"/>
+      <c r="GU14" s="66"/>
+      <c r="GV14" s="66"/>
+      <c r="GW14" s="66"/>
+      <c r="GX14" s="66"/>
+      <c r="GY14" s="66"/>
+      <c r="GZ14" s="66"/>
+      <c r="HA14" s="66"/>
+      <c r="HB14" s="66"/>
+      <c r="HC14" s="66"/>
+      <c r="HD14" s="66"/>
+      <c r="HE14" s="66"/>
+      <c r="HF14" s="66"/>
+      <c r="HG14" s="66"/>
+      <c r="HH14" s="66"/>
+      <c r="HI14" s="66"/>
+      <c r="HJ14" s="66"/>
+      <c r="HK14" s="66"/>
+      <c r="HL14" s="66"/>
+      <c r="HM14" s="66"/>
+      <c r="HN14" s="66"/>
+      <c r="HO14" s="66"/>
+      <c r="HP14" s="66"/>
+      <c r="HQ14" s="66"/>
+      <c r="HR14" s="66"/>
+      <c r="HS14" s="66"/>
+      <c r="HT14" s="66"/>
+      <c r="HU14" s="66"/>
+      <c r="HV14" s="66"/>
+      <c r="HW14" s="66"/>
+      <c r="HX14" s="66"/>
+      <c r="HY14" s="66"/>
+      <c r="HZ14" s="66"/>
+      <c r="IA14" s="66"/>
+      <c r="IB14" s="66"/>
+      <c r="IC14" s="66"/>
+      <c r="ID14" s="66"/>
+      <c r="IE14" s="66"/>
+      <c r="IF14" s="66"/>
+      <c r="IG14" s="66"/>
+      <c r="IH14" s="66"/>
+      <c r="II14" s="66"/>
+      <c r="IJ14" s="66"/>
+      <c r="IK14" s="66"/>
+      <c r="IL14" s="66"/>
+      <c r="IM14" s="66"/>
+      <c r="IN14" s="66"/>
+      <c r="IO14" s="66"/>
+      <c r="IP14" s="66"/>
+      <c r="IQ14" s="66"/>
+      <c r="IR14" s="66"/>
+      <c r="IS14" s="66"/>
+      <c r="IT14" s="66"/>
+      <c r="IU14" s="66"/>
+      <c r="IV14" s="66"/>
     </row>
     <row r="15" spans="1:256" ht="15" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="66"/>
+      <c r="N15" s="66"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="66"/>
+      <c r="Q15" s="66"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="66"/>
+      <c r="V15" s="66"/>
+      <c r="W15" s="66"/>
+      <c r="X15" s="66"/>
+      <c r="Y15" s="66"/>
+      <c r="Z15" s="66"/>
+      <c r="AA15" s="66"/>
+      <c r="AB15" s="66"/>
+      <c r="AC15" s="66"/>
+      <c r="AD15" s="66"/>
+      <c r="AE15" s="66"/>
+      <c r="AF15" s="66"/>
+      <c r="AG15" s="66"/>
+      <c r="AH15" s="66"/>
+      <c r="AI15" s="66"/>
+      <c r="AJ15" s="66"/>
+      <c r="AK15" s="66"/>
+      <c r="AL15" s="66"/>
+      <c r="AM15" s="66"/>
+      <c r="AN15" s="66"/>
+      <c r="AO15" s="66"/>
+      <c r="AP15" s="66"/>
+      <c r="AQ15" s="66"/>
+      <c r="AR15" s="66"/>
+      <c r="AS15" s="66"/>
+      <c r="AT15" s="66"/>
+      <c r="AU15" s="66"/>
+      <c r="AV15" s="66"/>
+      <c r="AW15" s="66"/>
+      <c r="AX15" s="66"/>
+      <c r="AY15" s="66"/>
+      <c r="AZ15" s="66"/>
+      <c r="BA15" s="66"/>
+      <c r="BB15" s="66"/>
+      <c r="BC15" s="66"/>
+      <c r="BD15" s="66"/>
+      <c r="BE15" s="66"/>
+      <c r="BF15" s="66"/>
+      <c r="BG15" s="66"/>
+      <c r="BH15" s="66"/>
+      <c r="BI15" s="66"/>
+      <c r="BJ15" s="66"/>
+      <c r="BK15" s="66"/>
+      <c r="BL15" s="66"/>
+      <c r="BM15" s="66"/>
+      <c r="BN15" s="66"/>
+      <c r="BO15" s="66"/>
+      <c r="BP15" s="66"/>
+      <c r="BQ15" s="66"/>
+      <c r="BR15" s="66"/>
+      <c r="BS15" s="66"/>
+      <c r="BT15" s="66"/>
+      <c r="BU15" s="66"/>
+      <c r="BV15" s="66"/>
+      <c r="BW15" s="66"/>
+      <c r="BX15" s="66"/>
+      <c r="BY15" s="66"/>
+      <c r="BZ15" s="66"/>
+      <c r="CA15" s="66"/>
+      <c r="CB15" s="66"/>
+      <c r="CC15" s="66"/>
+      <c r="CD15" s="66"/>
+      <c r="CE15" s="66"/>
+      <c r="CF15" s="66"/>
+      <c r="CG15" s="66"/>
+      <c r="CH15" s="66"/>
+      <c r="CI15" s="66"/>
+      <c r="CJ15" s="66"/>
+      <c r="CK15" s="66"/>
+      <c r="CL15" s="66"/>
+      <c r="CM15" s="66"/>
+      <c r="CN15" s="66"/>
+      <c r="CO15" s="66"/>
+      <c r="CP15" s="66"/>
+      <c r="CQ15" s="66"/>
+      <c r="CR15" s="66"/>
+      <c r="CS15" s="66"/>
+      <c r="CT15" s="66"/>
+      <c r="CU15" s="66"/>
+      <c r="CV15" s="66"/>
+      <c r="CW15" s="66"/>
+      <c r="CX15" s="66"/>
+      <c r="CY15" s="66"/>
+      <c r="CZ15" s="66"/>
+      <c r="DA15" s="66"/>
+      <c r="DB15" s="66"/>
+      <c r="DC15" s="66"/>
+      <c r="DD15" s="66"/>
+      <c r="DE15" s="66"/>
+      <c r="DF15" s="66"/>
+      <c r="DG15" s="66"/>
+      <c r="DH15" s="66"/>
+      <c r="DI15" s="66"/>
+      <c r="DJ15" s="66"/>
+      <c r="DK15" s="66"/>
+      <c r="DL15" s="66"/>
+      <c r="DM15" s="66"/>
+      <c r="DN15" s="66"/>
+      <c r="DO15" s="66"/>
+      <c r="DP15" s="66"/>
+      <c r="DQ15" s="66"/>
+      <c r="DR15" s="66"/>
+      <c r="DS15" s="66"/>
+      <c r="DT15" s="66"/>
+      <c r="DU15" s="66"/>
+      <c r="DV15" s="66"/>
+      <c r="DW15" s="66"/>
+      <c r="DX15" s="66"/>
+      <c r="DY15" s="66"/>
+      <c r="DZ15" s="66"/>
+      <c r="EA15" s="66"/>
+      <c r="EB15" s="66"/>
+      <c r="EC15" s="66"/>
+      <c r="ED15" s="66"/>
+      <c r="EE15" s="66"/>
+      <c r="EF15" s="66"/>
+      <c r="EG15" s="66"/>
+      <c r="EH15" s="66"/>
+      <c r="EI15" s="66"/>
+      <c r="EJ15" s="66"/>
+      <c r="EK15" s="66"/>
+      <c r="EL15" s="66"/>
+      <c r="EM15" s="66"/>
+      <c r="EN15" s="66"/>
+      <c r="EO15" s="66"/>
+      <c r="EP15" s="66"/>
+      <c r="EQ15" s="66"/>
+      <c r="ER15" s="66"/>
+      <c r="ES15" s="66"/>
+      <c r="ET15" s="66"/>
+      <c r="EU15" s="66"/>
+      <c r="EV15" s="66"/>
+      <c r="EW15" s="66"/>
+      <c r="EX15" s="66"/>
+      <c r="EY15" s="66"/>
+      <c r="EZ15" s="66"/>
+      <c r="FA15" s="66"/>
+      <c r="FB15" s="66"/>
+      <c r="FC15" s="66"/>
+      <c r="FD15" s="66"/>
+      <c r="FE15" s="66"/>
+      <c r="FF15" s="66"/>
+      <c r="FG15" s="66"/>
+      <c r="FH15" s="66"/>
+      <c r="FI15" s="66"/>
+      <c r="FJ15" s="66"/>
+      <c r="FK15" s="66"/>
+      <c r="FL15" s="66"/>
+      <c r="FM15" s="66"/>
+      <c r="FN15" s="66"/>
+      <c r="FO15" s="66"/>
+      <c r="FP15" s="66"/>
+      <c r="FQ15" s="66"/>
+      <c r="FR15" s="66"/>
+      <c r="FS15" s="66"/>
+      <c r="FT15" s="66"/>
+      <c r="FU15" s="66"/>
+      <c r="FV15" s="66"/>
+      <c r="FW15" s="66"/>
+      <c r="FX15" s="66"/>
+      <c r="FY15" s="66"/>
+      <c r="FZ15" s="66"/>
+      <c r="GA15" s="66"/>
+      <c r="GB15" s="66"/>
+      <c r="GC15" s="66"/>
+      <c r="GD15" s="66"/>
+      <c r="GE15" s="66"/>
+      <c r="GF15" s="66"/>
+      <c r="GG15" s="66"/>
+      <c r="GH15" s="66"/>
+      <c r="GI15" s="66"/>
+      <c r="GJ15" s="66"/>
+      <c r="GK15" s="66"/>
+      <c r="GL15" s="66"/>
+      <c r="GM15" s="66"/>
+      <c r="GN15" s="66"/>
+      <c r="GO15" s="66"/>
+      <c r="GP15" s="66"/>
+      <c r="GQ15" s="66"/>
+      <c r="GR15" s="66"/>
+      <c r="GS15" s="66"/>
+      <c r="GT15" s="66"/>
+      <c r="GU15" s="66"/>
+      <c r="GV15" s="66"/>
+      <c r="GW15" s="66"/>
+      <c r="GX15" s="66"/>
+      <c r="GY15" s="66"/>
+      <c r="GZ15" s="66"/>
+      <c r="HA15" s="66"/>
+      <c r="HB15" s="66"/>
+      <c r="HC15" s="66"/>
+      <c r="HD15" s="66"/>
+      <c r="HE15" s="66"/>
+      <c r="HF15" s="66"/>
+      <c r="HG15" s="66"/>
+      <c r="HH15" s="66"/>
+      <c r="HI15" s="66"/>
+      <c r="HJ15" s="66"/>
+      <c r="HK15" s="66"/>
+      <c r="HL15" s="66"/>
+      <c r="HM15" s="66"/>
+      <c r="HN15" s="66"/>
+      <c r="HO15" s="66"/>
+      <c r="HP15" s="66"/>
+      <c r="HQ15" s="66"/>
+      <c r="HR15" s="66"/>
+      <c r="HS15" s="66"/>
+      <c r="HT15" s="66"/>
+      <c r="HU15" s="66"/>
+      <c r="HV15" s="66"/>
+      <c r="HW15" s="66"/>
+      <c r="HX15" s="66"/>
+      <c r="HY15" s="66"/>
+      <c r="HZ15" s="66"/>
+      <c r="IA15" s="66"/>
+      <c r="IB15" s="66"/>
+      <c r="IC15" s="66"/>
+      <c r="ID15" s="66"/>
+      <c r="IE15" s="66"/>
+      <c r="IF15" s="66"/>
+      <c r="IG15" s="66"/>
+      <c r="IH15" s="66"/>
+      <c r="II15" s="66"/>
+      <c r="IJ15" s="66"/>
+      <c r="IK15" s="66"/>
+      <c r="IL15" s="66"/>
+      <c r="IM15" s="66"/>
+      <c r="IN15" s="66"/>
+      <c r="IO15" s="66"/>
+      <c r="IP15" s="66"/>
+      <c r="IQ15" s="66"/>
+      <c r="IR15" s="66"/>
+      <c r="IS15" s="66"/>
+      <c r="IT15" s="66"/>
+      <c r="IU15" s="66"/>
+      <c r="IV15" s="66"/>
     </row>
     <row r="16" spans="1:256" ht="15" customHeight="1">
       <c r="A16" s="76" t="s">
@@ -3292,11 +4061,11 @@
       <c r="IV16" s="66"/>
     </row>
     <row r="17" spans="1:256" ht="15" customHeight="1">
-      <c r="A17" s="76" t="s">
-        <v>95</v>
-      </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
+      <c r="A17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="66"/>
       <c r="E17" s="66"/>
       <c r="F17" s="66"/>
@@ -3552,532 +4321,536 @@
       <c r="IV17" s="66"/>
     </row>
     <row r="18" spans="1:256" ht="15" customHeight="1">
-      <c r="A18" s="8"/>
+      <c r="A18" s="76" t="s">
+        <v>96</v>
+      </c>
       <c r="B18" s="16"/>
       <c r="C18" s="17"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="66"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="66"/>
+      <c r="O18" s="66"/>
+      <c r="P18" s="66"/>
+      <c r="Q18" s="66"/>
+      <c r="R18" s="66"/>
+      <c r="S18" s="66"/>
+      <c r="T18" s="66"/>
+      <c r="U18" s="66"/>
+      <c r="V18" s="66"/>
+      <c r="W18" s="66"/>
+      <c r="X18" s="66"/>
+      <c r="Y18" s="66"/>
+      <c r="Z18" s="66"/>
+      <c r="AA18" s="66"/>
+      <c r="AB18" s="66"/>
+      <c r="AC18" s="66"/>
+      <c r="AD18" s="66"/>
+      <c r="AE18" s="66"/>
+      <c r="AF18" s="66"/>
+      <c r="AG18" s="66"/>
+      <c r="AH18" s="66"/>
+      <c r="AI18" s="66"/>
+      <c r="AJ18" s="66"/>
+      <c r="AK18" s="66"/>
+      <c r="AL18" s="66"/>
+      <c r="AM18" s="66"/>
+      <c r="AN18" s="66"/>
+      <c r="AO18" s="66"/>
+      <c r="AP18" s="66"/>
+      <c r="AQ18" s="66"/>
+      <c r="AR18" s="66"/>
+      <c r="AS18" s="66"/>
+      <c r="AT18" s="66"/>
+      <c r="AU18" s="66"/>
+      <c r="AV18" s="66"/>
+      <c r="AW18" s="66"/>
+      <c r="AX18" s="66"/>
+      <c r="AY18" s="66"/>
+      <c r="AZ18" s="66"/>
+      <c r="BA18" s="66"/>
+      <c r="BB18" s="66"/>
+      <c r="BC18" s="66"/>
+      <c r="BD18" s="66"/>
+      <c r="BE18" s="66"/>
+      <c r="BF18" s="66"/>
+      <c r="BG18" s="66"/>
+      <c r="BH18" s="66"/>
+      <c r="BI18" s="66"/>
+      <c r="BJ18" s="66"/>
+      <c r="BK18" s="66"/>
+      <c r="BL18" s="66"/>
+      <c r="BM18" s="66"/>
+      <c r="BN18" s="66"/>
+      <c r="BO18" s="66"/>
+      <c r="BP18" s="66"/>
+      <c r="BQ18" s="66"/>
+      <c r="BR18" s="66"/>
+      <c r="BS18" s="66"/>
+      <c r="BT18" s="66"/>
+      <c r="BU18" s="66"/>
+      <c r="BV18" s="66"/>
+      <c r="BW18" s="66"/>
+      <c r="BX18" s="66"/>
+      <c r="BY18" s="66"/>
+      <c r="BZ18" s="66"/>
+      <c r="CA18" s="66"/>
+      <c r="CB18" s="66"/>
+      <c r="CC18" s="66"/>
+      <c r="CD18" s="66"/>
+      <c r="CE18" s="66"/>
+      <c r="CF18" s="66"/>
+      <c r="CG18" s="66"/>
+      <c r="CH18" s="66"/>
+      <c r="CI18" s="66"/>
+      <c r="CJ18" s="66"/>
+      <c r="CK18" s="66"/>
+      <c r="CL18" s="66"/>
+      <c r="CM18" s="66"/>
+      <c r="CN18" s="66"/>
+      <c r="CO18" s="66"/>
+      <c r="CP18" s="66"/>
+      <c r="CQ18" s="66"/>
+      <c r="CR18" s="66"/>
+      <c r="CS18" s="66"/>
+      <c r="CT18" s="66"/>
+      <c r="CU18" s="66"/>
+      <c r="CV18" s="66"/>
+      <c r="CW18" s="66"/>
+      <c r="CX18" s="66"/>
+      <c r="CY18" s="66"/>
+      <c r="CZ18" s="66"/>
+      <c r="DA18" s="66"/>
+      <c r="DB18" s="66"/>
+      <c r="DC18" s="66"/>
+      <c r="DD18" s="66"/>
+      <c r="DE18" s="66"/>
+      <c r="DF18" s="66"/>
+      <c r="DG18" s="66"/>
+      <c r="DH18" s="66"/>
+      <c r="DI18" s="66"/>
+      <c r="DJ18" s="66"/>
+      <c r="DK18" s="66"/>
+      <c r="DL18" s="66"/>
+      <c r="DM18" s="66"/>
+      <c r="DN18" s="66"/>
+      <c r="DO18" s="66"/>
+      <c r="DP18" s="66"/>
+      <c r="DQ18" s="66"/>
+      <c r="DR18" s="66"/>
+      <c r="DS18" s="66"/>
+      <c r="DT18" s="66"/>
+      <c r="DU18" s="66"/>
+      <c r="DV18" s="66"/>
+      <c r="DW18" s="66"/>
+      <c r="DX18" s="66"/>
+      <c r="DY18" s="66"/>
+      <c r="DZ18" s="66"/>
+      <c r="EA18" s="66"/>
+      <c r="EB18" s="66"/>
+      <c r="EC18" s="66"/>
+      <c r="ED18" s="66"/>
+      <c r="EE18" s="66"/>
+      <c r="EF18" s="66"/>
+      <c r="EG18" s="66"/>
+      <c r="EH18" s="66"/>
+      <c r="EI18" s="66"/>
+      <c r="EJ18" s="66"/>
+      <c r="EK18" s="66"/>
+      <c r="EL18" s="66"/>
+      <c r="EM18" s="66"/>
+      <c r="EN18" s="66"/>
+      <c r="EO18" s="66"/>
+      <c r="EP18" s="66"/>
+      <c r="EQ18" s="66"/>
+      <c r="ER18" s="66"/>
+      <c r="ES18" s="66"/>
+      <c r="ET18" s="66"/>
+      <c r="EU18" s="66"/>
+      <c r="EV18" s="66"/>
+      <c r="EW18" s="66"/>
+      <c r="EX18" s="66"/>
+      <c r="EY18" s="66"/>
+      <c r="EZ18" s="66"/>
+      <c r="FA18" s="66"/>
+      <c r="FB18" s="66"/>
+      <c r="FC18" s="66"/>
+      <c r="FD18" s="66"/>
+      <c r="FE18" s="66"/>
+      <c r="FF18" s="66"/>
+      <c r="FG18" s="66"/>
+      <c r="FH18" s="66"/>
+      <c r="FI18" s="66"/>
+      <c r="FJ18" s="66"/>
+      <c r="FK18" s="66"/>
+      <c r="FL18" s="66"/>
+      <c r="FM18" s="66"/>
+      <c r="FN18" s="66"/>
+      <c r="FO18" s="66"/>
+      <c r="FP18" s="66"/>
+      <c r="FQ18" s="66"/>
+      <c r="FR18" s="66"/>
+      <c r="FS18" s="66"/>
+      <c r="FT18" s="66"/>
+      <c r="FU18" s="66"/>
+      <c r="FV18" s="66"/>
+      <c r="FW18" s="66"/>
+      <c r="FX18" s="66"/>
+      <c r="FY18" s="66"/>
+      <c r="FZ18" s="66"/>
+      <c r="GA18" s="66"/>
+      <c r="GB18" s="66"/>
+      <c r="GC18" s="66"/>
+      <c r="GD18" s="66"/>
+      <c r="GE18" s="66"/>
+      <c r="GF18" s="66"/>
+      <c r="GG18" s="66"/>
+      <c r="GH18" s="66"/>
+      <c r="GI18" s="66"/>
+      <c r="GJ18" s="66"/>
+      <c r="GK18" s="66"/>
+      <c r="GL18" s="66"/>
+      <c r="GM18" s="66"/>
+      <c r="GN18" s="66"/>
+      <c r="GO18" s="66"/>
+      <c r="GP18" s="66"/>
+      <c r="GQ18" s="66"/>
+      <c r="GR18" s="66"/>
+      <c r="GS18" s="66"/>
+      <c r="GT18" s="66"/>
+      <c r="GU18" s="66"/>
+      <c r="GV18" s="66"/>
+      <c r="GW18" s="66"/>
+      <c r="GX18" s="66"/>
+      <c r="GY18" s="66"/>
+      <c r="GZ18" s="66"/>
+      <c r="HA18" s="66"/>
+      <c r="HB18" s="66"/>
+      <c r="HC18" s="66"/>
+      <c r="HD18" s="66"/>
+      <c r="HE18" s="66"/>
+      <c r="HF18" s="66"/>
+      <c r="HG18" s="66"/>
+      <c r="HH18" s="66"/>
+      <c r="HI18" s="66"/>
+      <c r="HJ18" s="66"/>
+      <c r="HK18" s="66"/>
+      <c r="HL18" s="66"/>
+      <c r="HM18" s="66"/>
+      <c r="HN18" s="66"/>
+      <c r="HO18" s="66"/>
+      <c r="HP18" s="66"/>
+      <c r="HQ18" s="66"/>
+      <c r="HR18" s="66"/>
+      <c r="HS18" s="66"/>
+      <c r="HT18" s="66"/>
+      <c r="HU18" s="66"/>
+      <c r="HV18" s="66"/>
+      <c r="HW18" s="66"/>
+      <c r="HX18" s="66"/>
+      <c r="HY18" s="66"/>
+      <c r="HZ18" s="66"/>
+      <c r="IA18" s="66"/>
+      <c r="IB18" s="66"/>
+      <c r="IC18" s="66"/>
+      <c r="ID18" s="66"/>
+      <c r="IE18" s="66"/>
+      <c r="IF18" s="66"/>
+      <c r="IG18" s="66"/>
+      <c r="IH18" s="66"/>
+      <c r="II18" s="66"/>
+      <c r="IJ18" s="66"/>
+      <c r="IK18" s="66"/>
+      <c r="IL18" s="66"/>
+      <c r="IM18" s="66"/>
+      <c r="IN18" s="66"/>
+      <c r="IO18" s="66"/>
+      <c r="IP18" s="66"/>
+      <c r="IQ18" s="66"/>
+      <c r="IR18" s="66"/>
+      <c r="IS18" s="66"/>
+      <c r="IT18" s="66"/>
+      <c r="IU18" s="66"/>
+      <c r="IV18" s="66"/>
     </row>
     <row r="19" spans="1:256" ht="15" customHeight="1">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="66"/>
+      <c r="O19" s="66"/>
+      <c r="P19" s="66"/>
+      <c r="Q19" s="66"/>
+      <c r="R19" s="66"/>
+      <c r="S19" s="66"/>
+      <c r="T19" s="66"/>
+      <c r="U19" s="66"/>
+      <c r="V19" s="66"/>
+      <c r="W19" s="66"/>
+      <c r="X19" s="66"/>
+      <c r="Y19" s="66"/>
+      <c r="Z19" s="66"/>
+      <c r="AA19" s="66"/>
+      <c r="AB19" s="66"/>
+      <c r="AC19" s="66"/>
+      <c r="AD19" s="66"/>
+      <c r="AE19" s="66"/>
+      <c r="AF19" s="66"/>
+      <c r="AG19" s="66"/>
+      <c r="AH19" s="66"/>
+      <c r="AI19" s="66"/>
+      <c r="AJ19" s="66"/>
+      <c r="AK19" s="66"/>
+      <c r="AL19" s="66"/>
+      <c r="AM19" s="66"/>
+      <c r="AN19" s="66"/>
+      <c r="AO19" s="66"/>
+      <c r="AP19" s="66"/>
+      <c r="AQ19" s="66"/>
+      <c r="AR19" s="66"/>
+      <c r="AS19" s="66"/>
+      <c r="AT19" s="66"/>
+      <c r="AU19" s="66"/>
+      <c r="AV19" s="66"/>
+      <c r="AW19" s="66"/>
+      <c r="AX19" s="66"/>
+      <c r="AY19" s="66"/>
+      <c r="AZ19" s="66"/>
+      <c r="BA19" s="66"/>
+      <c r="BB19" s="66"/>
+      <c r="BC19" s="66"/>
+      <c r="BD19" s="66"/>
+      <c r="BE19" s="66"/>
+      <c r="BF19" s="66"/>
+      <c r="BG19" s="66"/>
+      <c r="BH19" s="66"/>
+      <c r="BI19" s="66"/>
+      <c r="BJ19" s="66"/>
+      <c r="BK19" s="66"/>
+      <c r="BL19" s="66"/>
+      <c r="BM19" s="66"/>
+      <c r="BN19" s="66"/>
+      <c r="BO19" s="66"/>
+      <c r="BP19" s="66"/>
+      <c r="BQ19" s="66"/>
+      <c r="BR19" s="66"/>
+      <c r="BS19" s="66"/>
+      <c r="BT19" s="66"/>
+      <c r="BU19" s="66"/>
+      <c r="BV19" s="66"/>
+      <c r="BW19" s="66"/>
+      <c r="BX19" s="66"/>
+      <c r="BY19" s="66"/>
+      <c r="BZ19" s="66"/>
+      <c r="CA19" s="66"/>
+      <c r="CB19" s="66"/>
+      <c r="CC19" s="66"/>
+      <c r="CD19" s="66"/>
+      <c r="CE19" s="66"/>
+      <c r="CF19" s="66"/>
+      <c r="CG19" s="66"/>
+      <c r="CH19" s="66"/>
+      <c r="CI19" s="66"/>
+      <c r="CJ19" s="66"/>
+      <c r="CK19" s="66"/>
+      <c r="CL19" s="66"/>
+      <c r="CM19" s="66"/>
+      <c r="CN19" s="66"/>
+      <c r="CO19" s="66"/>
+      <c r="CP19" s="66"/>
+      <c r="CQ19" s="66"/>
+      <c r="CR19" s="66"/>
+      <c r="CS19" s="66"/>
+      <c r="CT19" s="66"/>
+      <c r="CU19" s="66"/>
+      <c r="CV19" s="66"/>
+      <c r="CW19" s="66"/>
+      <c r="CX19" s="66"/>
+      <c r="CY19" s="66"/>
+      <c r="CZ19" s="66"/>
+      <c r="DA19" s="66"/>
+      <c r="DB19" s="66"/>
+      <c r="DC19" s="66"/>
+      <c r="DD19" s="66"/>
+      <c r="DE19" s="66"/>
+      <c r="DF19" s="66"/>
+      <c r="DG19" s="66"/>
+      <c r="DH19" s="66"/>
+      <c r="DI19" s="66"/>
+      <c r="DJ19" s="66"/>
+      <c r="DK19" s="66"/>
+      <c r="DL19" s="66"/>
+      <c r="DM19" s="66"/>
+      <c r="DN19" s="66"/>
+      <c r="DO19" s="66"/>
+      <c r="DP19" s="66"/>
+      <c r="DQ19" s="66"/>
+      <c r="DR19" s="66"/>
+      <c r="DS19" s="66"/>
+      <c r="DT19" s="66"/>
+      <c r="DU19" s="66"/>
+      <c r="DV19" s="66"/>
+      <c r="DW19" s="66"/>
+      <c r="DX19" s="66"/>
+      <c r="DY19" s="66"/>
+      <c r="DZ19" s="66"/>
+      <c r="EA19" s="66"/>
+      <c r="EB19" s="66"/>
+      <c r="EC19" s="66"/>
+      <c r="ED19" s="66"/>
+      <c r="EE19" s="66"/>
+      <c r="EF19" s="66"/>
+      <c r="EG19" s="66"/>
+      <c r="EH19" s="66"/>
+      <c r="EI19" s="66"/>
+      <c r="EJ19" s="66"/>
+      <c r="EK19" s="66"/>
+      <c r="EL19" s="66"/>
+      <c r="EM19" s="66"/>
+      <c r="EN19" s="66"/>
+      <c r="EO19" s="66"/>
+      <c r="EP19" s="66"/>
+      <c r="EQ19" s="66"/>
+      <c r="ER19" s="66"/>
+      <c r="ES19" s="66"/>
+      <c r="ET19" s="66"/>
+      <c r="EU19" s="66"/>
+      <c r="EV19" s="66"/>
+      <c r="EW19" s="66"/>
+      <c r="EX19" s="66"/>
+      <c r="EY19" s="66"/>
+      <c r="EZ19" s="66"/>
+      <c r="FA19" s="66"/>
+      <c r="FB19" s="66"/>
+      <c r="FC19" s="66"/>
+      <c r="FD19" s="66"/>
+      <c r="FE19" s="66"/>
+      <c r="FF19" s="66"/>
+      <c r="FG19" s="66"/>
+      <c r="FH19" s="66"/>
+      <c r="FI19" s="66"/>
+      <c r="FJ19" s="66"/>
+      <c r="FK19" s="66"/>
+      <c r="FL19" s="66"/>
+      <c r="FM19" s="66"/>
+      <c r="FN19" s="66"/>
+      <c r="FO19" s="66"/>
+      <c r="FP19" s="66"/>
+      <c r="FQ19" s="66"/>
+      <c r="FR19" s="66"/>
+      <c r="FS19" s="66"/>
+      <c r="FT19" s="66"/>
+      <c r="FU19" s="66"/>
+      <c r="FV19" s="66"/>
+      <c r="FW19" s="66"/>
+      <c r="FX19" s="66"/>
+      <c r="FY19" s="66"/>
+      <c r="FZ19" s="66"/>
+      <c r="GA19" s="66"/>
+      <c r="GB19" s="66"/>
+      <c r="GC19" s="66"/>
+      <c r="GD19" s="66"/>
+      <c r="GE19" s="66"/>
+      <c r="GF19" s="66"/>
+      <c r="GG19" s="66"/>
+      <c r="GH19" s="66"/>
+      <c r="GI19" s="66"/>
+      <c r="GJ19" s="66"/>
+      <c r="GK19" s="66"/>
+      <c r="GL19" s="66"/>
+      <c r="GM19" s="66"/>
+      <c r="GN19" s="66"/>
+      <c r="GO19" s="66"/>
+      <c r="GP19" s="66"/>
+      <c r="GQ19" s="66"/>
+      <c r="GR19" s="66"/>
+      <c r="GS19" s="66"/>
+      <c r="GT19" s="66"/>
+      <c r="GU19" s="66"/>
+      <c r="GV19" s="66"/>
+      <c r="GW19" s="66"/>
+      <c r="GX19" s="66"/>
+      <c r="GY19" s="66"/>
+      <c r="GZ19" s="66"/>
+      <c r="HA19" s="66"/>
+      <c r="HB19" s="66"/>
+      <c r="HC19" s="66"/>
+      <c r="HD19" s="66"/>
+      <c r="HE19" s="66"/>
+      <c r="HF19" s="66"/>
+      <c r="HG19" s="66"/>
+      <c r="HH19" s="66"/>
+      <c r="HI19" s="66"/>
+      <c r="HJ19" s="66"/>
+      <c r="HK19" s="66"/>
+      <c r="HL19" s="66"/>
+      <c r="HM19" s="66"/>
+      <c r="HN19" s="66"/>
+      <c r="HO19" s="66"/>
+      <c r="HP19" s="66"/>
+      <c r="HQ19" s="66"/>
+      <c r="HR19" s="66"/>
+      <c r="HS19" s="66"/>
+      <c r="HT19" s="66"/>
+      <c r="HU19" s="66"/>
+      <c r="HV19" s="66"/>
+      <c r="HW19" s="66"/>
+      <c r="HX19" s="66"/>
+      <c r="HY19" s="66"/>
+      <c r="HZ19" s="66"/>
+      <c r="IA19" s="66"/>
+      <c r="IB19" s="66"/>
+      <c r="IC19" s="66"/>
+      <c r="ID19" s="66"/>
+      <c r="IE19" s="66"/>
+      <c r="IF19" s="66"/>
+      <c r="IG19" s="66"/>
+      <c r="IH19" s="66"/>
+      <c r="II19" s="66"/>
+      <c r="IJ19" s="66"/>
+      <c r="IK19" s="66"/>
+      <c r="IL19" s="66"/>
+      <c r="IM19" s="66"/>
+      <c r="IN19" s="66"/>
+      <c r="IO19" s="66"/>
+      <c r="IP19" s="66"/>
+      <c r="IQ19" s="66"/>
+      <c r="IR19" s="66"/>
+      <c r="IS19" s="66"/>
+      <c r="IT19" s="66"/>
+      <c r="IU19" s="66"/>
+      <c r="IV19" s="66"/>
+    </row>
+    <row r="20" spans="1:256" ht="15" customHeight="1">
+      <c r="A20" s="8"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+    </row>
+    <row r="21" spans="1:256" ht="15" customHeight="1">
+      <c r="A21" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
-      <c r="O19"/>
-      <c r="P19"/>
-      <c r="Q19"/>
-      <c r="R19"/>
-      <c r="S19"/>
-      <c r="T19"/>
-      <c r="U19"/>
-      <c r="V19"/>
-      <c r="W19"/>
-      <c r="X19"/>
-      <c r="Y19"/>
-      <c r="Z19"/>
-      <c r="AA19"/>
-      <c r="AB19"/>
-      <c r="AC19"/>
-      <c r="AD19"/>
-      <c r="AE19"/>
-      <c r="AF19"/>
-      <c r="AG19"/>
-      <c r="AH19"/>
-      <c r="AI19"/>
-      <c r="AJ19"/>
-      <c r="AK19"/>
-      <c r="AL19"/>
-      <c r="AM19"/>
-      <c r="AN19"/>
-      <c r="AO19"/>
-      <c r="AP19"/>
-      <c r="AQ19"/>
-      <c r="AR19"/>
-      <c r="AS19"/>
-      <c r="AT19"/>
-      <c r="AU19"/>
-      <c r="AV19"/>
-      <c r="AW19"/>
-      <c r="AX19"/>
-      <c r="AY19"/>
-      <c r="AZ19"/>
-      <c r="BA19"/>
-      <c r="BB19"/>
-      <c r="BC19"/>
-      <c r="BD19"/>
-      <c r="BE19"/>
-      <c r="BF19"/>
-      <c r="BG19"/>
-      <c r="BH19"/>
-      <c r="BI19"/>
-      <c r="BJ19"/>
-      <c r="BK19"/>
-      <c r="BL19"/>
-      <c r="BM19"/>
-      <c r="BN19"/>
-      <c r="BO19"/>
-      <c r="BP19"/>
-      <c r="BQ19"/>
-      <c r="BR19"/>
-      <c r="BS19"/>
-      <c r="BT19"/>
-      <c r="BU19"/>
-      <c r="BV19"/>
-      <c r="BW19"/>
-      <c r="BX19"/>
-      <c r="BY19"/>
-      <c r="BZ19"/>
-      <c r="CA19"/>
-      <c r="CB19"/>
-      <c r="CC19"/>
-      <c r="CD19"/>
-      <c r="CE19"/>
-      <c r="CF19"/>
-      <c r="CG19"/>
-      <c r="CH19"/>
-      <c r="CI19"/>
-      <c r="CJ19"/>
-      <c r="CK19"/>
-      <c r="CL19"/>
-      <c r="CM19"/>
-      <c r="CN19"/>
-      <c r="CO19"/>
-      <c r="CP19"/>
-      <c r="CQ19"/>
-      <c r="CR19"/>
-      <c r="CS19"/>
-      <c r="CT19"/>
-      <c r="CU19"/>
-      <c r="CV19"/>
-      <c r="CW19"/>
-      <c r="CX19"/>
-      <c r="CY19"/>
-      <c r="CZ19"/>
-      <c r="DA19"/>
-      <c r="DB19"/>
-      <c r="DC19"/>
-      <c r="DD19"/>
-      <c r="DE19"/>
-      <c r="DF19"/>
-      <c r="DG19"/>
-      <c r="DH19"/>
-      <c r="DI19"/>
-      <c r="DJ19"/>
-      <c r="DK19"/>
-      <c r="DL19"/>
-      <c r="DM19"/>
-      <c r="DN19"/>
-      <c r="DO19"/>
-      <c r="DP19"/>
-      <c r="DQ19"/>
-      <c r="DR19"/>
-      <c r="DS19"/>
-      <c r="DT19"/>
-      <c r="DU19"/>
-      <c r="DV19"/>
-      <c r="DW19"/>
-      <c r="DX19"/>
-      <c r="DY19"/>
-      <c r="DZ19"/>
-      <c r="EA19"/>
-      <c r="EB19"/>
-      <c r="EC19"/>
-      <c r="ED19"/>
-      <c r="EE19"/>
-      <c r="EF19"/>
-      <c r="EG19"/>
-      <c r="EH19"/>
-      <c r="EI19"/>
-      <c r="EJ19"/>
-      <c r="EK19"/>
-      <c r="EL19"/>
-      <c r="EM19"/>
-      <c r="EN19"/>
-      <c r="EO19"/>
-      <c r="EP19"/>
-      <c r="EQ19"/>
-      <c r="ER19"/>
-      <c r="ES19"/>
-      <c r="ET19"/>
-      <c r="EU19"/>
-      <c r="EV19"/>
-      <c r="EW19"/>
-      <c r="EX19"/>
-      <c r="EY19"/>
-      <c r="EZ19"/>
-      <c r="FA19"/>
-      <c r="FB19"/>
-      <c r="FC19"/>
-      <c r="FD19"/>
-      <c r="FE19"/>
-      <c r="FF19"/>
-      <c r="FG19"/>
-      <c r="FH19"/>
-      <c r="FI19"/>
-      <c r="FJ19"/>
-      <c r="FK19"/>
-      <c r="FL19"/>
-      <c r="FM19"/>
-      <c r="FN19"/>
-      <c r="FO19"/>
-      <c r="FP19"/>
-      <c r="FQ19"/>
-      <c r="FR19"/>
-      <c r="FS19"/>
-      <c r="FT19"/>
-      <c r="FU19"/>
-      <c r="FV19"/>
-      <c r="FW19"/>
-      <c r="FX19"/>
-      <c r="FY19"/>
-      <c r="FZ19"/>
-      <c r="GA19"/>
-      <c r="GB19"/>
-      <c r="GC19"/>
-      <c r="GD19"/>
-      <c r="GE19"/>
-      <c r="GF19"/>
-      <c r="GG19"/>
-      <c r="GH19"/>
-      <c r="GI19"/>
-      <c r="GJ19"/>
-      <c r="GK19"/>
-      <c r="GL19"/>
-      <c r="GM19"/>
-      <c r="GN19"/>
-      <c r="GO19"/>
-      <c r="GP19"/>
-      <c r="GQ19"/>
-      <c r="GR19"/>
-      <c r="GS19"/>
-      <c r="GT19"/>
-      <c r="GU19"/>
-      <c r="GV19"/>
-      <c r="GW19"/>
-      <c r="GX19"/>
-      <c r="GY19"/>
-      <c r="GZ19"/>
-      <c r="HA19"/>
-      <c r="HB19"/>
-      <c r="HC19"/>
-      <c r="HD19"/>
-      <c r="HE19"/>
-      <c r="HF19"/>
-      <c r="HG19"/>
-      <c r="HH19"/>
-      <c r="HI19"/>
-      <c r="HJ19"/>
-      <c r="HK19"/>
-      <c r="HL19"/>
-      <c r="HM19"/>
-      <c r="HN19"/>
-      <c r="HO19"/>
-      <c r="HP19"/>
-      <c r="HQ19"/>
-      <c r="HR19"/>
-      <c r="HS19"/>
-      <c r="HT19"/>
-      <c r="HU19"/>
-      <c r="HV19"/>
-      <c r="HW19"/>
-      <c r="HX19"/>
-      <c r="HY19"/>
-      <c r="HZ19"/>
-      <c r="IA19"/>
-      <c r="IB19"/>
-      <c r="IC19"/>
-      <c r="ID19"/>
-      <c r="IE19"/>
-      <c r="IF19"/>
-      <c r="IG19"/>
-      <c r="IH19"/>
-      <c r="II19"/>
-      <c r="IJ19"/>
-      <c r="IK19"/>
-      <c r="IL19"/>
-      <c r="IM19"/>
-      <c r="IN19"/>
-      <c r="IO19"/>
-      <c r="IP19"/>
-      <c r="IQ19"/>
-      <c r="IR19"/>
-      <c r="IS19"/>
-      <c r="IT19"/>
-      <c r="IU19"/>
-      <c r="IV19"/>
-    </row>
-    <row r="20" spans="1:256" ht="15" customHeight="1">
-      <c r="A20" s="20"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20"/>
-      <c r="O20"/>
-      <c r="P20"/>
-      <c r="Q20"/>
-      <c r="R20"/>
-      <c r="S20"/>
-      <c r="T20"/>
-      <c r="U20"/>
-      <c r="V20"/>
-      <c r="W20"/>
-      <c r="X20"/>
-      <c r="Y20"/>
-      <c r="Z20"/>
-      <c r="AA20"/>
-      <c r="AB20"/>
-      <c r="AC20"/>
-      <c r="AD20"/>
-      <c r="AE20"/>
-      <c r="AF20"/>
-      <c r="AG20"/>
-      <c r="AH20"/>
-      <c r="AI20"/>
-      <c r="AJ20"/>
-      <c r="AK20"/>
-      <c r="AL20"/>
-      <c r="AM20"/>
-      <c r="AN20"/>
-      <c r="AO20"/>
-      <c r="AP20"/>
-      <c r="AQ20"/>
-      <c r="AR20"/>
-      <c r="AS20"/>
-      <c r="AT20"/>
-      <c r="AU20"/>
-      <c r="AV20"/>
-      <c r="AW20"/>
-      <c r="AX20"/>
-      <c r="AY20"/>
-      <c r="AZ20"/>
-      <c r="BA20"/>
-      <c r="BB20"/>
-      <c r="BC20"/>
-      <c r="BD20"/>
-      <c r="BE20"/>
-      <c r="BF20"/>
-      <c r="BG20"/>
-      <c r="BH20"/>
-      <c r="BI20"/>
-      <c r="BJ20"/>
-      <c r="BK20"/>
-      <c r="BL20"/>
-      <c r="BM20"/>
-      <c r="BN20"/>
-      <c r="BO20"/>
-      <c r="BP20"/>
-      <c r="BQ20"/>
-      <c r="BR20"/>
-      <c r="BS20"/>
-      <c r="BT20"/>
-      <c r="BU20"/>
-      <c r="BV20"/>
-      <c r="BW20"/>
-      <c r="BX20"/>
-      <c r="BY20"/>
-      <c r="BZ20"/>
-      <c r="CA20"/>
-      <c r="CB20"/>
-      <c r="CC20"/>
-      <c r="CD20"/>
-      <c r="CE20"/>
-      <c r="CF20"/>
-      <c r="CG20"/>
-      <c r="CH20"/>
-      <c r="CI20"/>
-      <c r="CJ20"/>
-      <c r="CK20"/>
-      <c r="CL20"/>
-      <c r="CM20"/>
-      <c r="CN20"/>
-      <c r="CO20"/>
-      <c r="CP20"/>
-      <c r="CQ20"/>
-      <c r="CR20"/>
-      <c r="CS20"/>
-      <c r="CT20"/>
-      <c r="CU20"/>
-      <c r="CV20"/>
-      <c r="CW20"/>
-      <c r="CX20"/>
-      <c r="CY20"/>
-      <c r="CZ20"/>
-      <c r="DA20"/>
-      <c r="DB20"/>
-      <c r="DC20"/>
-      <c r="DD20"/>
-      <c r="DE20"/>
-      <c r="DF20"/>
-      <c r="DG20"/>
-      <c r="DH20"/>
-      <c r="DI20"/>
-      <c r="DJ20"/>
-      <c r="DK20"/>
-      <c r="DL20"/>
-      <c r="DM20"/>
-      <c r="DN20"/>
-      <c r="DO20"/>
-      <c r="DP20"/>
-      <c r="DQ20"/>
-      <c r="DR20"/>
-      <c r="DS20"/>
-      <c r="DT20"/>
-      <c r="DU20"/>
-      <c r="DV20"/>
-      <c r="DW20"/>
-      <c r="DX20"/>
-      <c r="DY20"/>
-      <c r="DZ20"/>
-      <c r="EA20"/>
-      <c r="EB20"/>
-      <c r="EC20"/>
-      <c r="ED20"/>
-      <c r="EE20"/>
-      <c r="EF20"/>
-      <c r="EG20"/>
-      <c r="EH20"/>
-      <c r="EI20"/>
-      <c r="EJ20"/>
-      <c r="EK20"/>
-      <c r="EL20"/>
-      <c r="EM20"/>
-      <c r="EN20"/>
-      <c r="EO20"/>
-      <c r="EP20"/>
-      <c r="EQ20"/>
-      <c r="ER20"/>
-      <c r="ES20"/>
-      <c r="ET20"/>
-      <c r="EU20"/>
-      <c r="EV20"/>
-      <c r="EW20"/>
-      <c r="EX20"/>
-      <c r="EY20"/>
-      <c r="EZ20"/>
-      <c r="FA20"/>
-      <c r="FB20"/>
-      <c r="FC20"/>
-      <c r="FD20"/>
-      <c r="FE20"/>
-      <c r="FF20"/>
-      <c r="FG20"/>
-      <c r="FH20"/>
-      <c r="FI20"/>
-      <c r="FJ20"/>
-      <c r="FK20"/>
-      <c r="FL20"/>
-      <c r="FM20"/>
-      <c r="FN20"/>
-      <c r="FO20"/>
-      <c r="FP20"/>
-      <c r="FQ20"/>
-      <c r="FR20"/>
-      <c r="FS20"/>
-      <c r="FT20"/>
-      <c r="FU20"/>
-      <c r="FV20"/>
-      <c r="FW20"/>
-      <c r="FX20"/>
-      <c r="FY20"/>
-      <c r="FZ20"/>
-      <c r="GA20"/>
-      <c r="GB20"/>
-      <c r="GC20"/>
-      <c r="GD20"/>
-      <c r="GE20"/>
-      <c r="GF20"/>
-      <c r="GG20"/>
-      <c r="GH20"/>
-      <c r="GI20"/>
-      <c r="GJ20"/>
-      <c r="GK20"/>
-      <c r="GL20"/>
-      <c r="GM20"/>
-      <c r="GN20"/>
-      <c r="GO20"/>
-      <c r="GP20"/>
-      <c r="GQ20"/>
-      <c r="GR20"/>
-      <c r="GS20"/>
-      <c r="GT20"/>
-      <c r="GU20"/>
-      <c r="GV20"/>
-      <c r="GW20"/>
-      <c r="GX20"/>
-      <c r="GY20"/>
-      <c r="GZ20"/>
-      <c r="HA20"/>
-      <c r="HB20"/>
-      <c r="HC20"/>
-      <c r="HD20"/>
-      <c r="HE20"/>
-      <c r="HF20"/>
-      <c r="HG20"/>
-      <c r="HH20"/>
-      <c r="HI20"/>
-      <c r="HJ20"/>
-      <c r="HK20"/>
-      <c r="HL20"/>
-      <c r="HM20"/>
-      <c r="HN20"/>
-      <c r="HO20"/>
-      <c r="HP20"/>
-      <c r="HQ20"/>
-      <c r="HR20"/>
-      <c r="HS20"/>
-      <c r="HT20"/>
-      <c r="HU20"/>
-      <c r="HV20"/>
-      <c r="HW20"/>
-      <c r="HX20"/>
-      <c r="HY20"/>
-      <c r="HZ20"/>
-      <c r="IA20"/>
-      <c r="IB20"/>
-      <c r="IC20"/>
-      <c r="ID20"/>
-      <c r="IE20"/>
-      <c r="IF20"/>
-      <c r="IG20"/>
-      <c r="IH20"/>
-      <c r="II20"/>
-      <c r="IJ20"/>
-      <c r="IK20"/>
-      <c r="IL20"/>
-      <c r="IM20"/>
-      <c r="IN20"/>
-      <c r="IO20"/>
-      <c r="IP20"/>
-      <c r="IQ20"/>
-      <c r="IR20"/>
-      <c r="IS20"/>
-      <c r="IT20"/>
-      <c r="IU20"/>
-      <c r="IV20"/>
-    </row>
-    <row r="21" spans="1:256" ht="15" customHeight="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
@@ -4333,11 +5106,9 @@
       <c r="IV21"/>
     </row>
     <row r="22" spans="1:256" ht="15" customHeight="1">
-      <c r="A22" s="86" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="87"/>
-      <c r="C22" s="88"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22"/>
@@ -4593,11 +5364,9 @@
       <c r="IV22"/>
     </row>
     <row r="23" spans="1:256" ht="15" customHeight="1">
-      <c r="A23" s="79" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="80"/>
-      <c r="C23" s="81"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
@@ -4852,12 +5621,532 @@
       <c r="IU23"/>
       <c r="IV23"/>
     </row>
+    <row r="24" spans="1:256" ht="15" customHeight="1">
+      <c r="A24" s="86" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="87"/>
+      <c r="C24" s="88"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Y24"/>
+      <c r="Z24"/>
+      <c r="AA24"/>
+      <c r="AB24"/>
+      <c r="AC24"/>
+      <c r="AD24"/>
+      <c r="AE24"/>
+      <c r="AF24"/>
+      <c r="AG24"/>
+      <c r="AH24"/>
+      <c r="AI24"/>
+      <c r="AJ24"/>
+      <c r="AK24"/>
+      <c r="AL24"/>
+      <c r="AM24"/>
+      <c r="AN24"/>
+      <c r="AO24"/>
+      <c r="AP24"/>
+      <c r="AQ24"/>
+      <c r="AR24"/>
+      <c r="AS24"/>
+      <c r="AT24"/>
+      <c r="AU24"/>
+      <c r="AV24"/>
+      <c r="AW24"/>
+      <c r="AX24"/>
+      <c r="AY24"/>
+      <c r="AZ24"/>
+      <c r="BA24"/>
+      <c r="BB24"/>
+      <c r="BC24"/>
+      <c r="BD24"/>
+      <c r="BE24"/>
+      <c r="BF24"/>
+      <c r="BG24"/>
+      <c r="BH24"/>
+      <c r="BI24"/>
+      <c r="BJ24"/>
+      <c r="BK24"/>
+      <c r="BL24"/>
+      <c r="BM24"/>
+      <c r="BN24"/>
+      <c r="BO24"/>
+      <c r="BP24"/>
+      <c r="BQ24"/>
+      <c r="BR24"/>
+      <c r="BS24"/>
+      <c r="BT24"/>
+      <c r="BU24"/>
+      <c r="BV24"/>
+      <c r="BW24"/>
+      <c r="BX24"/>
+      <c r="BY24"/>
+      <c r="BZ24"/>
+      <c r="CA24"/>
+      <c r="CB24"/>
+      <c r="CC24"/>
+      <c r="CD24"/>
+      <c r="CE24"/>
+      <c r="CF24"/>
+      <c r="CG24"/>
+      <c r="CH24"/>
+      <c r="CI24"/>
+      <c r="CJ24"/>
+      <c r="CK24"/>
+      <c r="CL24"/>
+      <c r="CM24"/>
+      <c r="CN24"/>
+      <c r="CO24"/>
+      <c r="CP24"/>
+      <c r="CQ24"/>
+      <c r="CR24"/>
+      <c r="CS24"/>
+      <c r="CT24"/>
+      <c r="CU24"/>
+      <c r="CV24"/>
+      <c r="CW24"/>
+      <c r="CX24"/>
+      <c r="CY24"/>
+      <c r="CZ24"/>
+      <c r="DA24"/>
+      <c r="DB24"/>
+      <c r="DC24"/>
+      <c r="DD24"/>
+      <c r="DE24"/>
+      <c r="DF24"/>
+      <c r="DG24"/>
+      <c r="DH24"/>
+      <c r="DI24"/>
+      <c r="DJ24"/>
+      <c r="DK24"/>
+      <c r="DL24"/>
+      <c r="DM24"/>
+      <c r="DN24"/>
+      <c r="DO24"/>
+      <c r="DP24"/>
+      <c r="DQ24"/>
+      <c r="DR24"/>
+      <c r="DS24"/>
+      <c r="DT24"/>
+      <c r="DU24"/>
+      <c r="DV24"/>
+      <c r="DW24"/>
+      <c r="DX24"/>
+      <c r="DY24"/>
+      <c r="DZ24"/>
+      <c r="EA24"/>
+      <c r="EB24"/>
+      <c r="EC24"/>
+      <c r="ED24"/>
+      <c r="EE24"/>
+      <c r="EF24"/>
+      <c r="EG24"/>
+      <c r="EH24"/>
+      <c r="EI24"/>
+      <c r="EJ24"/>
+      <c r="EK24"/>
+      <c r="EL24"/>
+      <c r="EM24"/>
+      <c r="EN24"/>
+      <c r="EO24"/>
+      <c r="EP24"/>
+      <c r="EQ24"/>
+      <c r="ER24"/>
+      <c r="ES24"/>
+      <c r="ET24"/>
+      <c r="EU24"/>
+      <c r="EV24"/>
+      <c r="EW24"/>
+      <c r="EX24"/>
+      <c r="EY24"/>
+      <c r="EZ24"/>
+      <c r="FA24"/>
+      <c r="FB24"/>
+      <c r="FC24"/>
+      <c r="FD24"/>
+      <c r="FE24"/>
+      <c r="FF24"/>
+      <c r="FG24"/>
+      <c r="FH24"/>
+      <c r="FI24"/>
+      <c r="FJ24"/>
+      <c r="FK24"/>
+      <c r="FL24"/>
+      <c r="FM24"/>
+      <c r="FN24"/>
+      <c r="FO24"/>
+      <c r="FP24"/>
+      <c r="FQ24"/>
+      <c r="FR24"/>
+      <c r="FS24"/>
+      <c r="FT24"/>
+      <c r="FU24"/>
+      <c r="FV24"/>
+      <c r="FW24"/>
+      <c r="FX24"/>
+      <c r="FY24"/>
+      <c r="FZ24"/>
+      <c r="GA24"/>
+      <c r="GB24"/>
+      <c r="GC24"/>
+      <c r="GD24"/>
+      <c r="GE24"/>
+      <c r="GF24"/>
+      <c r="GG24"/>
+      <c r="GH24"/>
+      <c r="GI24"/>
+      <c r="GJ24"/>
+      <c r="GK24"/>
+      <c r="GL24"/>
+      <c r="GM24"/>
+      <c r="GN24"/>
+      <c r="GO24"/>
+      <c r="GP24"/>
+      <c r="GQ24"/>
+      <c r="GR24"/>
+      <c r="GS24"/>
+      <c r="GT24"/>
+      <c r="GU24"/>
+      <c r="GV24"/>
+      <c r="GW24"/>
+      <c r="GX24"/>
+      <c r="GY24"/>
+      <c r="GZ24"/>
+      <c r="HA24"/>
+      <c r="HB24"/>
+      <c r="HC24"/>
+      <c r="HD24"/>
+      <c r="HE24"/>
+      <c r="HF24"/>
+      <c r="HG24"/>
+      <c r="HH24"/>
+      <c r="HI24"/>
+      <c r="HJ24"/>
+      <c r="HK24"/>
+      <c r="HL24"/>
+      <c r="HM24"/>
+      <c r="HN24"/>
+      <c r="HO24"/>
+      <c r="HP24"/>
+      <c r="HQ24"/>
+      <c r="HR24"/>
+      <c r="HS24"/>
+      <c r="HT24"/>
+      <c r="HU24"/>
+      <c r="HV24"/>
+      <c r="HW24"/>
+      <c r="HX24"/>
+      <c r="HY24"/>
+      <c r="HZ24"/>
+      <c r="IA24"/>
+      <c r="IB24"/>
+      <c r="IC24"/>
+      <c r="ID24"/>
+      <c r="IE24"/>
+      <c r="IF24"/>
+      <c r="IG24"/>
+      <c r="IH24"/>
+      <c r="II24"/>
+      <c r="IJ24"/>
+      <c r="IK24"/>
+      <c r="IL24"/>
+      <c r="IM24"/>
+      <c r="IN24"/>
+      <c r="IO24"/>
+      <c r="IP24"/>
+      <c r="IQ24"/>
+      <c r="IR24"/>
+      <c r="IS24"/>
+      <c r="IT24"/>
+      <c r="IU24"/>
+      <c r="IV24"/>
+    </row>
+    <row r="25" spans="1:256" ht="15" customHeight="1">
+      <c r="A25" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="80"/>
+      <c r="C25" s="81"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25"/>
+      <c r="Z25"/>
+      <c r="AA25"/>
+      <c r="AB25"/>
+      <c r="AC25"/>
+      <c r="AD25"/>
+      <c r="AE25"/>
+      <c r="AF25"/>
+      <c r="AG25"/>
+      <c r="AH25"/>
+      <c r="AI25"/>
+      <c r="AJ25"/>
+      <c r="AK25"/>
+      <c r="AL25"/>
+      <c r="AM25"/>
+      <c r="AN25"/>
+      <c r="AO25"/>
+      <c r="AP25"/>
+      <c r="AQ25"/>
+      <c r="AR25"/>
+      <c r="AS25"/>
+      <c r="AT25"/>
+      <c r="AU25"/>
+      <c r="AV25"/>
+      <c r="AW25"/>
+      <c r="AX25"/>
+      <c r="AY25"/>
+      <c r="AZ25"/>
+      <c r="BA25"/>
+      <c r="BB25"/>
+      <c r="BC25"/>
+      <c r="BD25"/>
+      <c r="BE25"/>
+      <c r="BF25"/>
+      <c r="BG25"/>
+      <c r="BH25"/>
+      <c r="BI25"/>
+      <c r="BJ25"/>
+      <c r="BK25"/>
+      <c r="BL25"/>
+      <c r="BM25"/>
+      <c r="BN25"/>
+      <c r="BO25"/>
+      <c r="BP25"/>
+      <c r="BQ25"/>
+      <c r="BR25"/>
+      <c r="BS25"/>
+      <c r="BT25"/>
+      <c r="BU25"/>
+      <c r="BV25"/>
+      <c r="BW25"/>
+      <c r="BX25"/>
+      <c r="BY25"/>
+      <c r="BZ25"/>
+      <c r="CA25"/>
+      <c r="CB25"/>
+      <c r="CC25"/>
+      <c r="CD25"/>
+      <c r="CE25"/>
+      <c r="CF25"/>
+      <c r="CG25"/>
+      <c r="CH25"/>
+      <c r="CI25"/>
+      <c r="CJ25"/>
+      <c r="CK25"/>
+      <c r="CL25"/>
+      <c r="CM25"/>
+      <c r="CN25"/>
+      <c r="CO25"/>
+      <c r="CP25"/>
+      <c r="CQ25"/>
+      <c r="CR25"/>
+      <c r="CS25"/>
+      <c r="CT25"/>
+      <c r="CU25"/>
+      <c r="CV25"/>
+      <c r="CW25"/>
+      <c r="CX25"/>
+      <c r="CY25"/>
+      <c r="CZ25"/>
+      <c r="DA25"/>
+      <c r="DB25"/>
+      <c r="DC25"/>
+      <c r="DD25"/>
+      <c r="DE25"/>
+      <c r="DF25"/>
+      <c r="DG25"/>
+      <c r="DH25"/>
+      <c r="DI25"/>
+      <c r="DJ25"/>
+      <c r="DK25"/>
+      <c r="DL25"/>
+      <c r="DM25"/>
+      <c r="DN25"/>
+      <c r="DO25"/>
+      <c r="DP25"/>
+      <c r="DQ25"/>
+      <c r="DR25"/>
+      <c r="DS25"/>
+      <c r="DT25"/>
+      <c r="DU25"/>
+      <c r="DV25"/>
+      <c r="DW25"/>
+      <c r="DX25"/>
+      <c r="DY25"/>
+      <c r="DZ25"/>
+      <c r="EA25"/>
+      <c r="EB25"/>
+      <c r="EC25"/>
+      <c r="ED25"/>
+      <c r="EE25"/>
+      <c r="EF25"/>
+      <c r="EG25"/>
+      <c r="EH25"/>
+      <c r="EI25"/>
+      <c r="EJ25"/>
+      <c r="EK25"/>
+      <c r="EL25"/>
+      <c r="EM25"/>
+      <c r="EN25"/>
+      <c r="EO25"/>
+      <c r="EP25"/>
+      <c r="EQ25"/>
+      <c r="ER25"/>
+      <c r="ES25"/>
+      <c r="ET25"/>
+      <c r="EU25"/>
+      <c r="EV25"/>
+      <c r="EW25"/>
+      <c r="EX25"/>
+      <c r="EY25"/>
+      <c r="EZ25"/>
+      <c r="FA25"/>
+      <c r="FB25"/>
+      <c r="FC25"/>
+      <c r="FD25"/>
+      <c r="FE25"/>
+      <c r="FF25"/>
+      <c r="FG25"/>
+      <c r="FH25"/>
+      <c r="FI25"/>
+      <c r="FJ25"/>
+      <c r="FK25"/>
+      <c r="FL25"/>
+      <c r="FM25"/>
+      <c r="FN25"/>
+      <c r="FO25"/>
+      <c r="FP25"/>
+      <c r="FQ25"/>
+      <c r="FR25"/>
+      <c r="FS25"/>
+      <c r="FT25"/>
+      <c r="FU25"/>
+      <c r="FV25"/>
+      <c r="FW25"/>
+      <c r="FX25"/>
+      <c r="FY25"/>
+      <c r="FZ25"/>
+      <c r="GA25"/>
+      <c r="GB25"/>
+      <c r="GC25"/>
+      <c r="GD25"/>
+      <c r="GE25"/>
+      <c r="GF25"/>
+      <c r="GG25"/>
+      <c r="GH25"/>
+      <c r="GI25"/>
+      <c r="GJ25"/>
+      <c r="GK25"/>
+      <c r="GL25"/>
+      <c r="GM25"/>
+      <c r="GN25"/>
+      <c r="GO25"/>
+      <c r="GP25"/>
+      <c r="GQ25"/>
+      <c r="GR25"/>
+      <c r="GS25"/>
+      <c r="GT25"/>
+      <c r="GU25"/>
+      <c r="GV25"/>
+      <c r="GW25"/>
+      <c r="GX25"/>
+      <c r="GY25"/>
+      <c r="GZ25"/>
+      <c r="HA25"/>
+      <c r="HB25"/>
+      <c r="HC25"/>
+      <c r="HD25"/>
+      <c r="HE25"/>
+      <c r="HF25"/>
+      <c r="HG25"/>
+      <c r="HH25"/>
+      <c r="HI25"/>
+      <c r="HJ25"/>
+      <c r="HK25"/>
+      <c r="HL25"/>
+      <c r="HM25"/>
+      <c r="HN25"/>
+      <c r="HO25"/>
+      <c r="HP25"/>
+      <c r="HQ25"/>
+      <c r="HR25"/>
+      <c r="HS25"/>
+      <c r="HT25"/>
+      <c r="HU25"/>
+      <c r="HV25"/>
+      <c r="HW25"/>
+      <c r="HX25"/>
+      <c r="HY25"/>
+      <c r="HZ25"/>
+      <c r="IA25"/>
+      <c r="IB25"/>
+      <c r="IC25"/>
+      <c r="ID25"/>
+      <c r="IE25"/>
+      <c r="IF25"/>
+      <c r="IG25"/>
+      <c r="IH25"/>
+      <c r="II25"/>
+      <c r="IJ25"/>
+      <c r="IK25"/>
+      <c r="IL25"/>
+      <c r="IM25"/>
+      <c r="IN25"/>
+      <c r="IO25"/>
+      <c r="IP25"/>
+      <c r="IQ25"/>
+      <c r="IR25"/>
+      <c r="IS25"/>
+      <c r="IT25"/>
+      <c r="IU25"/>
+      <c r="IV25"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A12:C12"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A24:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4885,7 +6174,7 @@
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
       <c r="A1" s="84" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="85"/>
       <c r="C1" s="85"/>
@@ -4895,72 +6184,72 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:256" ht="15" customHeight="1">
       <c r="A3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="25" t="s">
         <v>39</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>40</v>
       </c>
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:256" ht="15" customHeight="1">
       <c r="A4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>41</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>42</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:256" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:256" ht="15" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:256" ht="15" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:256" ht="15" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:256" ht="15" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" s="72" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="66"/>
@@ -5266,21 +6555,21 @@
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="33">
         <v>42715</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="36">
         <v>42714</v>
       </c>
       <c r="F2" s="37"/>
       <c r="G2" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H2" s="38">
         <v>42714</v>
@@ -5288,21 +6577,21 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="9">
         <v>42715</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="33">
         <v>42349</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3" s="41">
         <v>42715</v>
@@ -5310,21 +6599,21 @@
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="36">
         <v>42714</v>
       </c>
       <c r="C4" s="43"/>
       <c r="D4" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="6">
         <v>42349</v>
       </c>
       <c r="F4" s="34"/>
       <c r="G4" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H4" s="38">
         <v>42714</v>
@@ -5332,7 +6621,7 @@
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="33">
         <v>42715</v>
@@ -5342,7 +6631,7 @@
       <c r="E5" s="14"/>
       <c r="F5" s="34"/>
       <c r="G5" s="35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H5" s="38">
         <v>42714</v>
@@ -5350,7 +6639,7 @@
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="9">
         <v>42715</v>
@@ -5364,33 +6653,33 @@
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="46"/>
       <c r="C7" s="37"/>
       <c r="D7" s="47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="46"/>
       <c r="F7" s="37"/>
       <c r="G7" s="47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H7" s="48"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="14"/>
       <c r="D8" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="14"/>
       <c r="G8" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H8" s="33">
         <v>42715</v>
@@ -5398,7 +6687,7 @@
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -5408,7 +6697,7 @@
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H9" s="14"/>
     </row>
@@ -5440,17 +6729,17 @@
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="14"/>
       <c r="D12" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="52"/>
       <c r="F12" s="14"/>
       <c r="G12" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H12" s="52"/>
     </row>
@@ -5459,12 +6748,12 @@
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" s="53"/>
       <c r="F13" s="14"/>
       <c r="G13" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H13" s="14"/>
     </row>
@@ -5558,7 +6847,7 @@
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="57"/>
       <c r="C2" s="57"/>
@@ -5567,10 +6856,10 @@
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="56" t="s">
         <v>69</v>
-      </c>
-      <c r="B3" s="56" t="s">
-        <v>70</v>
       </c>
       <c r="C3" s="57"/>
       <c r="D3" s="57"/>
@@ -5578,10 +6867,10 @@
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="56" t="s">
         <v>71</v>
-      </c>
-      <c r="B4" s="56" t="s">
-        <v>72</v>
       </c>
       <c r="C4" s="57"/>
       <c r="D4" s="57"/>
@@ -5597,28 +6886,28 @@
     <row r="6" spans="1:5" ht="15" customHeight="1">
       <c r="A6" s="57"/>
       <c r="B6" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="56" t="s">
         <v>73</v>
-      </c>
-      <c r="C6" s="56" t="s">
-        <v>74</v>
       </c>
       <c r="D6" s="57"/>
       <c r="E6" s="57"/>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1">
       <c r="A7" s="56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="57"/>
       <c r="C7" s="57"/>
       <c r="D7" s="57"/>
       <c r="E7" s="56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" s="58">
         <v>3</v>
@@ -5629,7 +6918,7 @@
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1">
       <c r="A9" s="59" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" s="60">
         <v>10</v>
@@ -5656,10 +6945,10 @@
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1">
       <c r="A12" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="64" t="s">
         <v>79</v>
-      </c>
-      <c r="B12" s="64" t="s">
-        <v>80</v>
       </c>
       <c r="C12" s="65"/>
       <c r="D12" s="57"/>
@@ -5667,7 +6956,7 @@
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1">
       <c r="A13" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" s="57"/>
       <c r="C13" s="57"/>
@@ -5698,7 +6987,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
       <c r="A1" s="56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -5714,7 +7003,7 @@
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="57"/>
       <c r="C3" s="57"/>
@@ -5723,7 +7012,7 @@
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="67" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="57"/>
       <c r="C4" s="57"/>
@@ -5732,7 +7021,7 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1">
       <c r="A5" s="68" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="57"/>
       <c r="C5" s="57"/>
@@ -5741,7 +7030,7 @@
     </row>
     <row r="6" spans="1:5" ht="45" customHeight="1">
       <c r="A6" s="69" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="57"/>
       <c r="C6" s="57"/>
@@ -5757,7 +7046,7 @@
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="67" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="57"/>
       <c r="C8" s="57"/>
@@ -5766,7 +7055,7 @@
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1">
       <c r="A9" s="68" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" s="57"/>
       <c r="C9" s="57"/>
@@ -5775,7 +7064,7 @@
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1">
       <c r="A10" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="57"/>
       <c r="C10" s="57"/>

</xml_diff>

<commit_message>
Revert "Actualización de actividades"
This reverts commit ec5839a445998b351dc3a1fce90346fac167bfeb.
</commit_message>
<xml_diff>
--- a/Scrum.xlsx
+++ b/Scrum.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="107">
   <si>
     <t>TOÑO</t>
   </si>
@@ -307,6 +307,9 @@
     <t>BUG - Cotización, revisar cuando se agrega un nuevo producto</t>
   </si>
   <si>
+    <t>Cotización - Enviar como PDF y Excel</t>
+  </si>
+  <si>
     <t>Cotización - Agregar CP de cliente?</t>
   </si>
   <si>
@@ -319,6 +322,9 @@
     <t>Envío mail - Que la alerta de enviando dure hasta que se haya mandado el mail</t>
   </si>
   <si>
+    <t>Otross - Módulo para asignar clientes por ejecutivo</t>
+  </si>
+  <si>
     <t>Cotización - Que el número interior no sea obligatorio y que sea carácter (tmb ext)</t>
   </si>
   <si>
@@ -335,24 +341,6 @@
   </si>
   <si>
     <t>Calendario - Mejorar estilos al ver detalle</t>
-  </si>
-  <si>
-    <t>Otros - Módulo para asignar clientes por ejecutivo</t>
-  </si>
-  <si>
-    <t>Servidor - Conexión entre base de datos y tomcat</t>
-  </si>
-  <si>
-    <t>19/02/2017</t>
-  </si>
-  <si>
-    <t>Indicador de llamadas - Activar modal para speech, manejo de obj, guía y líneas de negocio</t>
-  </si>
-  <si>
-    <t>PENDIENTE</t>
-  </si>
-  <si>
-    <t>Cotización - Enviar como PDF y Excel ??</t>
   </si>
 </sst>
 </file>
@@ -736,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -825,18 +813,16 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -861,14 +847,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2082,25 +2060,25 @@
   <dimension ref="A1:IV20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="59.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" customWidth="1"/>
     <col min="4" max="256" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="15" customHeight="1">
+    <row r="1" spans="1:3" ht="15" customHeight="1">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="90"/>
       <c r="C1" s="90"/>
     </row>
-    <row r="2" spans="1:256" ht="15" customHeight="1">
+    <row r="2" spans="1:3" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2111,357 +2089,96 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:256" ht="15" customHeight="1">
-      <c r="A3" s="96" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="97" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
-      <c r="S3" s="66"/>
-      <c r="T3" s="66"/>
-      <c r="U3" s="66"/>
-      <c r="V3" s="66"/>
-      <c r="W3" s="66"/>
-      <c r="X3" s="66"/>
-      <c r="Y3" s="66"/>
-      <c r="Z3" s="66"/>
-      <c r="AA3" s="66"/>
-      <c r="AB3" s="66"/>
-      <c r="AC3" s="66"/>
-      <c r="AD3" s="66"/>
-      <c r="AE3" s="66"/>
-      <c r="AF3" s="66"/>
-      <c r="AG3" s="66"/>
-      <c r="AH3" s="66"/>
-      <c r="AI3" s="66"/>
-      <c r="AJ3" s="66"/>
-      <c r="AK3" s="66"/>
-      <c r="AL3" s="66"/>
-      <c r="AM3" s="66"/>
-      <c r="AN3" s="66"/>
-      <c r="AO3" s="66"/>
-      <c r="AP3" s="66"/>
-      <c r="AQ3" s="66"/>
-      <c r="AR3" s="66"/>
-      <c r="AS3" s="66"/>
-      <c r="AT3" s="66"/>
-      <c r="AU3" s="66"/>
-      <c r="AV3" s="66"/>
-      <c r="AW3" s="66"/>
-      <c r="AX3" s="66"/>
-      <c r="AY3" s="66"/>
-      <c r="AZ3" s="66"/>
-      <c r="BA3" s="66"/>
-      <c r="BB3" s="66"/>
-      <c r="BC3" s="66"/>
-      <c r="BD3" s="66"/>
-      <c r="BE3" s="66"/>
-      <c r="BF3" s="66"/>
-      <c r="BG3" s="66"/>
-      <c r="BH3" s="66"/>
-      <c r="BI3" s="66"/>
-      <c r="BJ3" s="66"/>
-      <c r="BK3" s="66"/>
-      <c r="BL3" s="66"/>
-      <c r="BM3" s="66"/>
-      <c r="BN3" s="66"/>
-      <c r="BO3" s="66"/>
-      <c r="BP3" s="66"/>
-      <c r="BQ3" s="66"/>
-      <c r="BR3" s="66"/>
-      <c r="BS3" s="66"/>
-      <c r="BT3" s="66"/>
-      <c r="BU3" s="66"/>
-      <c r="BV3" s="66"/>
-      <c r="BW3" s="66"/>
-      <c r="BX3" s="66"/>
-      <c r="BY3" s="66"/>
-      <c r="BZ3" s="66"/>
-      <c r="CA3" s="66"/>
-      <c r="CB3" s="66"/>
-      <c r="CC3" s="66"/>
-      <c r="CD3" s="66"/>
-      <c r="CE3" s="66"/>
-      <c r="CF3" s="66"/>
-      <c r="CG3" s="66"/>
-      <c r="CH3" s="66"/>
-      <c r="CI3" s="66"/>
-      <c r="CJ3" s="66"/>
-      <c r="CK3" s="66"/>
-      <c r="CL3" s="66"/>
-      <c r="CM3" s="66"/>
-      <c r="CN3" s="66"/>
-      <c r="CO3" s="66"/>
-      <c r="CP3" s="66"/>
-      <c r="CQ3" s="66"/>
-      <c r="CR3" s="66"/>
-      <c r="CS3" s="66"/>
-      <c r="CT3" s="66"/>
-      <c r="CU3" s="66"/>
-      <c r="CV3" s="66"/>
-      <c r="CW3" s="66"/>
-      <c r="CX3" s="66"/>
-      <c r="CY3" s="66"/>
-      <c r="CZ3" s="66"/>
-      <c r="DA3" s="66"/>
-      <c r="DB3" s="66"/>
-      <c r="DC3" s="66"/>
-      <c r="DD3" s="66"/>
-      <c r="DE3" s="66"/>
-      <c r="DF3" s="66"/>
-      <c r="DG3" s="66"/>
-      <c r="DH3" s="66"/>
-      <c r="DI3" s="66"/>
-      <c r="DJ3" s="66"/>
-      <c r="DK3" s="66"/>
-      <c r="DL3" s="66"/>
-      <c r="DM3" s="66"/>
-      <c r="DN3" s="66"/>
-      <c r="DO3" s="66"/>
-      <c r="DP3" s="66"/>
-      <c r="DQ3" s="66"/>
-      <c r="DR3" s="66"/>
-      <c r="DS3" s="66"/>
-      <c r="DT3" s="66"/>
-      <c r="DU3" s="66"/>
-      <c r="DV3" s="66"/>
-      <c r="DW3" s="66"/>
-      <c r="DX3" s="66"/>
-      <c r="DY3" s="66"/>
-      <c r="DZ3" s="66"/>
-      <c r="EA3" s="66"/>
-      <c r="EB3" s="66"/>
-      <c r="EC3" s="66"/>
-      <c r="ED3" s="66"/>
-      <c r="EE3" s="66"/>
-      <c r="EF3" s="66"/>
-      <c r="EG3" s="66"/>
-      <c r="EH3" s="66"/>
-      <c r="EI3" s="66"/>
-      <c r="EJ3" s="66"/>
-      <c r="EK3" s="66"/>
-      <c r="EL3" s="66"/>
-      <c r="EM3" s="66"/>
-      <c r="EN3" s="66"/>
-      <c r="EO3" s="66"/>
-      <c r="EP3" s="66"/>
-      <c r="EQ3" s="66"/>
-      <c r="ER3" s="66"/>
-      <c r="ES3" s="66"/>
-      <c r="ET3" s="66"/>
-      <c r="EU3" s="66"/>
-      <c r="EV3" s="66"/>
-      <c r="EW3" s="66"/>
-      <c r="EX3" s="66"/>
-      <c r="EY3" s="66"/>
-      <c r="EZ3" s="66"/>
-      <c r="FA3" s="66"/>
-      <c r="FB3" s="66"/>
-      <c r="FC3" s="66"/>
-      <c r="FD3" s="66"/>
-      <c r="FE3" s="66"/>
-      <c r="FF3" s="66"/>
-      <c r="FG3" s="66"/>
-      <c r="FH3" s="66"/>
-      <c r="FI3" s="66"/>
-      <c r="FJ3" s="66"/>
-      <c r="FK3" s="66"/>
-      <c r="FL3" s="66"/>
-      <c r="FM3" s="66"/>
-      <c r="FN3" s="66"/>
-      <c r="FO3" s="66"/>
-      <c r="FP3" s="66"/>
-      <c r="FQ3" s="66"/>
-      <c r="FR3" s="66"/>
-      <c r="FS3" s="66"/>
-      <c r="FT3" s="66"/>
-      <c r="FU3" s="66"/>
-      <c r="FV3" s="66"/>
-      <c r="FW3" s="66"/>
-      <c r="FX3" s="66"/>
-      <c r="FY3" s="66"/>
-      <c r="FZ3" s="66"/>
-      <c r="GA3" s="66"/>
-      <c r="GB3" s="66"/>
-      <c r="GC3" s="66"/>
-      <c r="GD3" s="66"/>
-      <c r="GE3" s="66"/>
-      <c r="GF3" s="66"/>
-      <c r="GG3" s="66"/>
-      <c r="GH3" s="66"/>
-      <c r="GI3" s="66"/>
-      <c r="GJ3" s="66"/>
-      <c r="GK3" s="66"/>
-      <c r="GL3" s="66"/>
-      <c r="GM3" s="66"/>
-      <c r="GN3" s="66"/>
-      <c r="GO3" s="66"/>
-      <c r="GP3" s="66"/>
-      <c r="GQ3" s="66"/>
-      <c r="GR3" s="66"/>
-      <c r="GS3" s="66"/>
-      <c r="GT3" s="66"/>
-      <c r="GU3" s="66"/>
-      <c r="GV3" s="66"/>
-      <c r="GW3" s="66"/>
-      <c r="GX3" s="66"/>
-      <c r="GY3" s="66"/>
-      <c r="GZ3" s="66"/>
-      <c r="HA3" s="66"/>
-      <c r="HB3" s="66"/>
-      <c r="HC3" s="66"/>
-      <c r="HD3" s="66"/>
-      <c r="HE3" s="66"/>
-      <c r="HF3" s="66"/>
-      <c r="HG3" s="66"/>
-      <c r="HH3" s="66"/>
-      <c r="HI3" s="66"/>
-      <c r="HJ3" s="66"/>
-      <c r="HK3" s="66"/>
-      <c r="HL3" s="66"/>
-      <c r="HM3" s="66"/>
-      <c r="HN3" s="66"/>
-      <c r="HO3" s="66"/>
-      <c r="HP3" s="66"/>
-      <c r="HQ3" s="66"/>
-      <c r="HR3" s="66"/>
-      <c r="HS3" s="66"/>
-      <c r="HT3" s="66"/>
-      <c r="HU3" s="66"/>
-      <c r="HV3" s="66"/>
-      <c r="HW3" s="66"/>
-      <c r="HX3" s="66"/>
-      <c r="HY3" s="66"/>
-      <c r="HZ3" s="66"/>
-      <c r="IA3" s="66"/>
-      <c r="IB3" s="66"/>
-      <c r="IC3" s="66"/>
-      <c r="ID3" s="66"/>
-      <c r="IE3" s="66"/>
-      <c r="IF3" s="66"/>
-      <c r="IG3" s="66"/>
-      <c r="IH3" s="66"/>
-      <c r="II3" s="66"/>
-      <c r="IJ3" s="66"/>
-      <c r="IK3" s="66"/>
-      <c r="IL3" s="66"/>
-      <c r="IM3" s="66"/>
-      <c r="IN3" s="66"/>
-      <c r="IO3" s="66"/>
-      <c r="IP3" s="66"/>
-      <c r="IQ3" s="66"/>
-      <c r="IR3" s="66"/>
-      <c r="IS3" s="66"/>
-      <c r="IT3" s="66"/>
-      <c r="IU3" s="66"/>
-      <c r="IV3" s="66"/>
-    </row>
-    <row r="4" spans="1:256" ht="15" customHeight="1">
+    <row r="3" spans="1:3" ht="15" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6">
+        <v>43071</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="97" t="s">
-        <v>107</v>
+        <v>5</v>
+      </c>
+      <c r="B4" s="6">
+        <v>43071</v>
       </c>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:256" ht="15" customHeight="1">
-      <c r="A5" s="76" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="77">
-        <v>42778</v>
-      </c>
-      <c r="C5" s="77" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:256" ht="15" customHeight="1">
+    <row r="5" spans="1:3" ht="15" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6">
+        <v>43071</v>
+      </c>
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="97" t="s">
-        <v>107</v>
+        <v>7</v>
+      </c>
+      <c r="B6" s="6">
+        <v>43071</v>
       </c>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:256" ht="15" customHeight="1">
-      <c r="A7" s="76" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="77">
-        <v>42778</v>
-      </c>
-      <c r="C7" s="77">
-        <v>42778</v>
-      </c>
-    </row>
-    <row r="8" spans="1:256" ht="15" customHeight="1">
+    <row r="7" spans="1:3" ht="15" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1">
       <c r="A8" s="87" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="88"/>
       <c r="C8" s="88"/>
     </row>
-    <row r="9" spans="1:256" ht="15" customHeight="1">
+    <row r="9" spans="1:3" ht="15" customHeight="1">
       <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
     </row>
-    <row r="10" spans="1:256" ht="15" customHeight="1">
+    <row r="10" spans="1:3" ht="15" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
     </row>
-    <row r="11" spans="1:256" ht="15" customHeight="1">
+    <row r="11" spans="1:3" ht="15" customHeight="1">
       <c r="A11" s="8"/>
       <c r="B11" s="16"/>
       <c r="C11" s="17"/>
     </row>
-    <row r="12" spans="1:256" ht="15" customHeight="1">
+    <row r="12" spans="1:3" ht="15" customHeight="1">
       <c r="A12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
     </row>
-    <row r="13" spans="1:256" ht="15" customHeight="1">
+    <row r="13" spans="1:3" ht="15" customHeight="1">
       <c r="A13" s="20"/>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
     </row>
-    <row r="14" spans="1:256" ht="15" customHeight="1">
+    <row r="14" spans="1:3" ht="15" customHeight="1">
       <c r="A14" s="21"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:256" ht="15" hidden="1" customHeight="1">
+    <row r="15" spans="1:3" ht="15" hidden="1" customHeight="1">
       <c r="A15" s="21"/>
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:256" ht="15" hidden="1" customHeight="1">
+    <row r="16" spans="1:3" ht="15" hidden="1" customHeight="1">
       <c r="A16" s="21"/>
       <c r="B16" s="14"/>
       <c r="C16" s="15"/>
@@ -2498,7 +2215,7 @@
     <mergeCell ref="A19:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2516,8 +2233,8 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="82.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="22" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="256" width="8.85546875" style="22" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2540,58 +2257,58 @@
       </c>
     </row>
     <row r="3" spans="1:256" ht="15" customHeight="1">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="77">
-        <v>42778</v>
-      </c>
-      <c r="C3" s="77">
-        <v>42778</v>
+      <c r="B3" s="78">
+        <v>43071</v>
+      </c>
+      <c r="C3" s="80">
+        <v>43041</v>
       </c>
     </row>
     <row r="4" spans="1:256" ht="15" customHeight="1">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="77">
-        <v>42778</v>
-      </c>
-      <c r="C4" s="77">
-        <v>42778</v>
+      <c r="B4" s="78">
+        <v>43071</v>
+      </c>
+      <c r="C4" s="80">
+        <v>43041</v>
       </c>
     </row>
     <row r="5" spans="1:256" ht="15" customHeight="1">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="77">
-        <v>42778</v>
-      </c>
-      <c r="C5" s="77" t="s">
-        <v>109</v>
+      <c r="B5" s="78">
+        <v>43071</v>
+      </c>
+      <c r="C5" s="80">
+        <v>43041</v>
       </c>
     </row>
     <row r="6" spans="1:256" ht="15" customHeight="1">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="77">
-        <v>42778</v>
-      </c>
-      <c r="C6" s="77">
-        <v>42778</v>
+      <c r="B6" s="78">
+        <v>43071</v>
+      </c>
+      <c r="C6" s="80">
+        <v>43041</v>
       </c>
     </row>
     <row r="7" spans="1:256" ht="15" customHeight="1">
-      <c r="A7" s="76" t="s">
+      <c r="A7" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="77">
-        <v>42778</v>
-      </c>
-      <c r="C7" s="77">
-        <v>42778</v>
+      <c r="B7" s="78">
+        <v>43071</v>
+      </c>
+      <c r="C7" s="80">
+        <v>43041</v>
       </c>
       <c r="D7" s="66"/>
       <c r="E7" s="66"/>
@@ -2848,14 +2565,14 @@
       <c r="IV7" s="66"/>
     </row>
     <row r="8" spans="1:256" ht="15" customHeight="1">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="77">
-        <v>42778</v>
-      </c>
-      <c r="C8" s="77">
-        <v>42778</v>
+      <c r="B8" s="78">
+        <v>43071</v>
+      </c>
+      <c r="C8" s="80">
+        <v>43041</v>
       </c>
       <c r="D8" s="66"/>
       <c r="E8" s="66"/>
@@ -3116,29 +2833,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="6">
-        <v>42778</v>
-      </c>
-      <c r="C9" s="99" t="s">
-        <v>109</v>
-      </c>
+        <v>43071</v>
+      </c>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:256" ht="15" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="6">
-        <v>42778</v>
-      </c>
-      <c r="C10" s="99" t="s">
-        <v>109</v>
-      </c>
+        <v>43071</v>
+      </c>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:256" ht="15" customHeight="1">
-      <c r="A11" s="75" t="s">
-        <v>97</v>
+      <c r="A11" s="76" t="s">
+        <v>98</v>
       </c>
       <c r="B11" s="6">
-        <v>42785</v>
+        <v>43071</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="66"/>
@@ -3396,12 +3109,8 @@
       <c r="IV11" s="66"/>
     </row>
     <row r="12" spans="1:256" ht="15" customHeight="1">
-      <c r="A12" s="98" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="6">
-        <v>42785</v>
-      </c>
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:256" ht="15" customHeight="1">
@@ -3495,10 +3204,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV33"/>
+  <dimension ref="A1:IV32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A13" sqref="A13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -3528,36 +3237,36 @@
       </c>
     </row>
     <row r="3" spans="1:256" ht="15" customHeight="1">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="77">
-        <v>42778</v>
-      </c>
-      <c r="C3" s="74">
-        <v>42777</v>
+      <c r="B3" s="78">
+        <v>43071</v>
+      </c>
+      <c r="C3" s="75">
+        <v>43041</v>
       </c>
     </row>
     <row r="4" spans="1:256" ht="15" customHeight="1">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="77">
-        <v>42778</v>
-      </c>
-      <c r="C4" s="74">
-        <v>42777</v>
+      <c r="B4" s="78">
+        <v>43071</v>
+      </c>
+      <c r="C4" s="75">
+        <v>43041</v>
       </c>
     </row>
     <row r="5" spans="1:256" ht="15" customHeight="1">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="77">
-        <v>42778</v>
-      </c>
-      <c r="C5" s="74">
-        <v>42777</v>
+      <c r="B5" s="78">
+        <v>43071</v>
+      </c>
+      <c r="C5" s="80">
+        <v>43041</v>
       </c>
       <c r="D5" s="66"/>
       <c r="E5" s="66"/>
@@ -3814,299 +3523,46 @@
       <c r="IV5" s="66"/>
     </row>
     <row r="6" spans="1:256" ht="15" customHeight="1">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="6">
+        <v>43071</v>
+      </c>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:256" ht="15" customHeight="1">
+      <c r="A7" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="77">
-        <v>42778</v>
-      </c>
-      <c r="C6" s="74">
-        <v>42777</v>
-      </c>
-    </row>
-    <row r="7" spans="1:256" ht="15" customHeight="1">
-      <c r="A7" s="76" t="s">
+      <c r="B7" s="78">
+        <v>43071</v>
+      </c>
+      <c r="C7" s="75">
+        <v>43041</v>
+      </c>
+    </row>
+    <row r="8" spans="1:256" ht="15" customHeight="1">
+      <c r="A8" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="77">
-        <v>42778</v>
-      </c>
-      <c r="C7" s="77">
-        <v>42778</v>
-      </c>
-    </row>
-    <row r="8" spans="1:256" ht="15" customHeight="1">
-      <c r="A8" s="73" t="s">
+      <c r="B8" s="78">
+        <v>43071</v>
+      </c>
+      <c r="C8" s="80">
+        <v>43071</v>
+      </c>
+    </row>
+    <row r="9" spans="1:256" ht="15" customHeight="1">
+      <c r="A9" s="73" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="77">
-        <v>42778</v>
-      </c>
-      <c r="C8" s="74">
-        <v>42777</v>
-      </c>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="66"/>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="66"/>
-      <c r="R8" s="66"/>
-      <c r="S8" s="66"/>
-      <c r="T8" s="66"/>
-      <c r="U8" s="66"/>
-      <c r="V8" s="66"/>
-      <c r="W8" s="66"/>
-      <c r="X8" s="66"/>
-      <c r="Y8" s="66"/>
-      <c r="Z8" s="66"/>
-      <c r="AA8" s="66"/>
-      <c r="AB8" s="66"/>
-      <c r="AC8" s="66"/>
-      <c r="AD8" s="66"/>
-      <c r="AE8" s="66"/>
-      <c r="AF8" s="66"/>
-      <c r="AG8" s="66"/>
-      <c r="AH8" s="66"/>
-      <c r="AI8" s="66"/>
-      <c r="AJ8" s="66"/>
-      <c r="AK8" s="66"/>
-      <c r="AL8" s="66"/>
-      <c r="AM8" s="66"/>
-      <c r="AN8" s="66"/>
-      <c r="AO8" s="66"/>
-      <c r="AP8" s="66"/>
-      <c r="AQ8" s="66"/>
-      <c r="AR8" s="66"/>
-      <c r="AS8" s="66"/>
-      <c r="AT8" s="66"/>
-      <c r="AU8" s="66"/>
-      <c r="AV8" s="66"/>
-      <c r="AW8" s="66"/>
-      <c r="AX8" s="66"/>
-      <c r="AY8" s="66"/>
-      <c r="AZ8" s="66"/>
-      <c r="BA8" s="66"/>
-      <c r="BB8" s="66"/>
-      <c r="BC8" s="66"/>
-      <c r="BD8" s="66"/>
-      <c r="BE8" s="66"/>
-      <c r="BF8" s="66"/>
-      <c r="BG8" s="66"/>
-      <c r="BH8" s="66"/>
-      <c r="BI8" s="66"/>
-      <c r="BJ8" s="66"/>
-      <c r="BK8" s="66"/>
-      <c r="BL8" s="66"/>
-      <c r="BM8" s="66"/>
-      <c r="BN8" s="66"/>
-      <c r="BO8" s="66"/>
-      <c r="BP8" s="66"/>
-      <c r="BQ8" s="66"/>
-      <c r="BR8" s="66"/>
-      <c r="BS8" s="66"/>
-      <c r="BT8" s="66"/>
-      <c r="BU8" s="66"/>
-      <c r="BV8" s="66"/>
-      <c r="BW8" s="66"/>
-      <c r="BX8" s="66"/>
-      <c r="BY8" s="66"/>
-      <c r="BZ8" s="66"/>
-      <c r="CA8" s="66"/>
-      <c r="CB8" s="66"/>
-      <c r="CC8" s="66"/>
-      <c r="CD8" s="66"/>
-      <c r="CE8" s="66"/>
-      <c r="CF8" s="66"/>
-      <c r="CG8" s="66"/>
-      <c r="CH8" s="66"/>
-      <c r="CI8" s="66"/>
-      <c r="CJ8" s="66"/>
-      <c r="CK8" s="66"/>
-      <c r="CL8" s="66"/>
-      <c r="CM8" s="66"/>
-      <c r="CN8" s="66"/>
-      <c r="CO8" s="66"/>
-      <c r="CP8" s="66"/>
-      <c r="CQ8" s="66"/>
-      <c r="CR8" s="66"/>
-      <c r="CS8" s="66"/>
-      <c r="CT8" s="66"/>
-      <c r="CU8" s="66"/>
-      <c r="CV8" s="66"/>
-      <c r="CW8" s="66"/>
-      <c r="CX8" s="66"/>
-      <c r="CY8" s="66"/>
-      <c r="CZ8" s="66"/>
-      <c r="DA8" s="66"/>
-      <c r="DB8" s="66"/>
-      <c r="DC8" s="66"/>
-      <c r="DD8" s="66"/>
-      <c r="DE8" s="66"/>
-      <c r="DF8" s="66"/>
-      <c r="DG8" s="66"/>
-      <c r="DH8" s="66"/>
-      <c r="DI8" s="66"/>
-      <c r="DJ8" s="66"/>
-      <c r="DK8" s="66"/>
-      <c r="DL8" s="66"/>
-      <c r="DM8" s="66"/>
-      <c r="DN8" s="66"/>
-      <c r="DO8" s="66"/>
-      <c r="DP8" s="66"/>
-      <c r="DQ8" s="66"/>
-      <c r="DR8" s="66"/>
-      <c r="DS8" s="66"/>
-      <c r="DT8" s="66"/>
-      <c r="DU8" s="66"/>
-      <c r="DV8" s="66"/>
-      <c r="DW8" s="66"/>
-      <c r="DX8" s="66"/>
-      <c r="DY8" s="66"/>
-      <c r="DZ8" s="66"/>
-      <c r="EA8" s="66"/>
-      <c r="EB8" s="66"/>
-      <c r="EC8" s="66"/>
-      <c r="ED8" s="66"/>
-      <c r="EE8" s="66"/>
-      <c r="EF8" s="66"/>
-      <c r="EG8" s="66"/>
-      <c r="EH8" s="66"/>
-      <c r="EI8" s="66"/>
-      <c r="EJ8" s="66"/>
-      <c r="EK8" s="66"/>
-      <c r="EL8" s="66"/>
-      <c r="EM8" s="66"/>
-      <c r="EN8" s="66"/>
-      <c r="EO8" s="66"/>
-      <c r="EP8" s="66"/>
-      <c r="EQ8" s="66"/>
-      <c r="ER8" s="66"/>
-      <c r="ES8" s="66"/>
-      <c r="ET8" s="66"/>
-      <c r="EU8" s="66"/>
-      <c r="EV8" s="66"/>
-      <c r="EW8" s="66"/>
-      <c r="EX8" s="66"/>
-      <c r="EY8" s="66"/>
-      <c r="EZ8" s="66"/>
-      <c r="FA8" s="66"/>
-      <c r="FB8" s="66"/>
-      <c r="FC8" s="66"/>
-      <c r="FD8" s="66"/>
-      <c r="FE8" s="66"/>
-      <c r="FF8" s="66"/>
-      <c r="FG8" s="66"/>
-      <c r="FH8" s="66"/>
-      <c r="FI8" s="66"/>
-      <c r="FJ8" s="66"/>
-      <c r="FK8" s="66"/>
-      <c r="FL8" s="66"/>
-      <c r="FM8" s="66"/>
-      <c r="FN8" s="66"/>
-      <c r="FO8" s="66"/>
-      <c r="FP8" s="66"/>
-      <c r="FQ8" s="66"/>
-      <c r="FR8" s="66"/>
-      <c r="FS8" s="66"/>
-      <c r="FT8" s="66"/>
-      <c r="FU8" s="66"/>
-      <c r="FV8" s="66"/>
-      <c r="FW8" s="66"/>
-      <c r="FX8" s="66"/>
-      <c r="FY8" s="66"/>
-      <c r="FZ8" s="66"/>
-      <c r="GA8" s="66"/>
-      <c r="GB8" s="66"/>
-      <c r="GC8" s="66"/>
-      <c r="GD8" s="66"/>
-      <c r="GE8" s="66"/>
-      <c r="GF8" s="66"/>
-      <c r="GG8" s="66"/>
-      <c r="GH8" s="66"/>
-      <c r="GI8" s="66"/>
-      <c r="GJ8" s="66"/>
-      <c r="GK8" s="66"/>
-      <c r="GL8" s="66"/>
-      <c r="GM8" s="66"/>
-      <c r="GN8" s="66"/>
-      <c r="GO8" s="66"/>
-      <c r="GP8" s="66"/>
-      <c r="GQ8" s="66"/>
-      <c r="GR8" s="66"/>
-      <c r="GS8" s="66"/>
-      <c r="GT8" s="66"/>
-      <c r="GU8" s="66"/>
-      <c r="GV8" s="66"/>
-      <c r="GW8" s="66"/>
-      <c r="GX8" s="66"/>
-      <c r="GY8" s="66"/>
-      <c r="GZ8" s="66"/>
-      <c r="HA8" s="66"/>
-      <c r="HB8" s="66"/>
-      <c r="HC8" s="66"/>
-      <c r="HD8" s="66"/>
-      <c r="HE8" s="66"/>
-      <c r="HF8" s="66"/>
-      <c r="HG8" s="66"/>
-      <c r="HH8" s="66"/>
-      <c r="HI8" s="66"/>
-      <c r="HJ8" s="66"/>
-      <c r="HK8" s="66"/>
-      <c r="HL8" s="66"/>
-      <c r="HM8" s="66"/>
-      <c r="HN8" s="66"/>
-      <c r="HO8" s="66"/>
-      <c r="HP8" s="66"/>
-      <c r="HQ8" s="66"/>
-      <c r="HR8" s="66"/>
-      <c r="HS8" s="66"/>
-      <c r="HT8" s="66"/>
-      <c r="HU8" s="66"/>
-      <c r="HV8" s="66"/>
-      <c r="HW8" s="66"/>
-      <c r="HX8" s="66"/>
-      <c r="HY8" s="66"/>
-      <c r="HZ8" s="66"/>
-      <c r="IA8" s="66"/>
-      <c r="IB8" s="66"/>
-      <c r="IC8" s="66"/>
-      <c r="ID8" s="66"/>
-      <c r="IE8" s="66"/>
-      <c r="IF8" s="66"/>
-      <c r="IG8" s="66"/>
-      <c r="IH8" s="66"/>
-      <c r="II8" s="66"/>
-      <c r="IJ8" s="66"/>
-      <c r="IK8" s="66"/>
-      <c r="IL8" s="66"/>
-      <c r="IM8" s="66"/>
-      <c r="IN8" s="66"/>
-      <c r="IO8" s="66"/>
-      <c r="IP8" s="66"/>
-      <c r="IQ8" s="66"/>
-      <c r="IR8" s="66"/>
-      <c r="IS8" s="66"/>
-      <c r="IT8" s="66"/>
-      <c r="IU8" s="66"/>
-      <c r="IV8" s="66"/>
-    </row>
-    <row r="9" spans="1:256" ht="15" customHeight="1">
-      <c r="A9" s="71" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" s="6">
-        <v>42778</v>
-      </c>
-      <c r="C9" s="10"/>
+      <c r="B9" s="74">
+        <v>43071</v>
+      </c>
+      <c r="C9" s="75">
+        <v>43041</v>
+      </c>
       <c r="D9" s="66"/>
       <c r="E9" s="66"/>
       <c r="F9" s="66"/>
@@ -4363,10 +3819,10 @@
     </row>
     <row r="10" spans="1:256" ht="15" customHeight="1">
       <c r="A10" s="71" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="6">
-        <v>42778</v>
+        <v>105</v>
+      </c>
+      <c r="B10" s="9">
+        <v>43071</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="66"/>
@@ -4624,11 +4080,11 @@
       <c r="IV10" s="66"/>
     </row>
     <row r="11" spans="1:256" ht="15" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="6">
-        <v>42778</v>
+      <c r="A11" s="71" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="9">
+        <v>43071</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="66"/>
@@ -4886,285 +4342,287 @@
       <c r="IV11" s="66"/>
     </row>
     <row r="12" spans="1:256" ht="15" customHeight="1">
-      <c r="A12" s="71"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="66"/>
-      <c r="O12" s="66"/>
-      <c r="P12" s="66"/>
-      <c r="Q12" s="66"/>
-      <c r="R12" s="66"/>
-      <c r="S12" s="66"/>
-      <c r="T12" s="66"/>
-      <c r="U12" s="66"/>
-      <c r="V12" s="66"/>
-      <c r="W12" s="66"/>
-      <c r="X12" s="66"/>
-      <c r="Y12" s="66"/>
-      <c r="Z12" s="66"/>
-      <c r="AA12" s="66"/>
-      <c r="AB12" s="66"/>
-      <c r="AC12" s="66"/>
-      <c r="AD12" s="66"/>
-      <c r="AE12" s="66"/>
-      <c r="AF12" s="66"/>
-      <c r="AG12" s="66"/>
-      <c r="AH12" s="66"/>
-      <c r="AI12" s="66"/>
-      <c r="AJ12" s="66"/>
-      <c r="AK12" s="66"/>
-      <c r="AL12" s="66"/>
-      <c r="AM12" s="66"/>
-      <c r="AN12" s="66"/>
-      <c r="AO12" s="66"/>
-      <c r="AP12" s="66"/>
-      <c r="AQ12" s="66"/>
-      <c r="AR12" s="66"/>
-      <c r="AS12" s="66"/>
-      <c r="AT12" s="66"/>
-      <c r="AU12" s="66"/>
-      <c r="AV12" s="66"/>
-      <c r="AW12" s="66"/>
-      <c r="AX12" s="66"/>
-      <c r="AY12" s="66"/>
-      <c r="AZ12" s="66"/>
-      <c r="BA12" s="66"/>
-      <c r="BB12" s="66"/>
-      <c r="BC12" s="66"/>
-      <c r="BD12" s="66"/>
-      <c r="BE12" s="66"/>
-      <c r="BF12" s="66"/>
-      <c r="BG12" s="66"/>
-      <c r="BH12" s="66"/>
-      <c r="BI12" s="66"/>
-      <c r="BJ12" s="66"/>
-      <c r="BK12" s="66"/>
-      <c r="BL12" s="66"/>
-      <c r="BM12" s="66"/>
-      <c r="BN12" s="66"/>
-      <c r="BO12" s="66"/>
-      <c r="BP12" s="66"/>
-      <c r="BQ12" s="66"/>
-      <c r="BR12" s="66"/>
-      <c r="BS12" s="66"/>
-      <c r="BT12" s="66"/>
-      <c r="BU12" s="66"/>
-      <c r="BV12" s="66"/>
-      <c r="BW12" s="66"/>
-      <c r="BX12" s="66"/>
-      <c r="BY12" s="66"/>
-      <c r="BZ12" s="66"/>
-      <c r="CA12" s="66"/>
-      <c r="CB12" s="66"/>
-      <c r="CC12" s="66"/>
-      <c r="CD12" s="66"/>
-      <c r="CE12" s="66"/>
-      <c r="CF12" s="66"/>
-      <c r="CG12" s="66"/>
-      <c r="CH12" s="66"/>
-      <c r="CI12" s="66"/>
-      <c r="CJ12" s="66"/>
-      <c r="CK12" s="66"/>
-      <c r="CL12" s="66"/>
-      <c r="CM12" s="66"/>
-      <c r="CN12" s="66"/>
-      <c r="CO12" s="66"/>
-      <c r="CP12" s="66"/>
-      <c r="CQ12" s="66"/>
-      <c r="CR12" s="66"/>
-      <c r="CS12" s="66"/>
-      <c r="CT12" s="66"/>
-      <c r="CU12" s="66"/>
-      <c r="CV12" s="66"/>
-      <c r="CW12" s="66"/>
-      <c r="CX12" s="66"/>
-      <c r="CY12" s="66"/>
-      <c r="CZ12" s="66"/>
-      <c r="DA12" s="66"/>
-      <c r="DB12" s="66"/>
-      <c r="DC12" s="66"/>
-      <c r="DD12" s="66"/>
-      <c r="DE12" s="66"/>
-      <c r="DF12" s="66"/>
-      <c r="DG12" s="66"/>
-      <c r="DH12" s="66"/>
-      <c r="DI12" s="66"/>
-      <c r="DJ12" s="66"/>
-      <c r="DK12" s="66"/>
-      <c r="DL12" s="66"/>
-      <c r="DM12" s="66"/>
-      <c r="DN12" s="66"/>
-      <c r="DO12" s="66"/>
-      <c r="DP12" s="66"/>
-      <c r="DQ12" s="66"/>
-      <c r="DR12" s="66"/>
-      <c r="DS12" s="66"/>
-      <c r="DT12" s="66"/>
-      <c r="DU12" s="66"/>
-      <c r="DV12" s="66"/>
-      <c r="DW12" s="66"/>
-      <c r="DX12" s="66"/>
-      <c r="DY12" s="66"/>
-      <c r="DZ12" s="66"/>
-      <c r="EA12" s="66"/>
-      <c r="EB12" s="66"/>
-      <c r="EC12" s="66"/>
-      <c r="ED12" s="66"/>
-      <c r="EE12" s="66"/>
-      <c r="EF12" s="66"/>
-      <c r="EG12" s="66"/>
-      <c r="EH12" s="66"/>
-      <c r="EI12" s="66"/>
-      <c r="EJ12" s="66"/>
-      <c r="EK12" s="66"/>
-      <c r="EL12" s="66"/>
-      <c r="EM12" s="66"/>
-      <c r="EN12" s="66"/>
-      <c r="EO12" s="66"/>
-      <c r="EP12" s="66"/>
-      <c r="EQ12" s="66"/>
-      <c r="ER12" s="66"/>
-      <c r="ES12" s="66"/>
-      <c r="ET12" s="66"/>
-      <c r="EU12" s="66"/>
-      <c r="EV12" s="66"/>
-      <c r="EW12" s="66"/>
-      <c r="EX12" s="66"/>
-      <c r="EY12" s="66"/>
-      <c r="EZ12" s="66"/>
-      <c r="FA12" s="66"/>
-      <c r="FB12" s="66"/>
-      <c r="FC12" s="66"/>
-      <c r="FD12" s="66"/>
-      <c r="FE12" s="66"/>
-      <c r="FF12" s="66"/>
-      <c r="FG12" s="66"/>
-      <c r="FH12" s="66"/>
-      <c r="FI12" s="66"/>
-      <c r="FJ12" s="66"/>
-      <c r="FK12" s="66"/>
-      <c r="FL12" s="66"/>
-      <c r="FM12" s="66"/>
-      <c r="FN12" s="66"/>
-      <c r="FO12" s="66"/>
-      <c r="FP12" s="66"/>
-      <c r="FQ12" s="66"/>
-      <c r="FR12" s="66"/>
-      <c r="FS12" s="66"/>
-      <c r="FT12" s="66"/>
-      <c r="FU12" s="66"/>
-      <c r="FV12" s="66"/>
-      <c r="FW12" s="66"/>
-      <c r="FX12" s="66"/>
-      <c r="FY12" s="66"/>
-      <c r="FZ12" s="66"/>
-      <c r="GA12" s="66"/>
-      <c r="GB12" s="66"/>
-      <c r="GC12" s="66"/>
-      <c r="GD12" s="66"/>
-      <c r="GE12" s="66"/>
-      <c r="GF12" s="66"/>
-      <c r="GG12" s="66"/>
-      <c r="GH12" s="66"/>
-      <c r="GI12" s="66"/>
-      <c r="GJ12" s="66"/>
-      <c r="GK12" s="66"/>
-      <c r="GL12" s="66"/>
-      <c r="GM12" s="66"/>
-      <c r="GN12" s="66"/>
-      <c r="GO12" s="66"/>
-      <c r="GP12" s="66"/>
-      <c r="GQ12" s="66"/>
-      <c r="GR12" s="66"/>
-      <c r="GS12" s="66"/>
-      <c r="GT12" s="66"/>
-      <c r="GU12" s="66"/>
-      <c r="GV12" s="66"/>
-      <c r="GW12" s="66"/>
-      <c r="GX12" s="66"/>
-      <c r="GY12" s="66"/>
-      <c r="GZ12" s="66"/>
-      <c r="HA12" s="66"/>
-      <c r="HB12" s="66"/>
-      <c r="HC12" s="66"/>
-      <c r="HD12" s="66"/>
-      <c r="HE12" s="66"/>
-      <c r="HF12" s="66"/>
-      <c r="HG12" s="66"/>
-      <c r="HH12" s="66"/>
-      <c r="HI12" s="66"/>
-      <c r="HJ12" s="66"/>
-      <c r="HK12" s="66"/>
-      <c r="HL12" s="66"/>
-      <c r="HM12" s="66"/>
-      <c r="HN12" s="66"/>
-      <c r="HO12" s="66"/>
-      <c r="HP12" s="66"/>
-      <c r="HQ12" s="66"/>
-      <c r="HR12" s="66"/>
-      <c r="HS12" s="66"/>
-      <c r="HT12" s="66"/>
-      <c r="HU12" s="66"/>
-      <c r="HV12" s="66"/>
-      <c r="HW12" s="66"/>
-      <c r="HX12" s="66"/>
-      <c r="HY12" s="66"/>
-      <c r="HZ12" s="66"/>
-      <c r="IA12" s="66"/>
-      <c r="IB12" s="66"/>
-      <c r="IC12" s="66"/>
-      <c r="ID12" s="66"/>
-      <c r="IE12" s="66"/>
-      <c r="IF12" s="66"/>
-      <c r="IG12" s="66"/>
-      <c r="IH12" s="66"/>
-      <c r="II12" s="66"/>
-      <c r="IJ12" s="66"/>
-      <c r="IK12" s="66"/>
-      <c r="IL12" s="66"/>
-      <c r="IM12" s="66"/>
-      <c r="IN12" s="66"/>
-      <c r="IO12" s="66"/>
-      <c r="IP12" s="66"/>
-      <c r="IQ12" s="66"/>
-      <c r="IR12" s="66"/>
-      <c r="IS12" s="66"/>
-      <c r="IT12" s="66"/>
-      <c r="IU12" s="66"/>
-      <c r="IV12" s="66"/>
     </row>
     <row r="13" spans="1:256" ht="15" customHeight="1">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
+      <c r="A13" s="87" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="88"/>
+      <c r="C13" s="88"/>
     </row>
     <row r="14" spans="1:256" ht="15" customHeight="1">
-      <c r="A14" s="87" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="88"/>
-      <c r="C14" s="88"/>
+      <c r="A14" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
     </row>
     <row r="15" spans="1:256" ht="15" customHeight="1">
-      <c r="A15" s="75" t="s">
-        <v>110</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
+      <c r="A15" s="79" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="66"/>
+      <c r="N15" s="66"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="66"/>
+      <c r="Q15" s="66"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="66"/>
+      <c r="V15" s="66"/>
+      <c r="W15" s="66"/>
+      <c r="X15" s="66"/>
+      <c r="Y15" s="66"/>
+      <c r="Z15" s="66"/>
+      <c r="AA15" s="66"/>
+      <c r="AB15" s="66"/>
+      <c r="AC15" s="66"/>
+      <c r="AD15" s="66"/>
+      <c r="AE15" s="66"/>
+      <c r="AF15" s="66"/>
+      <c r="AG15" s="66"/>
+      <c r="AH15" s="66"/>
+      <c r="AI15" s="66"/>
+      <c r="AJ15" s="66"/>
+      <c r="AK15" s="66"/>
+      <c r="AL15" s="66"/>
+      <c r="AM15" s="66"/>
+      <c r="AN15" s="66"/>
+      <c r="AO15" s="66"/>
+      <c r="AP15" s="66"/>
+      <c r="AQ15" s="66"/>
+      <c r="AR15" s="66"/>
+      <c r="AS15" s="66"/>
+      <c r="AT15" s="66"/>
+      <c r="AU15" s="66"/>
+      <c r="AV15" s="66"/>
+      <c r="AW15" s="66"/>
+      <c r="AX15" s="66"/>
+      <c r="AY15" s="66"/>
+      <c r="AZ15" s="66"/>
+      <c r="BA15" s="66"/>
+      <c r="BB15" s="66"/>
+      <c r="BC15" s="66"/>
+      <c r="BD15" s="66"/>
+      <c r="BE15" s="66"/>
+      <c r="BF15" s="66"/>
+      <c r="BG15" s="66"/>
+      <c r="BH15" s="66"/>
+      <c r="BI15" s="66"/>
+      <c r="BJ15" s="66"/>
+      <c r="BK15" s="66"/>
+      <c r="BL15" s="66"/>
+      <c r="BM15" s="66"/>
+      <c r="BN15" s="66"/>
+      <c r="BO15" s="66"/>
+      <c r="BP15" s="66"/>
+      <c r="BQ15" s="66"/>
+      <c r="BR15" s="66"/>
+      <c r="BS15" s="66"/>
+      <c r="BT15" s="66"/>
+      <c r="BU15" s="66"/>
+      <c r="BV15" s="66"/>
+      <c r="BW15" s="66"/>
+      <c r="BX15" s="66"/>
+      <c r="BY15" s="66"/>
+      <c r="BZ15" s="66"/>
+      <c r="CA15" s="66"/>
+      <c r="CB15" s="66"/>
+      <c r="CC15" s="66"/>
+      <c r="CD15" s="66"/>
+      <c r="CE15" s="66"/>
+      <c r="CF15" s="66"/>
+      <c r="CG15" s="66"/>
+      <c r="CH15" s="66"/>
+      <c r="CI15" s="66"/>
+      <c r="CJ15" s="66"/>
+      <c r="CK15" s="66"/>
+      <c r="CL15" s="66"/>
+      <c r="CM15" s="66"/>
+      <c r="CN15" s="66"/>
+      <c r="CO15" s="66"/>
+      <c r="CP15" s="66"/>
+      <c r="CQ15" s="66"/>
+      <c r="CR15" s="66"/>
+      <c r="CS15" s="66"/>
+      <c r="CT15" s="66"/>
+      <c r="CU15" s="66"/>
+      <c r="CV15" s="66"/>
+      <c r="CW15" s="66"/>
+      <c r="CX15" s="66"/>
+      <c r="CY15" s="66"/>
+      <c r="CZ15" s="66"/>
+      <c r="DA15" s="66"/>
+      <c r="DB15" s="66"/>
+      <c r="DC15" s="66"/>
+      <c r="DD15" s="66"/>
+      <c r="DE15" s="66"/>
+      <c r="DF15" s="66"/>
+      <c r="DG15" s="66"/>
+      <c r="DH15" s="66"/>
+      <c r="DI15" s="66"/>
+      <c r="DJ15" s="66"/>
+      <c r="DK15" s="66"/>
+      <c r="DL15" s="66"/>
+      <c r="DM15" s="66"/>
+      <c r="DN15" s="66"/>
+      <c r="DO15" s="66"/>
+      <c r="DP15" s="66"/>
+      <c r="DQ15" s="66"/>
+      <c r="DR15" s="66"/>
+      <c r="DS15" s="66"/>
+      <c r="DT15" s="66"/>
+      <c r="DU15" s="66"/>
+      <c r="DV15" s="66"/>
+      <c r="DW15" s="66"/>
+      <c r="DX15" s="66"/>
+      <c r="DY15" s="66"/>
+      <c r="DZ15" s="66"/>
+      <c r="EA15" s="66"/>
+      <c r="EB15" s="66"/>
+      <c r="EC15" s="66"/>
+      <c r="ED15" s="66"/>
+      <c r="EE15" s="66"/>
+      <c r="EF15" s="66"/>
+      <c r="EG15" s="66"/>
+      <c r="EH15" s="66"/>
+      <c r="EI15" s="66"/>
+      <c r="EJ15" s="66"/>
+      <c r="EK15" s="66"/>
+      <c r="EL15" s="66"/>
+      <c r="EM15" s="66"/>
+      <c r="EN15" s="66"/>
+      <c r="EO15" s="66"/>
+      <c r="EP15" s="66"/>
+      <c r="EQ15" s="66"/>
+      <c r="ER15" s="66"/>
+      <c r="ES15" s="66"/>
+      <c r="ET15" s="66"/>
+      <c r="EU15" s="66"/>
+      <c r="EV15" s="66"/>
+      <c r="EW15" s="66"/>
+      <c r="EX15" s="66"/>
+      <c r="EY15" s="66"/>
+      <c r="EZ15" s="66"/>
+      <c r="FA15" s="66"/>
+      <c r="FB15" s="66"/>
+      <c r="FC15" s="66"/>
+      <c r="FD15" s="66"/>
+      <c r="FE15" s="66"/>
+      <c r="FF15" s="66"/>
+      <c r="FG15" s="66"/>
+      <c r="FH15" s="66"/>
+      <c r="FI15" s="66"/>
+      <c r="FJ15" s="66"/>
+      <c r="FK15" s="66"/>
+      <c r="FL15" s="66"/>
+      <c r="FM15" s="66"/>
+      <c r="FN15" s="66"/>
+      <c r="FO15" s="66"/>
+      <c r="FP15" s="66"/>
+      <c r="FQ15" s="66"/>
+      <c r="FR15" s="66"/>
+      <c r="FS15" s="66"/>
+      <c r="FT15" s="66"/>
+      <c r="FU15" s="66"/>
+      <c r="FV15" s="66"/>
+      <c r="FW15" s="66"/>
+      <c r="FX15" s="66"/>
+      <c r="FY15" s="66"/>
+      <c r="FZ15" s="66"/>
+      <c r="GA15" s="66"/>
+      <c r="GB15" s="66"/>
+      <c r="GC15" s="66"/>
+      <c r="GD15" s="66"/>
+      <c r="GE15" s="66"/>
+      <c r="GF15" s="66"/>
+      <c r="GG15" s="66"/>
+      <c r="GH15" s="66"/>
+      <c r="GI15" s="66"/>
+      <c r="GJ15" s="66"/>
+      <c r="GK15" s="66"/>
+      <c r="GL15" s="66"/>
+      <c r="GM15" s="66"/>
+      <c r="GN15" s="66"/>
+      <c r="GO15" s="66"/>
+      <c r="GP15" s="66"/>
+      <c r="GQ15" s="66"/>
+      <c r="GR15" s="66"/>
+      <c r="GS15" s="66"/>
+      <c r="GT15" s="66"/>
+      <c r="GU15" s="66"/>
+      <c r="GV15" s="66"/>
+      <c r="GW15" s="66"/>
+      <c r="GX15" s="66"/>
+      <c r="GY15" s="66"/>
+      <c r="GZ15" s="66"/>
+      <c r="HA15" s="66"/>
+      <c r="HB15" s="66"/>
+      <c r="HC15" s="66"/>
+      <c r="HD15" s="66"/>
+      <c r="HE15" s="66"/>
+      <c r="HF15" s="66"/>
+      <c r="HG15" s="66"/>
+      <c r="HH15" s="66"/>
+      <c r="HI15" s="66"/>
+      <c r="HJ15" s="66"/>
+      <c r="HK15" s="66"/>
+      <c r="HL15" s="66"/>
+      <c r="HM15" s="66"/>
+      <c r="HN15" s="66"/>
+      <c r="HO15" s="66"/>
+      <c r="HP15" s="66"/>
+      <c r="HQ15" s="66"/>
+      <c r="HR15" s="66"/>
+      <c r="HS15" s="66"/>
+      <c r="HT15" s="66"/>
+      <c r="HU15" s="66"/>
+      <c r="HV15" s="66"/>
+      <c r="HW15" s="66"/>
+      <c r="HX15" s="66"/>
+      <c r="HY15" s="66"/>
+      <c r="HZ15" s="66"/>
+      <c r="IA15" s="66"/>
+      <c r="IB15" s="66"/>
+      <c r="IC15" s="66"/>
+      <c r="ID15" s="66"/>
+      <c r="IE15" s="66"/>
+      <c r="IF15" s="66"/>
+      <c r="IG15" s="66"/>
+      <c r="IH15" s="66"/>
+      <c r="II15" s="66"/>
+      <c r="IJ15" s="66"/>
+      <c r="IK15" s="66"/>
+      <c r="IL15" s="66"/>
+      <c r="IM15" s="66"/>
+      <c r="IN15" s="66"/>
+      <c r="IO15" s="66"/>
+      <c r="IP15" s="66"/>
+      <c r="IQ15" s="66"/>
+      <c r="IR15" s="66"/>
+      <c r="IS15" s="66"/>
+      <c r="IT15" s="66"/>
+      <c r="IU15" s="66"/>
+      <c r="IV15" s="66"/>
     </row>
     <row r="16" spans="1:256" ht="15" customHeight="1">
-      <c r="A16" s="78" t="s">
-        <v>96</v>
+      <c r="A16" s="76" t="s">
+        <v>93</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="17"/>
@@ -5423,8 +4881,8 @@
       <c r="IV16" s="66"/>
     </row>
     <row r="17" spans="1:256" ht="15" customHeight="1">
-      <c r="A17" s="75" t="s">
-        <v>93</v>
+      <c r="A17" s="76" t="s">
+        <v>94</v>
       </c>
       <c r="B17" s="16"/>
       <c r="C17" s="17"/>
@@ -5683,11 +5141,11 @@
       <c r="IV17" s="66"/>
     </row>
     <row r="18" spans="1:256" ht="15" customHeight="1">
-      <c r="A18" s="75" t="s">
-        <v>94</v>
-      </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
+      <c r="A18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
       <c r="D18" s="66"/>
       <c r="E18" s="66"/>
       <c r="F18" s="66"/>
@@ -5943,11 +5401,11 @@
       <c r="IV18" s="66"/>
     </row>
     <row r="19" spans="1:256" ht="15" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
+      <c r="A19" s="76" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="66"/>
       <c r="E19" s="66"/>
       <c r="F19" s="66"/>
@@ -6203,8 +5661,8 @@
       <c r="IV19" s="66"/>
     </row>
     <row r="20" spans="1:256" ht="15" customHeight="1">
-      <c r="A20" s="75" t="s">
-        <v>95</v>
+      <c r="A20" s="76" t="s">
+        <v>33</v>
       </c>
       <c r="B20" s="16"/>
       <c r="C20" s="17"/>
@@ -6463,8 +5921,8 @@
       <c r="IV20" s="66"/>
     </row>
     <row r="21" spans="1:256" ht="15" customHeight="1">
-      <c r="A21" s="75" t="s">
-        <v>33</v>
+      <c r="A21" s="76" t="s">
+        <v>99</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="17"/>
@@ -6723,11 +6181,11 @@
       <c r="IV21" s="66"/>
     </row>
     <row r="22" spans="1:256" ht="15" customHeight="1">
-      <c r="A22" s="75" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
+      <c r="A22" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="82"/>
+      <c r="C22" s="83"/>
       <c r="D22" s="66"/>
       <c r="E22" s="66"/>
       <c r="F22" s="66"/>
@@ -6983,11 +6441,11 @@
       <c r="IV22" s="66"/>
     </row>
     <row r="23" spans="1:256" ht="15" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" s="80"/>
-      <c r="C23" s="81"/>
+      <c r="A23" s="76" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="66"/>
       <c r="E23" s="66"/>
       <c r="F23" s="66"/>
@@ -7243,11 +6701,11 @@
       <c r="IV23" s="66"/>
     </row>
     <row r="24" spans="1:256" ht="15" customHeight="1">
-      <c r="A24" s="75" t="s">
-        <v>100</v>
-      </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="17"/>
+      <c r="A24" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="82"/>
+      <c r="C24" s="83"/>
       <c r="D24" s="66"/>
       <c r="E24" s="66"/>
       <c r="F24" s="66"/>
@@ -7503,11 +6961,11 @@
       <c r="IV24" s="66"/>
     </row>
     <row r="25" spans="1:256" ht="15" customHeight="1">
-      <c r="A25" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B25" s="80"/>
-      <c r="C25" s="81"/>
+      <c r="A25" s="71" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="66"/>
       <c r="E25" s="66"/>
       <c r="F25" s="66"/>
@@ -7764,7 +7222,7 @@
     </row>
     <row r="26" spans="1:256" ht="15" customHeight="1">
       <c r="A26" s="71" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="17"/>
@@ -8023,276 +7481,274 @@
       <c r="IV26" s="66"/>
     </row>
     <row r="27" spans="1:256" ht="15" customHeight="1">
-      <c r="A27" s="71" t="s">
-        <v>104</v>
-      </c>
+      <c r="A27" s="8"/>
       <c r="B27" s="16"/>
       <c r="C27" s="17"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="66"/>
-      <c r="J27" s="66"/>
-      <c r="K27" s="66"/>
-      <c r="L27" s="66"/>
-      <c r="M27" s="66"/>
-      <c r="N27" s="66"/>
-      <c r="O27" s="66"/>
-      <c r="P27" s="66"/>
-      <c r="Q27" s="66"/>
-      <c r="R27" s="66"/>
-      <c r="S27" s="66"/>
-      <c r="T27" s="66"/>
-      <c r="U27" s="66"/>
-      <c r="V27" s="66"/>
-      <c r="W27" s="66"/>
-      <c r="X27" s="66"/>
-      <c r="Y27" s="66"/>
-      <c r="Z27" s="66"/>
-      <c r="AA27" s="66"/>
-      <c r="AB27" s="66"/>
-      <c r="AC27" s="66"/>
-      <c r="AD27" s="66"/>
-      <c r="AE27" s="66"/>
-      <c r="AF27" s="66"/>
-      <c r="AG27" s="66"/>
-      <c r="AH27" s="66"/>
-      <c r="AI27" s="66"/>
-      <c r="AJ27" s="66"/>
-      <c r="AK27" s="66"/>
-      <c r="AL27" s="66"/>
-      <c r="AM27" s="66"/>
-      <c r="AN27" s="66"/>
-      <c r="AO27" s="66"/>
-      <c r="AP27" s="66"/>
-      <c r="AQ27" s="66"/>
-      <c r="AR27" s="66"/>
-      <c r="AS27" s="66"/>
-      <c r="AT27" s="66"/>
-      <c r="AU27" s="66"/>
-      <c r="AV27" s="66"/>
-      <c r="AW27" s="66"/>
-      <c r="AX27" s="66"/>
-      <c r="AY27" s="66"/>
-      <c r="AZ27" s="66"/>
-      <c r="BA27" s="66"/>
-      <c r="BB27" s="66"/>
-      <c r="BC27" s="66"/>
-      <c r="BD27" s="66"/>
-      <c r="BE27" s="66"/>
-      <c r="BF27" s="66"/>
-      <c r="BG27" s="66"/>
-      <c r="BH27" s="66"/>
-      <c r="BI27" s="66"/>
-      <c r="BJ27" s="66"/>
-      <c r="BK27" s="66"/>
-      <c r="BL27" s="66"/>
-      <c r="BM27" s="66"/>
-      <c r="BN27" s="66"/>
-      <c r="BO27" s="66"/>
-      <c r="BP27" s="66"/>
-      <c r="BQ27" s="66"/>
-      <c r="BR27" s="66"/>
-      <c r="BS27" s="66"/>
-      <c r="BT27" s="66"/>
-      <c r="BU27" s="66"/>
-      <c r="BV27" s="66"/>
-      <c r="BW27" s="66"/>
-      <c r="BX27" s="66"/>
-      <c r="BY27" s="66"/>
-      <c r="BZ27" s="66"/>
-      <c r="CA27" s="66"/>
-      <c r="CB27" s="66"/>
-      <c r="CC27" s="66"/>
-      <c r="CD27" s="66"/>
-      <c r="CE27" s="66"/>
-      <c r="CF27" s="66"/>
-      <c r="CG27" s="66"/>
-      <c r="CH27" s="66"/>
-      <c r="CI27" s="66"/>
-      <c r="CJ27" s="66"/>
-      <c r="CK27" s="66"/>
-      <c r="CL27" s="66"/>
-      <c r="CM27" s="66"/>
-      <c r="CN27" s="66"/>
-      <c r="CO27" s="66"/>
-      <c r="CP27" s="66"/>
-      <c r="CQ27" s="66"/>
-      <c r="CR27" s="66"/>
-      <c r="CS27" s="66"/>
-      <c r="CT27" s="66"/>
-      <c r="CU27" s="66"/>
-      <c r="CV27" s="66"/>
-      <c r="CW27" s="66"/>
-      <c r="CX27" s="66"/>
-      <c r="CY27" s="66"/>
-      <c r="CZ27" s="66"/>
-      <c r="DA27" s="66"/>
-      <c r="DB27" s="66"/>
-      <c r="DC27" s="66"/>
-      <c r="DD27" s="66"/>
-      <c r="DE27" s="66"/>
-      <c r="DF27" s="66"/>
-      <c r="DG27" s="66"/>
-      <c r="DH27" s="66"/>
-      <c r="DI27" s="66"/>
-      <c r="DJ27" s="66"/>
-      <c r="DK27" s="66"/>
-      <c r="DL27" s="66"/>
-      <c r="DM27" s="66"/>
-      <c r="DN27" s="66"/>
-      <c r="DO27" s="66"/>
-      <c r="DP27" s="66"/>
-      <c r="DQ27" s="66"/>
-      <c r="DR27" s="66"/>
-      <c r="DS27" s="66"/>
-      <c r="DT27" s="66"/>
-      <c r="DU27" s="66"/>
-      <c r="DV27" s="66"/>
-      <c r="DW27" s="66"/>
-      <c r="DX27" s="66"/>
-      <c r="DY27" s="66"/>
-      <c r="DZ27" s="66"/>
-      <c r="EA27" s="66"/>
-      <c r="EB27" s="66"/>
-      <c r="EC27" s="66"/>
-      <c r="ED27" s="66"/>
-      <c r="EE27" s="66"/>
-      <c r="EF27" s="66"/>
-      <c r="EG27" s="66"/>
-      <c r="EH27" s="66"/>
-      <c r="EI27" s="66"/>
-      <c r="EJ27" s="66"/>
-      <c r="EK27" s="66"/>
-      <c r="EL27" s="66"/>
-      <c r="EM27" s="66"/>
-      <c r="EN27" s="66"/>
-      <c r="EO27" s="66"/>
-      <c r="EP27" s="66"/>
-      <c r="EQ27" s="66"/>
-      <c r="ER27" s="66"/>
-      <c r="ES27" s="66"/>
-      <c r="ET27" s="66"/>
-      <c r="EU27" s="66"/>
-      <c r="EV27" s="66"/>
-      <c r="EW27" s="66"/>
-      <c r="EX27" s="66"/>
-      <c r="EY27" s="66"/>
-      <c r="EZ27" s="66"/>
-      <c r="FA27" s="66"/>
-      <c r="FB27" s="66"/>
-      <c r="FC27" s="66"/>
-      <c r="FD27" s="66"/>
-      <c r="FE27" s="66"/>
-      <c r="FF27" s="66"/>
-      <c r="FG27" s="66"/>
-      <c r="FH27" s="66"/>
-      <c r="FI27" s="66"/>
-      <c r="FJ27" s="66"/>
-      <c r="FK27" s="66"/>
-      <c r="FL27" s="66"/>
-      <c r="FM27" s="66"/>
-      <c r="FN27" s="66"/>
-      <c r="FO27" s="66"/>
-      <c r="FP27" s="66"/>
-      <c r="FQ27" s="66"/>
-      <c r="FR27" s="66"/>
-      <c r="FS27" s="66"/>
-      <c r="FT27" s="66"/>
-      <c r="FU27" s="66"/>
-      <c r="FV27" s="66"/>
-      <c r="FW27" s="66"/>
-      <c r="FX27" s="66"/>
-      <c r="FY27" s="66"/>
-      <c r="FZ27" s="66"/>
-      <c r="GA27" s="66"/>
-      <c r="GB27" s="66"/>
-      <c r="GC27" s="66"/>
-      <c r="GD27" s="66"/>
-      <c r="GE27" s="66"/>
-      <c r="GF27" s="66"/>
-      <c r="GG27" s="66"/>
-      <c r="GH27" s="66"/>
-      <c r="GI27" s="66"/>
-      <c r="GJ27" s="66"/>
-      <c r="GK27" s="66"/>
-      <c r="GL27" s="66"/>
-      <c r="GM27" s="66"/>
-      <c r="GN27" s="66"/>
-      <c r="GO27" s="66"/>
-      <c r="GP27" s="66"/>
-      <c r="GQ27" s="66"/>
-      <c r="GR27" s="66"/>
-      <c r="GS27" s="66"/>
-      <c r="GT27" s="66"/>
-      <c r="GU27" s="66"/>
-      <c r="GV27" s="66"/>
-      <c r="GW27" s="66"/>
-      <c r="GX27" s="66"/>
-      <c r="GY27" s="66"/>
-      <c r="GZ27" s="66"/>
-      <c r="HA27" s="66"/>
-      <c r="HB27" s="66"/>
-      <c r="HC27" s="66"/>
-      <c r="HD27" s="66"/>
-      <c r="HE27" s="66"/>
-      <c r="HF27" s="66"/>
-      <c r="HG27" s="66"/>
-      <c r="HH27" s="66"/>
-      <c r="HI27" s="66"/>
-      <c r="HJ27" s="66"/>
-      <c r="HK27" s="66"/>
-      <c r="HL27" s="66"/>
-      <c r="HM27" s="66"/>
-      <c r="HN27" s="66"/>
-      <c r="HO27" s="66"/>
-      <c r="HP27" s="66"/>
-      <c r="HQ27" s="66"/>
-      <c r="HR27" s="66"/>
-      <c r="HS27" s="66"/>
-      <c r="HT27" s="66"/>
-      <c r="HU27" s="66"/>
-      <c r="HV27" s="66"/>
-      <c r="HW27" s="66"/>
-      <c r="HX27" s="66"/>
-      <c r="HY27" s="66"/>
-      <c r="HZ27" s="66"/>
-      <c r="IA27" s="66"/>
-      <c r="IB27" s="66"/>
-      <c r="IC27" s="66"/>
-      <c r="ID27" s="66"/>
-      <c r="IE27" s="66"/>
-      <c r="IF27" s="66"/>
-      <c r="IG27" s="66"/>
-      <c r="IH27" s="66"/>
-      <c r="II27" s="66"/>
-      <c r="IJ27" s="66"/>
-      <c r="IK27" s="66"/>
-      <c r="IL27" s="66"/>
-      <c r="IM27" s="66"/>
-      <c r="IN27" s="66"/>
-      <c r="IO27" s="66"/>
-      <c r="IP27" s="66"/>
-      <c r="IQ27" s="66"/>
-      <c r="IR27" s="66"/>
-      <c r="IS27" s="66"/>
-      <c r="IT27" s="66"/>
-      <c r="IU27" s="66"/>
-      <c r="IV27" s="66"/>
     </row>
     <row r="28" spans="1:256" ht="15" customHeight="1">
-      <c r="A28" s="8"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17"/>
+      <c r="A28" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28"/>
+      <c r="Z28"/>
+      <c r="AA28"/>
+      <c r="AB28"/>
+      <c r="AC28"/>
+      <c r="AD28"/>
+      <c r="AE28"/>
+      <c r="AF28"/>
+      <c r="AG28"/>
+      <c r="AH28"/>
+      <c r="AI28"/>
+      <c r="AJ28"/>
+      <c r="AK28"/>
+      <c r="AL28"/>
+      <c r="AM28"/>
+      <c r="AN28"/>
+      <c r="AO28"/>
+      <c r="AP28"/>
+      <c r="AQ28"/>
+      <c r="AR28"/>
+      <c r="AS28"/>
+      <c r="AT28"/>
+      <c r="AU28"/>
+      <c r="AV28"/>
+      <c r="AW28"/>
+      <c r="AX28"/>
+      <c r="AY28"/>
+      <c r="AZ28"/>
+      <c r="BA28"/>
+      <c r="BB28"/>
+      <c r="BC28"/>
+      <c r="BD28"/>
+      <c r="BE28"/>
+      <c r="BF28"/>
+      <c r="BG28"/>
+      <c r="BH28"/>
+      <c r="BI28"/>
+      <c r="BJ28"/>
+      <c r="BK28"/>
+      <c r="BL28"/>
+      <c r="BM28"/>
+      <c r="BN28"/>
+      <c r="BO28"/>
+      <c r="BP28"/>
+      <c r="BQ28"/>
+      <c r="BR28"/>
+      <c r="BS28"/>
+      <c r="BT28"/>
+      <c r="BU28"/>
+      <c r="BV28"/>
+      <c r="BW28"/>
+      <c r="BX28"/>
+      <c r="BY28"/>
+      <c r="BZ28"/>
+      <c r="CA28"/>
+      <c r="CB28"/>
+      <c r="CC28"/>
+      <c r="CD28"/>
+      <c r="CE28"/>
+      <c r="CF28"/>
+      <c r="CG28"/>
+      <c r="CH28"/>
+      <c r="CI28"/>
+      <c r="CJ28"/>
+      <c r="CK28"/>
+      <c r="CL28"/>
+      <c r="CM28"/>
+      <c r="CN28"/>
+      <c r="CO28"/>
+      <c r="CP28"/>
+      <c r="CQ28"/>
+      <c r="CR28"/>
+      <c r="CS28"/>
+      <c r="CT28"/>
+      <c r="CU28"/>
+      <c r="CV28"/>
+      <c r="CW28"/>
+      <c r="CX28"/>
+      <c r="CY28"/>
+      <c r="CZ28"/>
+      <c r="DA28"/>
+      <c r="DB28"/>
+      <c r="DC28"/>
+      <c r="DD28"/>
+      <c r="DE28"/>
+      <c r="DF28"/>
+      <c r="DG28"/>
+      <c r="DH28"/>
+      <c r="DI28"/>
+      <c r="DJ28"/>
+      <c r="DK28"/>
+      <c r="DL28"/>
+      <c r="DM28"/>
+      <c r="DN28"/>
+      <c r="DO28"/>
+      <c r="DP28"/>
+      <c r="DQ28"/>
+      <c r="DR28"/>
+      <c r="DS28"/>
+      <c r="DT28"/>
+      <c r="DU28"/>
+      <c r="DV28"/>
+      <c r="DW28"/>
+      <c r="DX28"/>
+      <c r="DY28"/>
+      <c r="DZ28"/>
+      <c r="EA28"/>
+      <c r="EB28"/>
+      <c r="EC28"/>
+      <c r="ED28"/>
+      <c r="EE28"/>
+      <c r="EF28"/>
+      <c r="EG28"/>
+      <c r="EH28"/>
+      <c r="EI28"/>
+      <c r="EJ28"/>
+      <c r="EK28"/>
+      <c r="EL28"/>
+      <c r="EM28"/>
+      <c r="EN28"/>
+      <c r="EO28"/>
+      <c r="EP28"/>
+      <c r="EQ28"/>
+      <c r="ER28"/>
+      <c r="ES28"/>
+      <c r="ET28"/>
+      <c r="EU28"/>
+      <c r="EV28"/>
+      <c r="EW28"/>
+      <c r="EX28"/>
+      <c r="EY28"/>
+      <c r="EZ28"/>
+      <c r="FA28"/>
+      <c r="FB28"/>
+      <c r="FC28"/>
+      <c r="FD28"/>
+      <c r="FE28"/>
+      <c r="FF28"/>
+      <c r="FG28"/>
+      <c r="FH28"/>
+      <c r="FI28"/>
+      <c r="FJ28"/>
+      <c r="FK28"/>
+      <c r="FL28"/>
+      <c r="FM28"/>
+      <c r="FN28"/>
+      <c r="FO28"/>
+      <c r="FP28"/>
+      <c r="FQ28"/>
+      <c r="FR28"/>
+      <c r="FS28"/>
+      <c r="FT28"/>
+      <c r="FU28"/>
+      <c r="FV28"/>
+      <c r="FW28"/>
+      <c r="FX28"/>
+      <c r="FY28"/>
+      <c r="FZ28"/>
+      <c r="GA28"/>
+      <c r="GB28"/>
+      <c r="GC28"/>
+      <c r="GD28"/>
+      <c r="GE28"/>
+      <c r="GF28"/>
+      <c r="GG28"/>
+      <c r="GH28"/>
+      <c r="GI28"/>
+      <c r="GJ28"/>
+      <c r="GK28"/>
+      <c r="GL28"/>
+      <c r="GM28"/>
+      <c r="GN28"/>
+      <c r="GO28"/>
+      <c r="GP28"/>
+      <c r="GQ28"/>
+      <c r="GR28"/>
+      <c r="GS28"/>
+      <c r="GT28"/>
+      <c r="GU28"/>
+      <c r="GV28"/>
+      <c r="GW28"/>
+      <c r="GX28"/>
+      <c r="GY28"/>
+      <c r="GZ28"/>
+      <c r="HA28"/>
+      <c r="HB28"/>
+      <c r="HC28"/>
+      <c r="HD28"/>
+      <c r="HE28"/>
+      <c r="HF28"/>
+      <c r="HG28"/>
+      <c r="HH28"/>
+      <c r="HI28"/>
+      <c r="HJ28"/>
+      <c r="HK28"/>
+      <c r="HL28"/>
+      <c r="HM28"/>
+      <c r="HN28"/>
+      <c r="HO28"/>
+      <c r="HP28"/>
+      <c r="HQ28"/>
+      <c r="HR28"/>
+      <c r="HS28"/>
+      <c r="HT28"/>
+      <c r="HU28"/>
+      <c r="HV28"/>
+      <c r="HW28"/>
+      <c r="HX28"/>
+      <c r="HY28"/>
+      <c r="HZ28"/>
+      <c r="IA28"/>
+      <c r="IB28"/>
+      <c r="IC28"/>
+      <c r="ID28"/>
+      <c r="IE28"/>
+      <c r="IF28"/>
+      <c r="IG28"/>
+      <c r="IH28"/>
+      <c r="II28"/>
+      <c r="IJ28"/>
+      <c r="IK28"/>
+      <c r="IL28"/>
+      <c r="IM28"/>
+      <c r="IN28"/>
+      <c r="IO28"/>
+      <c r="IP28"/>
+      <c r="IQ28"/>
+      <c r="IR28"/>
+      <c r="IS28"/>
+      <c r="IT28"/>
+      <c r="IU28"/>
+      <c r="IV28"/>
     </row>
     <row r="29" spans="1:256" ht="15" customHeight="1">
-      <c r="A29" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
@@ -8548,9 +8004,9 @@
       <c r="IV29"/>
     </row>
     <row r="30" spans="1:256" ht="15" customHeight="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="13"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
@@ -8806,9 +8262,11 @@
       <c r="IV30"/>
     </row>
     <row r="31" spans="1:256" ht="15" customHeight="1">
-      <c r="A31" s="21"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
+      <c r="A31" s="91" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="92"/>
+      <c r="C31" s="93"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
@@ -9064,11 +8522,11 @@
       <c r="IV31"/>
     </row>
     <row r="32" spans="1:256" ht="15" customHeight="1">
-      <c r="A32" s="91" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="92"/>
-      <c r="C32" s="93"/>
+      <c r="A32" s="84" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="85"/>
+      <c r="C32" s="86"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
@@ -9323,272 +8781,12 @@
       <c r="IU32"/>
       <c r="IV32"/>
     </row>
-    <row r="33" spans="1:256" ht="15" customHeight="1">
-      <c r="A33" s="84" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="85"/>
-      <c r="C33" s="86"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
-      <c r="J33"/>
-      <c r="K33"/>
-      <c r="L33"/>
-      <c r="M33"/>
-      <c r="N33"/>
-      <c r="O33"/>
-      <c r="P33"/>
-      <c r="Q33"/>
-      <c r="R33"/>
-      <c r="S33"/>
-      <c r="T33"/>
-      <c r="U33"/>
-      <c r="V33"/>
-      <c r="W33"/>
-      <c r="X33"/>
-      <c r="Y33"/>
-      <c r="Z33"/>
-      <c r="AA33"/>
-      <c r="AB33"/>
-      <c r="AC33"/>
-      <c r="AD33"/>
-      <c r="AE33"/>
-      <c r="AF33"/>
-      <c r="AG33"/>
-      <c r="AH33"/>
-      <c r="AI33"/>
-      <c r="AJ33"/>
-      <c r="AK33"/>
-      <c r="AL33"/>
-      <c r="AM33"/>
-      <c r="AN33"/>
-      <c r="AO33"/>
-      <c r="AP33"/>
-      <c r="AQ33"/>
-      <c r="AR33"/>
-      <c r="AS33"/>
-      <c r="AT33"/>
-      <c r="AU33"/>
-      <c r="AV33"/>
-      <c r="AW33"/>
-      <c r="AX33"/>
-      <c r="AY33"/>
-      <c r="AZ33"/>
-      <c r="BA33"/>
-      <c r="BB33"/>
-      <c r="BC33"/>
-      <c r="BD33"/>
-      <c r="BE33"/>
-      <c r="BF33"/>
-      <c r="BG33"/>
-      <c r="BH33"/>
-      <c r="BI33"/>
-      <c r="BJ33"/>
-      <c r="BK33"/>
-      <c r="BL33"/>
-      <c r="BM33"/>
-      <c r="BN33"/>
-      <c r="BO33"/>
-      <c r="BP33"/>
-      <c r="BQ33"/>
-      <c r="BR33"/>
-      <c r="BS33"/>
-      <c r="BT33"/>
-      <c r="BU33"/>
-      <c r="BV33"/>
-      <c r="BW33"/>
-      <c r="BX33"/>
-      <c r="BY33"/>
-      <c r="BZ33"/>
-      <c r="CA33"/>
-      <c r="CB33"/>
-      <c r="CC33"/>
-      <c r="CD33"/>
-      <c r="CE33"/>
-      <c r="CF33"/>
-      <c r="CG33"/>
-      <c r="CH33"/>
-      <c r="CI33"/>
-      <c r="CJ33"/>
-      <c r="CK33"/>
-      <c r="CL33"/>
-      <c r="CM33"/>
-      <c r="CN33"/>
-      <c r="CO33"/>
-      <c r="CP33"/>
-      <c r="CQ33"/>
-      <c r="CR33"/>
-      <c r="CS33"/>
-      <c r="CT33"/>
-      <c r="CU33"/>
-      <c r="CV33"/>
-      <c r="CW33"/>
-      <c r="CX33"/>
-      <c r="CY33"/>
-      <c r="CZ33"/>
-      <c r="DA33"/>
-      <c r="DB33"/>
-      <c r="DC33"/>
-      <c r="DD33"/>
-      <c r="DE33"/>
-      <c r="DF33"/>
-      <c r="DG33"/>
-      <c r="DH33"/>
-      <c r="DI33"/>
-      <c r="DJ33"/>
-      <c r="DK33"/>
-      <c r="DL33"/>
-      <c r="DM33"/>
-      <c r="DN33"/>
-      <c r="DO33"/>
-      <c r="DP33"/>
-      <c r="DQ33"/>
-      <c r="DR33"/>
-      <c r="DS33"/>
-      <c r="DT33"/>
-      <c r="DU33"/>
-      <c r="DV33"/>
-      <c r="DW33"/>
-      <c r="DX33"/>
-      <c r="DY33"/>
-      <c r="DZ33"/>
-      <c r="EA33"/>
-      <c r="EB33"/>
-      <c r="EC33"/>
-      <c r="ED33"/>
-      <c r="EE33"/>
-      <c r="EF33"/>
-      <c r="EG33"/>
-      <c r="EH33"/>
-      <c r="EI33"/>
-      <c r="EJ33"/>
-      <c r="EK33"/>
-      <c r="EL33"/>
-      <c r="EM33"/>
-      <c r="EN33"/>
-      <c r="EO33"/>
-      <c r="EP33"/>
-      <c r="EQ33"/>
-      <c r="ER33"/>
-      <c r="ES33"/>
-      <c r="ET33"/>
-      <c r="EU33"/>
-      <c r="EV33"/>
-      <c r="EW33"/>
-      <c r="EX33"/>
-      <c r="EY33"/>
-      <c r="EZ33"/>
-      <c r="FA33"/>
-      <c r="FB33"/>
-      <c r="FC33"/>
-      <c r="FD33"/>
-      <c r="FE33"/>
-      <c r="FF33"/>
-      <c r="FG33"/>
-      <c r="FH33"/>
-      <c r="FI33"/>
-      <c r="FJ33"/>
-      <c r="FK33"/>
-      <c r="FL33"/>
-      <c r="FM33"/>
-      <c r="FN33"/>
-      <c r="FO33"/>
-      <c r="FP33"/>
-      <c r="FQ33"/>
-      <c r="FR33"/>
-      <c r="FS33"/>
-      <c r="FT33"/>
-      <c r="FU33"/>
-      <c r="FV33"/>
-      <c r="FW33"/>
-      <c r="FX33"/>
-      <c r="FY33"/>
-      <c r="FZ33"/>
-      <c r="GA33"/>
-      <c r="GB33"/>
-      <c r="GC33"/>
-      <c r="GD33"/>
-      <c r="GE33"/>
-      <c r="GF33"/>
-      <c r="GG33"/>
-      <c r="GH33"/>
-      <c r="GI33"/>
-      <c r="GJ33"/>
-      <c r="GK33"/>
-      <c r="GL33"/>
-      <c r="GM33"/>
-      <c r="GN33"/>
-      <c r="GO33"/>
-      <c r="GP33"/>
-      <c r="GQ33"/>
-      <c r="GR33"/>
-      <c r="GS33"/>
-      <c r="GT33"/>
-      <c r="GU33"/>
-      <c r="GV33"/>
-      <c r="GW33"/>
-      <c r="GX33"/>
-      <c r="GY33"/>
-      <c r="GZ33"/>
-      <c r="HA33"/>
-      <c r="HB33"/>
-      <c r="HC33"/>
-      <c r="HD33"/>
-      <c r="HE33"/>
-      <c r="HF33"/>
-      <c r="HG33"/>
-      <c r="HH33"/>
-      <c r="HI33"/>
-      <c r="HJ33"/>
-      <c r="HK33"/>
-      <c r="HL33"/>
-      <c r="HM33"/>
-      <c r="HN33"/>
-      <c r="HO33"/>
-      <c r="HP33"/>
-      <c r="HQ33"/>
-      <c r="HR33"/>
-      <c r="HS33"/>
-      <c r="HT33"/>
-      <c r="HU33"/>
-      <c r="HV33"/>
-      <c r="HW33"/>
-      <c r="HX33"/>
-      <c r="HY33"/>
-      <c r="HZ33"/>
-      <c r="IA33"/>
-      <c r="IB33"/>
-      <c r="IC33"/>
-      <c r="ID33"/>
-      <c r="IE33"/>
-      <c r="IF33"/>
-      <c r="IG33"/>
-      <c r="IH33"/>
-      <c r="II33"/>
-      <c r="IJ33"/>
-      <c r="IK33"/>
-      <c r="IL33"/>
-      <c r="IM33"/>
-      <c r="IN33"/>
-      <c r="IO33"/>
-      <c r="IP33"/>
-      <c r="IQ33"/>
-      <c r="IR33"/>
-      <c r="IS33"/>
-      <c r="IT33"/>
-      <c r="IU33"/>
-      <c r="IV33"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A31:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9602,7 +8800,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -9613,11 +8813,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
     </row>
     <row r="2" spans="1:256" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -9639,7 +8839,7 @@
       </c>
       <c r="C3" s="7"/>
     </row>
-    <row r="4" spans="1:256" ht="15" hidden="1" customHeight="1">
+    <row r="4" spans="1:256" ht="15" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>40</v>
       </c>
@@ -9947,8 +9147,8 @@
       <c r="IV9" s="66"/>
     </row>
     <row r="10" spans="1:256" ht="15" customHeight="1">
-      <c r="A10" s="79" t="s">
-        <v>105</v>
+      <c r="A10" s="81" t="s">
+        <v>100</v>
       </c>
       <c r="B10" s="72" t="s">
         <v>39</v>
@@ -9956,6 +9156,9 @@
       <c r="C10" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
Actualización de actividades 2
</commit_message>
<xml_diff>
--- a/Scrum.xlsx
+++ b/Scrum.xlsx
@@ -370,6 +370,7 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -837,6 +838,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -861,14 +870,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2094,11 +2095,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
     </row>
     <row r="2" spans="1:256" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -2112,10 +2113,10 @@
       </c>
     </row>
     <row r="3" spans="1:256" ht="15" customHeight="1">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="84" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="85" t="s">
         <v>107</v>
       </c>
       <c r="C3" s="4"/>
@@ -2377,7 +2378,7 @@
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="85" t="s">
         <v>107</v>
       </c>
       <c r="C4" s="7"/>
@@ -2397,7 +2398,7 @@
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="85" t="s">
         <v>107</v>
       </c>
       <c r="C6" s="7"/>
@@ -2414,11 +2415,11 @@
       </c>
     </row>
     <row r="8" spans="1:256" ht="15" customHeight="1">
-      <c r="A8" s="87" t="s">
+      <c r="A8" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="88"/>
-      <c r="C8" s="88"/>
+      <c r="B8" s="92"/>
+      <c r="C8" s="92"/>
     </row>
     <row r="9" spans="1:256" ht="15" customHeight="1">
       <c r="A9" s="11" t="s">
@@ -2477,18 +2478,18 @@
       <c r="C18" s="15"/>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1">
-      <c r="A19" s="91" t="s">
+      <c r="A19" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="92"/>
-      <c r="C19" s="93"/>
+      <c r="B19" s="96"/>
+      <c r="C19" s="97"/>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1">
-      <c r="A20" s="84" t="s">
+      <c r="A20" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="85"/>
-      <c r="C20" s="86"/>
+      <c r="B20" s="89"/>
+      <c r="C20" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2522,11 +2523,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
     </row>
     <row r="2" spans="1:256" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -3118,7 +3119,7 @@
       <c r="B9" s="6">
         <v>42778</v>
       </c>
-      <c r="C9" s="99" t="s">
+      <c r="C9" s="87" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3129,7 +3130,7 @@
       <c r="B10" s="6">
         <v>42778</v>
       </c>
-      <c r="C10" s="99" t="s">
+      <c r="C10" s="87" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3396,7 +3397,7 @@
       <c r="IV11" s="66"/>
     </row>
     <row r="12" spans="1:256" ht="15" customHeight="1">
-      <c r="A12" s="98" t="s">
+      <c r="A12" s="86" t="s">
         <v>108</v>
       </c>
       <c r="B12" s="6">
@@ -3405,11 +3406,11 @@
       <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:256" ht="15" customHeight="1">
-      <c r="A13" s="87" t="s">
+      <c r="A13" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
+      <c r="B13" s="92"/>
+      <c r="C13" s="92"/>
     </row>
     <row r="14" spans="1:256" ht="15" customHeight="1">
       <c r="A14" s="11" t="s">
@@ -3465,18 +3466,18 @@
       <c r="C22" s="15"/>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1">
-      <c r="A23" s="91" t="s">
+      <c r="A23" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="92"/>
-      <c r="C23" s="93"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="97"/>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1">
-      <c r="A24" s="84" t="s">
+      <c r="A24" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="85"/>
-      <c r="C24" s="86"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3498,7 +3499,7 @@
   <dimension ref="A1:IV33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -3510,11 +3511,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
     </row>
     <row r="2" spans="1:256" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -4104,7 +4105,7 @@
         <v>103</v>
       </c>
       <c r="B9" s="6">
-        <v>42778</v>
+        <v>42785</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="66"/>
@@ -4366,7 +4367,7 @@
         <v>90</v>
       </c>
       <c r="B10" s="6">
-        <v>42778</v>
+        <v>42785</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="66"/>
@@ -4628,7 +4629,7 @@
         <v>29</v>
       </c>
       <c r="B11" s="6">
-        <v>42778</v>
+        <v>42785</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="66"/>
@@ -5149,11 +5150,11 @@
       <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:256" ht="15" customHeight="1">
-      <c r="A14" s="87" t="s">
+      <c r="A14" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="88"/>
-      <c r="C14" s="88"/>
+      <c r="B14" s="92"/>
+      <c r="C14" s="92"/>
     </row>
     <row r="15" spans="1:256" ht="15" customHeight="1">
       <c r="A15" s="75" t="s">
@@ -9064,11 +9065,11 @@
       <c r="IV31"/>
     </row>
     <row r="32" spans="1:256" ht="15" customHeight="1">
-      <c r="A32" s="91" t="s">
+      <c r="A32" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="92"/>
-      <c r="C32" s="93"/>
+      <c r="B32" s="96"/>
+      <c r="C32" s="97"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
@@ -9324,11 +9325,11 @@
       <c r="IV32"/>
     </row>
     <row r="33" spans="1:256" ht="15" customHeight="1">
-      <c r="A33" s="84" t="s">
+      <c r="A33" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="85"/>
-      <c r="C33" s="86"/>
+      <c r="B33" s="89"/>
+      <c r="C33" s="90"/>
       <c r="D33"/>
       <c r="E33"/>
       <c r="F33"/>
@@ -10244,15 +10245,15 @@
       <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="94" t="s">
+      <c r="A18" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="95"/>
-      <c r="C18" s="95"/>
-      <c r="D18" s="95"/>
-      <c r="E18" s="95"/>
-      <c r="F18" s="95"/>
-      <c r="G18" s="95"/>
+      <c r="B18" s="99"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="99"/>
+      <c r="E18" s="99"/>
+      <c r="F18" s="99"/>
+      <c r="G18" s="99"/>
       <c r="H18" s="54"/>
     </row>
   </sheetData>

</xml_diff>